<commit_message>
galacticPubs::publish() [2022-06-27 11:08:58]  fix steam epaulette
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -437,7 +437,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="132">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1171,7 +1171,7 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="233">
+  <cellXfs count="515">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1541,6 +1541,852 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
@@ -4980,42 +5826,42 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="139" t="s">
+      <c r="A3" s="421" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="423" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="143" t="s">
+      <c r="C3" s="425" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="145" t="s">
+      <c r="D3" s="427" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="147" t="s">
+      <c r="E3" s="429" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="149" t="s">
+      <c r="F3" s="431" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A4" s="140" t="s">
+      <c r="A4" s="422" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="142" t="s">
+      <c r="B4" s="424" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="144" t="s">
+      <c r="C4" s="426" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="146" t="s">
+      <c r="D4" s="428" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="148" t="s">
+      <c r="E4" s="430" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="150" t="s">
+      <c r="F4" s="432" t="s">
         <v>64</v>
       </c>
     </row>
@@ -6169,25 +7015,25 @@
     <row r="3" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="433" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="154" t="s">
+      <c r="D3" s="436" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="157" t="s">
+      <c r="E3" s="439" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="160" t="s">
+      <c r="F3" s="442" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="163" t="s">
+      <c r="G3" s="445" t="s">
         <v>64</v>
       </c>
-      <c r="H3" s="166" t="s">
+      <c r="H3" s="448" t="s">
         <v>71</v>
       </c>
-      <c r="I3" s="169" t="s">
+      <c r="I3" s="451" t="s">
         <v>74</v>
       </c>
       <c r="J3"/>
@@ -6195,25 +7041,25 @@
     <row r="4" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="152" t="s">
+      <c r="C4" s="434" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="155" t="s">
+      <c r="D4" s="437" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="158" t="s">
+      <c r="E4" s="440" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="161" t="s">
+      <c r="F4" s="443" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="164" t="s">
+      <c r="G4" s="446" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="167" t="s">
+      <c r="H4" s="449" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="170" t="s">
+      <c r="I4" s="452" t="s">
         <v>76</v>
       </c>
       <c r="J4"/>
@@ -6221,25 +7067,25 @@
     <row r="5" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="153" t="s">
+      <c r="C5" s="435" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="156" t="s">
+      <c r="D5" s="438" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="159" t="s">
+      <c r="E5" s="441" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="162" t="s">
+      <c r="F5" s="444" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="165" t="s">
+      <c r="G5" s="447" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="168" t="s">
+      <c r="H5" s="450" t="s">
         <v>72</v>
       </c>
-      <c r="I5" s="171" t="s">
+      <c r="I5" s="453" t="s">
         <v>75</v>
       </c>
       <c r="J5"/>
@@ -7780,31 +8626,31 @@
     <row r="3" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="172" t="s">
+      <c r="C3" s="454" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="179" t="s">
+      <c r="D3" s="461" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="186" t="s">
+      <c r="E3" s="468" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="191" t="s">
+      <c r="F3" s="473" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="198" t="s">
+      <c r="G3" s="480" t="s">
         <v>82</v>
       </c>
-      <c r="H3" s="205" t="s">
+      <c r="H3" s="487" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="212" t="s">
+      <c r="I3" s="494" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="219" t="s">
+      <c r="J3" s="501" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="226" t="s">
+      <c r="K3" s="508" t="s">
         <v>103</v>
       </c>
       <c r="U3" s="6"/>
@@ -7818,31 +8664,31 @@
     <row r="4" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="173" t="s">
+      <c r="C4" s="455" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="180" t="s">
+      <c r="D4" s="462" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="187" t="s">
+      <c r="E4" s="469" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="192" t="s">
+      <c r="F4" s="474" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="199" t="s">
+      <c r="G4" s="481" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="206" t="s">
+      <c r="H4" s="488" t="s">
         <v>90</v>
       </c>
-      <c r="I4" s="213" t="s">
+      <c r="I4" s="495" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="220" t="s">
+      <c r="J4" s="502" t="s">
         <v>97</v>
       </c>
-      <c r="K4" s="227" t="s">
+      <c r="K4" s="509" t="s">
         <v>104</v>
       </c>
       <c r="U4" s="6"/>
@@ -7856,29 +8702,29 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="174" t="s">
+      <c r="C5" s="456" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="181" t="s">
+      <c r="D5" s="463" t="s">
         <v>77</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="193" t="s">
+      <c r="F5" s="475" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="200" t="s">
+      <c r="G5" s="482" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="207" t="s">
+      <c r="H5" s="489" t="s">
         <v>91</v>
       </c>
-      <c r="I5" s="214" t="s">
+      <c r="I5" s="496" t="s">
         <v>64</v>
       </c>
-      <c r="J5" s="221" t="s">
+      <c r="J5" s="503" t="s">
         <v>98</v>
       </c>
-      <c r="K5" s="228" t="s">
+      <c r="K5" s="510" t="s">
         <v>105</v>
       </c>
       <c r="U5" s="6"/>
@@ -7892,31 +8738,31 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="175" t="s">
+      <c r="C6" s="457" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="182" t="s">
+      <c r="D6" s="464" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="188" t="s">
+      <c r="E6" s="470" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="194" t="s">
+      <c r="F6" s="476" t="s">
         <v>110</v>
       </c>
-      <c r="G6" s="201" t="s">
+      <c r="G6" s="483" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="208" t="s">
+      <c r="H6" s="490" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="215" t="s">
+      <c r="I6" s="497" t="s">
         <v>64</v>
       </c>
-      <c r="J6" s="222" t="s">
+      <c r="J6" s="504" t="s">
         <v>99</v>
       </c>
-      <c r="K6" s="229" t="s">
+      <c r="K6" s="511" t="s">
         <v>106</v>
       </c>
       <c r="U6" s="6"/>
@@ -7930,31 +8776,31 @@
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="176" t="s">
+      <c r="C7" s="458" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="183" t="s">
+      <c r="D7" s="465" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="189" t="s">
+      <c r="E7" s="471" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="195" t="s">
+      <c r="F7" s="477" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="202" t="s">
+      <c r="G7" s="484" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="209" t="s">
+      <c r="H7" s="491" t="s">
         <v>93</v>
       </c>
-      <c r="I7" s="216" t="s">
+      <c r="I7" s="498" t="s">
         <v>64</v>
       </c>
-      <c r="J7" s="223" t="s">
+      <c r="J7" s="505" t="s">
         <v>100</v>
       </c>
-      <c r="K7" s="230" t="s">
+      <c r="K7" s="512" t="s">
         <v>107</v>
       </c>
       <c r="U7" s="6"/>
@@ -7968,29 +8814,29 @@
     <row r="8" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8"/>
-      <c r="C8" s="177" t="s">
+      <c r="C8" s="459" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="184" t="s">
+      <c r="D8" s="466" t="s">
         <v>78</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="196" t="s">
+      <c r="F8" s="478" t="s">
         <v>112</v>
       </c>
-      <c r="G8" s="203" t="s">
+      <c r="G8" s="485" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="210" t="s">
+      <c r="H8" s="492" t="s">
         <v>94</v>
       </c>
-      <c r="I8" s="217" t="s">
+      <c r="I8" s="499" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="224" t="s">
+      <c r="J8" s="506" t="s">
         <v>101</v>
       </c>
-      <c r="K8" s="231" t="s">
+      <c r="K8" s="513" t="s">
         <v>108</v>
       </c>
       <c r="U8" s="6"/>
@@ -8004,31 +8850,31 @@
     <row r="9" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9"/>
-      <c r="C9" s="178" t="s">
+      <c r="C9" s="460" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="185" t="s">
+      <c r="D9" s="467" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="190" t="s">
+      <c r="E9" s="472" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="197" t="s">
+      <c r="F9" s="479" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="204" t="s">
+      <c r="G9" s="486" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="211" t="s">
+      <c r="H9" s="493" t="s">
         <v>95</v>
       </c>
-      <c r="I9" s="218" t="s">
+      <c r="I9" s="500" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="225" t="s">
+      <c r="J9" s="507" t="s">
         <v>102</v>
       </c>
-      <c r="K9" s="232" t="s">
+      <c r="K9" s="514" t="s">
         <v>109</v>
       </c>
       <c r="U9" s="6"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-06-29 15:32:49]  fix markdown relative link paths
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="150">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -967,7 +967,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1584">
+  <cellXfs count="1686">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1076,6 +1076,312 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -8770,44 +9076,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1482" t="s">
+      <c r="A3" s="1584" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1484" t="s">
+      <c r="B3" s="1586" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="1486" t="s">
+      <c r="C3" s="1588" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1488" t="s">
+      <c r="D3" s="1590" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="1490" t="s">
+      <c r="E3" s="1592" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" t="s" s="1492">
+      <c r="G3" t="s" s="1594">
         <v>133</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1483" t="s">
+      <c r="A4" s="1585" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1485" t="s">
+      <c r="B4" s="1587" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1487" t="s">
+      <c r="C4" s="1589" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1489" t="s">
+      <c r="D4" s="1591" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="1491" t="s">
+      <c r="E4" s="1593" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" t="s" s="1493">
+      <c r="G4" t="s" s="1595">
         <v>134</v>
       </c>
     </row>
@@ -9964,81 +10270,81 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="1494" t="s">
+      <c r="C3" s="1596" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="1497" t="s">
+      <c r="D3" s="1599" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1500" t="s">
-        <v>50</v>
+      <c r="E3" s="1602" t="s">
+        <v>55</v>
       </c>
-      <c r="F3" s="1503" t="s">
+      <c r="F3" s="1605" t="s">
         <v>46</v>
       </c>
       <c r="G3" s="13"/>
-      <c r="H3" s="1506" t="s">
+      <c r="H3" s="1608" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="1509" t="s">
+      <c r="I3" s="1611" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="1512">
+      <c r="K3" t="s" s="1614">
         <v>135</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="1495" t="s">
+      <c r="C4" s="1597" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="1498" t="s">
+      <c r="D4" s="1600" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="1501" t="s">
+      <c r="E4" s="1603" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="1504" t="s">
+      <c r="F4" s="1606" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="13"/>
-      <c r="H4" s="1507" t="s">
+      <c r="H4" s="1609" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="1510" t="s">
+      <c r="I4" s="1612" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="1513">
+      <c r="K4" t="s" s="1615">
         <v>136</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="1496" t="s">
+      <c r="C5" s="1598" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="1499" t="s">
+      <c r="D5" s="1601" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="1502" t="s">
-        <v>55</v>
+      <c r="E5" s="1604" t="s">
+        <v>50</v>
       </c>
-      <c r="F5" s="1505" t="s">
+      <c r="F5" s="1607" t="s">
         <v>56</v>
       </c>
       <c r="G5" s="13"/>
-      <c r="H5" s="1508" t="s">
+      <c r="H5" s="1610" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="1511" t="s">
+      <c r="I5" s="1613" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
-      <c r="K5" t="s" s="1514">
+      <c r="K5" t="s" s="1616">
         <v>137</v>
       </c>
     </row>
@@ -11583,32 +11889,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="1515" t="s">
+      <c r="C3" s="1617" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="1523" t="s">
+      <c r="D3" s="1625" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="1531" t="s">
+      <c r="E3" s="1633" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="1537" t="s">
-        <v>64</v>
+      <c r="F3" s="1639" t="s">
+        <v>11</v>
       </c>
-      <c r="G3" s="1544" t="s">
-        <v>65</v>
+      <c r="G3" s="1646" t="s">
+        <v>83</v>
       </c>
-      <c r="H3" s="1552" t="s">
+      <c r="H3" s="1654" t="s">
         <v>66</v>
       </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="1560" t="s">
+      <c r="J3" s="1662" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="1568" t="s">
+      <c r="K3" s="1670" t="s">
         <v>68</v>
       </c>
-      <c r="L3" t="s" s="1576">
+      <c r="L3" t="s" s="1678">
         <v>138</v>
       </c>
       <c r="U3" s="8"/>
@@ -11622,32 +11928,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="1516" t="s">
+      <c r="C4" s="1618" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="1524" t="s">
+      <c r="D4" s="1626" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="1532" t="s">
+      <c r="E4" s="1634" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="1538" t="s">
-        <v>11</v>
+      <c r="F4" s="1640" t="s">
+        <v>87</v>
       </c>
-      <c r="G4" s="1545" t="s">
-        <v>92</v>
+      <c r="G4" s="1647" t="s">
+        <v>88</v>
       </c>
-      <c r="H4" s="1553" t="s">
+      <c r="H4" s="1655" t="s">
         <v>71</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="1561" t="s">
+      <c r="J4" s="1663" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="1569" t="s">
+      <c r="K4" s="1671" t="s">
         <v>73</v>
       </c>
-      <c r="L4" t="s" s="1577">
+      <c r="L4" t="s" s="1679">
         <v>139</v>
       </c>
       <c r="U4" s="8"/>
@@ -11661,30 +11967,30 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="1517" t="s">
+      <c r="C5" s="1619" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="1525" t="s">
+      <c r="D5" s="1627" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="1539" t="s">
-        <v>64</v>
+      <c r="F5" s="1641" t="s">
+        <v>11</v>
       </c>
-      <c r="G5" s="1546" t="s">
-        <v>79</v>
+      <c r="G5" s="1648" t="s">
+        <v>92</v>
       </c>
-      <c r="H5" s="1554" t="s">
+      <c r="H5" s="1656" t="s">
         <v>76</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="1562" t="s">
+      <c r="J5" s="1664" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="1570" t="s">
+      <c r="K5" s="1672" t="s">
         <v>78</v>
       </c>
-      <c r="L5" t="s" s="1578">
+      <c r="L5" t="s" s="1680">
         <v>140</v>
       </c>
       <c r="U5" s="8"/>
@@ -11698,32 +12004,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="1518" t="s">
+      <c r="C6" s="1620" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="1526" t="s">
+      <c r="D6" s="1628" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="1533" t="s">
+      <c r="E6" s="1635" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="1540" t="s">
+      <c r="F6" s="1642" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="1547" t="s">
+      <c r="G6" s="1649" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="1555" t="s">
+      <c r="H6" s="1657" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="13"/>
-      <c r="J6" s="1563" t="s">
+      <c r="J6" s="1665" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="1571" t="s">
+      <c r="K6" s="1673" t="s">
         <v>82</v>
       </c>
-      <c r="L6" t="s" s="1579">
+      <c r="L6" t="s" s="1681">
         <v>141</v>
       </c>
       <c r="U6" s="8"/>
@@ -11737,32 +12043,30 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="1519" t="s">
+      <c r="C7" s="1621" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="1527" t="s">
+      <c r="D7" s="1629" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="1534" t="s">
+      <c r="E7" s="1636" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="1541" t="s">
-        <v>87</v>
+      <c r="F7" s="1541"/>
+      <c r="G7" s="1650" t="s">
+        <v>145</v>
       </c>
-      <c r="G7" s="1548" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="1556" t="s">
+      <c r="H7" s="1658" t="s">
         <v>84</v>
       </c>
       <c r="I7" s="13"/>
-      <c r="J7" s="1564" t="s">
+      <c r="J7" s="1666" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="1572" t="s">
+      <c r="K7" s="1674" t="s">
         <v>86</v>
       </c>
-      <c r="L7" t="s" s="1580">
+      <c r="L7" t="s" s="1682">
         <v>142</v>
       </c>
       <c r="U7" s="8"/>
@@ -11776,28 +12080,30 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="1520" t="s">
+      <c r="C8" s="1622" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="1528" t="s">
+      <c r="D8" s="1630" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="22"/>
-      <c r="F8" s="1439"/>
-      <c r="G8" s="1549" t="s">
-        <v>145</v>
+      <c r="F8" s="1643" t="s">
+        <v>64</v>
       </c>
-      <c r="H8" s="1557" t="s">
+      <c r="G8" s="1651" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="1659" t="s">
         <v>89</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="1565" t="s">
+      <c r="J8" s="1667" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="1573" t="s">
+      <c r="K8" s="1675" t="s">
         <v>91</v>
       </c>
-      <c r="L8" t="s" s="1581">
+      <c r="L8" t="s" s="1683">
         <v>143</v>
       </c>
       <c r="U8" s="8"/>
@@ -11811,32 +12117,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="1521" t="s">
+      <c r="C9" s="1623" t="s">
         <v>132</v>
       </c>
-      <c r="D9" s="1529" t="s">
+      <c r="D9" s="1631" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="1535" t="s">
+      <c r="E9" s="1637" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="1542" t="s">
-        <v>11</v>
+      <c r="F9" s="1644" t="s">
+        <v>74</v>
       </c>
-      <c r="G9" s="1550" t="s">
-        <v>83</v>
+      <c r="G9" s="1652" t="s">
+        <v>75</v>
       </c>
-      <c r="H9" s="1558" t="s">
+      <c r="H9" s="1660" t="s">
         <v>146</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="1566" t="s">
+      <c r="J9" s="1668" t="s">
         <v>147</v>
       </c>
-      <c r="K9" s="1574" t="s">
+      <c r="K9" s="1676" t="s">
         <v>148</v>
       </c>
-      <c r="L9" t="s" s="1582">
+      <c r="L9" t="s" s="1684">
         <v>149</v>
       </c>
       <c r="U9" s="8"/>
@@ -11850,32 +12156,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="1522" t="s">
+      <c r="C10" s="1624" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="1530" t="s">
+      <c r="D10" s="1632" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="1536" t="s">
+      <c r="E10" s="1638" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="1543" t="s">
-        <v>74</v>
+      <c r="F10" s="1645" t="s">
+        <v>64</v>
       </c>
-      <c r="G10" s="1551" t="s">
-        <v>75</v>
+      <c r="G10" s="1653" t="s">
+        <v>79</v>
       </c>
-      <c r="H10" s="1559" t="s">
+      <c r="H10" s="1661" t="s">
         <v>93</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="1567" t="s">
+      <c r="J10" s="1669" t="s">
         <v>94</v>
       </c>
-      <c r="K10" s="1575" t="s">
+      <c r="K10" s="1677" t="s">
         <v>95</v>
       </c>
-      <c r="L10" t="s" s="1583">
+      <c r="L10" t="s" s="1685">
         <v>144</v>
       </c>
       <c r="U10" s="8"/>

</xml_diff>

<commit_message>
galacticPubs::publish() [2022-07-15 23:24:01]  All projects rebuilt with DefaultLocale
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3369" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4083" uniqueCount="150">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -967,7 +967,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3114">
+  <cellXfs count="3828">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1076,6 +1076,2148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -13360,44 +15502,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="3012" t="s">
+      <c r="A3" s="3726" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3014" t="s">
+      <c r="B3" s="3728" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="3016" t="s">
+      <c r="C3" s="3730" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="3018" t="s">
+      <c r="D3" s="3732" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="3020" t="s">
+      <c r="E3" s="3734" t="s">
         <v>36</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" t="s" s="3022">
+      <c r="G3" t="s" s="3736">
         <v>133</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3013" t="s">
+      <c r="A4" s="3727" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3015" t="s">
+      <c r="B4" s="3729" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="3017" t="s">
+      <c r="C4" s="3731" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3019" t="s">
+      <c r="D4" s="3733" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="3021" t="s">
+      <c r="E4" s="3735" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" t="s" s="3023">
+      <c r="G4" t="s" s="3737">
         <v>134</v>
       </c>
     </row>
@@ -14554,81 +16696,81 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="3024" t="s">
+      <c r="C3" s="3738" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="3027" t="s">
+      <c r="D3" s="3741" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="3030" t="s">
+      <c r="E3" s="3744" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="3033" t="s">
+      <c r="F3" s="3747" t="s">
         <v>46</v>
       </c>
       <c r="G3" s="13"/>
-      <c r="H3" s="3036" t="s">
+      <c r="H3" s="3750" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="3039" t="s">
+      <c r="I3" s="3753" t="s">
         <v>48</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="3042">
+      <c r="K3" t="s" s="3756">
         <v>135</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="3025" t="s">
+      <c r="C4" s="3739" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="3028" t="s">
+      <c r="D4" s="3742" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="3031" t="s">
-        <v>45</v>
+      <c r="E4" s="3745" t="s">
+        <v>50</v>
       </c>
-      <c r="F4" s="3034" t="s">
+      <c r="F4" s="3748" t="s">
         <v>51</v>
       </c>
       <c r="G4" s="13"/>
-      <c r="H4" s="3037" t="s">
+      <c r="H4" s="3751" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="3040" t="s">
+      <c r="I4" s="3754" t="s">
         <v>53</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="3043">
+      <c r="K4" t="s" s="3757">
         <v>136</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="3026" t="s">
+      <c r="C5" s="3740" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="3029" t="s">
+      <c r="D5" s="3743" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="3032" t="s">
-        <v>50</v>
+      <c r="E5" s="3746" t="s">
+        <v>45</v>
       </c>
-      <c r="F5" s="3035" t="s">
+      <c r="F5" s="3749" t="s">
         <v>56</v>
       </c>
       <c r="G5" s="13"/>
-      <c r="H5" s="3038" t="s">
+      <c r="H5" s="3752" t="s">
         <v>57</v>
       </c>
-      <c r="I5" s="3041" t="s">
+      <c r="I5" s="3755" t="s">
         <v>58</v>
       </c>
       <c r="J5"/>
-      <c r="K5" t="s" s="3044">
+      <c r="K5" t="s" s="3758">
         <v>137</v>
       </c>
     </row>
@@ -16173,32 +18315,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="3045" t="s">
+      <c r="C3" s="3759" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="3053" t="s">
+      <c r="D3" s="3767" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="3061" t="s">
+      <c r="E3" s="3775" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="3067" t="s">
+      <c r="F3" s="3781" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="3074" t="s">
+      <c r="G3" s="3788" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="3082" t="s">
+      <c r="H3" s="3796" t="s">
         <v>66</v>
       </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="3090" t="s">
+      <c r="J3" s="3804" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="3098" t="s">
+      <c r="K3" s="3812" t="s">
         <v>68</v>
       </c>
-      <c r="L3" t="s" s="3106">
+      <c r="L3" t="s" s="3820">
         <v>138</v>
       </c>
       <c r="U3" s="8"/>
@@ -16212,32 +18354,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="3046" t="s">
+      <c r="C4" s="3760" t="s">
         <v>132</v>
       </c>
-      <c r="D4" s="3054" t="s">
+      <c r="D4" s="3768" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="3062" t="s">
+      <c r="E4" s="3776" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="3068" t="s">
+      <c r="F4" s="3782" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="3075" t="s">
+      <c r="G4" s="3789" t="s">
         <v>88</v>
       </c>
-      <c r="H4" s="3083" t="s">
+      <c r="H4" s="3797" t="s">
         <v>71</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="3091" t="s">
+      <c r="J4" s="3805" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="3099" t="s">
+      <c r="K4" s="3813" t="s">
         <v>73</v>
       </c>
-      <c r="L4" t="s" s="3107">
+      <c r="L4" t="s" s="3821">
         <v>139</v>
       </c>
       <c r="U4" s="8"/>
@@ -16251,30 +18393,30 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="3047" t="s">
+      <c r="C5" s="3761" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="3055" t="s">
+      <c r="D5" s="3769" t="s">
         <v>44</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="3069" t="s">
+      <c r="F5" s="3783" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="3076" t="s">
+      <c r="G5" s="3790" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="3084" t="s">
+      <c r="H5" s="3798" t="s">
         <v>76</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="3092" t="s">
+      <c r="J5" s="3806" t="s">
         <v>77</v>
       </c>
-      <c r="K5" s="3100" t="s">
+      <c r="K5" s="3814" t="s">
         <v>78</v>
       </c>
-      <c r="L5" t="s" s="3108">
+      <c r="L5" t="s" s="3822">
         <v>140</v>
       </c>
       <c r="U5" s="8"/>
@@ -16288,32 +18430,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="3048" t="s">
+      <c r="C6" s="3762" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="3056" t="s">
+      <c r="D6" s="3770" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="3063" t="s">
+      <c r="E6" s="3777" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="3070" t="s">
+      <c r="F6" s="3784" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3077" t="s">
+      <c r="G6" s="3791" t="s">
         <v>70</v>
       </c>
-      <c r="H6" s="3085" t="s">
+      <c r="H6" s="3799" t="s">
         <v>80</v>
       </c>
       <c r="I6" s="13"/>
-      <c r="J6" s="3093" t="s">
+      <c r="J6" s="3807" t="s">
         <v>81</v>
       </c>
-      <c r="K6" s="3101" t="s">
+      <c r="K6" s="3815" t="s">
         <v>82</v>
       </c>
-      <c r="L6" t="s" s="3109">
+      <c r="L6" t="s" s="3823">
         <v>141</v>
       </c>
       <c r="U6" s="8"/>
@@ -16327,30 +18469,30 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="3049" t="s">
+      <c r="C7" s="3763" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="3057" t="s">
+      <c r="D7" s="3771" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="3064" t="s">
+      <c r="E7" s="3778" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="2969"/>
-      <c r="G7" s="3078" t="s">
+      <c r="F7" s="3683"/>
+      <c r="G7" s="3792" t="s">
         <v>145</v>
       </c>
-      <c r="H7" s="3086" t="s">
+      <c r="H7" s="3800" t="s">
         <v>84</v>
       </c>
       <c r="I7" s="13"/>
-      <c r="J7" s="3094" t="s">
+      <c r="J7" s="3808" t="s">
         <v>85</v>
       </c>
-      <c r="K7" s="3102" t="s">
+      <c r="K7" s="3816" t="s">
         <v>86</v>
       </c>
-      <c r="L7" t="s" s="3110">
+      <c r="L7" t="s" s="3824">
         <v>142</v>
       </c>
       <c r="U7" s="8"/>
@@ -16364,30 +18506,30 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="3050" t="s">
+      <c r="C8" s="3764" t="s">
         <v>132</v>
       </c>
-      <c r="D8" s="3058" t="s">
+      <c r="D8" s="3772" t="s">
         <v>49</v>
       </c>
       <c r="E8" s="22"/>
-      <c r="F8" s="3071" t="s">
+      <c r="F8" s="3785" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="3079" t="s">
+      <c r="G8" s="3793" t="s">
         <v>65</v>
       </c>
-      <c r="H8" s="3087" t="s">
+      <c r="H8" s="3801" t="s">
         <v>89</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="3095" t="s">
+      <c r="J8" s="3809" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="3103" t="s">
+      <c r="K8" s="3817" t="s">
         <v>91</v>
       </c>
-      <c r="L8" t="s" s="3111">
+      <c r="L8" t="s" s="3825">
         <v>143</v>
       </c>
       <c r="U8" s="8"/>
@@ -16401,32 +18543,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="3051" t="s">
+      <c r="C9" s="3765" t="s">
         <v>132</v>
       </c>
-      <c r="D9" s="3059" t="s">
+      <c r="D9" s="3773" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="3065" t="s">
+      <c r="E9" s="3779" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="3072" t="s">
+      <c r="F9" s="3786" t="s">
         <v>74</v>
       </c>
-      <c r="G9" s="3080" t="s">
+      <c r="G9" s="3794" t="s">
         <v>75</v>
       </c>
-      <c r="H9" s="3088" t="s">
+      <c r="H9" s="3802" t="s">
         <v>146</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="3096" t="s">
+      <c r="J9" s="3810" t="s">
         <v>147</v>
       </c>
-      <c r="K9" s="3104" t="s">
+      <c r="K9" s="3818" t="s">
         <v>148</v>
       </c>
-      <c r="L9" t="s" s="3112">
+      <c r="L9" t="s" s="3826">
         <v>149</v>
       </c>
       <c r="U9" s="8"/>
@@ -16440,32 +18582,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="3052" t="s">
+      <c r="C10" s="3766" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="3060" t="s">
+      <c r="D10" s="3774" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="3066" t="s">
+      <c r="E10" s="3780" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="3073" t="s">
+      <c r="F10" s="3787" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="3081" t="s">
+      <c r="G10" s="3795" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="3089" t="s">
+      <c r="H10" s="3803" t="s">
         <v>93</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="3097" t="s">
+      <c r="J10" s="3811" t="s">
         <v>94</v>
       </c>
-      <c r="K10" s="3105" t="s">
+      <c r="K10" s="3819" t="s">
         <v>95</v>
       </c>
-      <c r="L10" t="s" s="3113">
+      <c r="L10" t="s" s="3827">
         <v>144</v>
       </c>
       <c r="U10" s="8"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-07-26 17:58:52] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -427,7 +427,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="153">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1202,7 +1202,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="254">
+  <cellXfs count="872">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1609,6 +1609,1860 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -5073,44 +6927,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="151" t="s">
+      <c r="A3" s="769" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="153" t="s">
+      <c r="B3" s="771" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="155" t="s">
+      <c r="C3" s="773" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="157" t="s">
+      <c r="D3" s="775" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="159" t="s">
+      <c r="E3" s="777" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="161" t="s">
+      <c r="G3" s="779" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="70" x14ac:dyDescent="0.15">
-      <c r="A4" s="152" t="s">
+      <c r="A4" s="770" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="154" t="s">
+      <c r="B4" s="772" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="156" t="s">
+      <c r="C4" s="774" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="158" t="s">
+      <c r="D4" s="776" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="160" t="s">
+      <c r="E4" s="778" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="162" t="s">
+      <c r="G4" s="780" t="s">
         <v>99</v>
       </c>
     </row>
@@ -6264,81 +8118,81 @@
     <row r="3" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="163" t="s">
+      <c r="C3" s="781" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="166" t="s">
+      <c r="D3" s="784" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="169" t="s">
+      <c r="E3" s="787" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="172" t="s">
+      <c r="F3" s="790" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="10"/>
-      <c r="H3" s="175" t="s">
+      <c r="H3" s="793" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="178" t="s">
+      <c r="I3" s="796" t="s">
         <v>46</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="181" t="s">
+      <c r="K3" s="799" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="164" t="s">
+      <c r="C4" s="782" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="167" t="s">
+      <c r="D4" s="785" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="170" t="s">
+      <c r="E4" s="788" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="173" t="s">
+      <c r="F4" s="791" t="s">
         <v>49</v>
       </c>
       <c r="G4" s="10"/>
-      <c r="H4" s="176" t="s">
+      <c r="H4" s="794" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="179" t="s">
+      <c r="I4" s="797" t="s">
         <v>51</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="182" t="s">
+      <c r="K4" s="800" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="165" t="s">
+      <c r="C5" s="783" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="168" t="s">
+      <c r="D5" s="786" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="171" t="s">
+      <c r="E5" s="789" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="174" t="s">
+      <c r="F5" s="792" t="s">
         <v>54</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="177" t="s">
+      <c r="H5" s="795" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="180" t="s">
+      <c r="I5" s="798" t="s">
         <v>56</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="183" t="s">
+      <c r="K5" s="801" t="s">
         <v>102</v>
       </c>
     </row>
@@ -7878,32 +9732,32 @@
     <row r="3" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="184" t="s">
+      <c r="C3" s="802" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="192" t="s">
+      <c r="D3" s="810" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="200" t="s">
+      <c r="E3" s="818" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="206" t="s">
+      <c r="F3" s="824" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="214" t="s">
+      <c r="G3" s="832" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="222" t="s">
+      <c r="H3" s="840" t="s">
         <v>120</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="J3" s="230" t="s">
+      <c r="J3" s="848" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="238" t="s">
+      <c r="K3" s="856" t="s">
         <v>136</v>
       </c>
-      <c r="L3" s="246" t="s">
+      <c r="L3" s="864" t="s">
         <v>144</v>
       </c>
       <c r="U3" s="6"/>
@@ -7917,32 +9771,32 @@
     <row r="4" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="185" t="s">
+      <c r="C4" s="803" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="193" t="s">
+      <c r="D4" s="811" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="201" t="s">
+      <c r="E4" s="819" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="207" t="s">
+      <c r="F4" s="825" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="215" t="s">
+      <c r="G4" s="833" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="223" t="s">
+      <c r="H4" s="841" t="s">
         <v>121</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="231" t="s">
+      <c r="J4" s="849" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="239" t="s">
+      <c r="K4" s="857" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="247" t="s">
+      <c r="L4" s="865" t="s">
         <v>145</v>
       </c>
       <c r="U4" s="6"/>
@@ -7956,30 +9810,30 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="186" t="s">
+      <c r="C5" s="804" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="194" t="s">
+      <c r="D5" s="812" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="208" t="s">
+      <c r="F5" s="826" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="216" t="s">
+      <c r="G5" s="834" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="224" t="s">
+      <c r="H5" s="842" t="s">
         <v>122</v>
       </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="232" t="s">
+      <c r="J5" s="850" t="s">
         <v>130</v>
       </c>
-      <c r="K5" s="240" t="s">
+      <c r="K5" s="858" t="s">
         <v>138</v>
       </c>
-      <c r="L5" s="248" t="s">
+      <c r="L5" s="866" t="s">
         <v>146</v>
       </c>
       <c r="U5" s="6"/>
@@ -7993,32 +9847,32 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="187" t="s">
+      <c r="C6" s="805" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="195" t="s">
+      <c r="D6" s="813" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="202" t="s">
+      <c r="E6" s="820" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="209" t="s">
+      <c r="F6" s="827" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="217" t="s">
+      <c r="G6" s="835" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="225" t="s">
+      <c r="H6" s="843" t="s">
         <v>123</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="233" t="s">
+      <c r="J6" s="851" t="s">
         <v>131</v>
       </c>
-      <c r="K6" s="241" t="s">
+      <c r="K6" s="859" t="s">
         <v>139</v>
       </c>
-      <c r="L6" s="249" t="s">
+      <c r="L6" s="867" t="s">
         <v>147</v>
       </c>
       <c r="U6" s="6"/>
@@ -8032,32 +9886,32 @@
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="188" t="s">
+      <c r="C7" s="806" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="196" t="s">
+      <c r="D7" s="814" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="203" t="s">
+      <c r="E7" s="821" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="210" t="s">
+      <c r="F7" s="828" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="218" t="s">
+      <c r="G7" s="836" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="226" t="s">
+      <c r="H7" s="844" t="s">
         <v>124</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="234" t="s">
+      <c r="J7" s="852" t="s">
         <v>132</v>
       </c>
-      <c r="K7" s="242" t="s">
+      <c r="K7" s="860" t="s">
         <v>140</v>
       </c>
-      <c r="L7" s="250" t="s">
+      <c r="L7" s="868" t="s">
         <v>148</v>
       </c>
       <c r="U7" s="6"/>
@@ -8071,30 +9925,30 @@
     <row r="8" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8"/>
-      <c r="C8" s="189" t="s">
+      <c r="C8" s="807" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="197" t="s">
+      <c r="D8" s="815" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="211" t="s">
+      <c r="F8" s="829" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="219" t="s">
+      <c r="G8" s="837" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="227" t="s">
+      <c r="H8" s="845" t="s">
         <v>125</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="235" t="s">
+      <c r="J8" s="853" t="s">
         <v>133</v>
       </c>
-      <c r="K8" s="243" t="s">
+      <c r="K8" s="861" t="s">
         <v>141</v>
       </c>
-      <c r="L8" s="251" t="s">
+      <c r="L8" s="869" t="s">
         <v>149</v>
       </c>
       <c r="U8" s="6"/>
@@ -8108,32 +9962,32 @@
     <row r="9" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9"/>
-      <c r="C9" s="190" t="s">
+      <c r="C9" s="808" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="198" t="s">
+      <c r="D9" s="816" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="204" t="s">
+      <c r="E9" s="822" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="212" t="s">
+      <c r="F9" s="830" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="220" t="s">
+      <c r="G9" s="838" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="228" t="s">
+      <c r="H9" s="846" t="s">
         <v>126</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="236" t="s">
+      <c r="J9" s="854" t="s">
         <v>134</v>
       </c>
-      <c r="K9" s="244" t="s">
+      <c r="K9" s="862" t="s">
         <v>142</v>
       </c>
-      <c r="L9" s="252" t="s">
+      <c r="L9" s="870" t="s">
         <v>150</v>
       </c>
       <c r="U9" s="6"/>
@@ -8147,32 +10001,32 @@
     <row r="10" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10"/>
-      <c r="C10" s="191" t="s">
+      <c r="C10" s="809" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="199" t="s">
+      <c r="D10" s="817" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="205" t="s">
+      <c r="E10" s="823" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="213" t="s">
+      <c r="F10" s="831" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="221" t="s">
+      <c r="G10" s="839" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="229" t="s">
+      <c r="H10" s="847" t="s">
         <v>127</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="237" t="s">
+      <c r="J10" s="855" t="s">
         <v>135</v>
       </c>
-      <c r="K10" s="245" t="s">
+      <c r="K10" s="863" t="s">
         <v>143</v>
       </c>
-      <c r="L10" s="253" t="s">
+      <c r="L10" s="871" t="s">
         <v>151</v>
       </c>
       <c r="U10" s="6"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-03 19:15:13]  fixed missing standards"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -427,7 +427,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="153">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1202,7 +1202,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="872">
+  <cellXfs count="975">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1609,6 +1609,315 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -6927,44 +7236,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="769" t="s">
+      <c r="A3" s="872" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="771" t="s">
+      <c r="B3" s="874" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="773" t="s">
+      <c r="C3" s="876" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="775" t="s">
+      <c r="D3" s="878" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="777" t="s">
+      <c r="E3" s="880" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="779" t="s">
+      <c r="G3" s="882" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="70" x14ac:dyDescent="0.15">
-      <c r="A4" s="770" t="s">
+      <c r="A4" s="873" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="772" t="s">
+      <c r="B4" s="875" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="774" t="s">
+      <c r="C4" s="877" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="776" t="s">
+      <c r="D4" s="879" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="778" t="s">
+      <c r="E4" s="881" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="780" t="s">
+      <c r="G4" s="883" t="s">
         <v>99</v>
       </c>
     </row>
@@ -8118,81 +8427,81 @@
     <row r="3" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="781" t="s">
+      <c r="C3" s="884" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="784" t="s">
+      <c r="D3" s="887" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="787" t="s">
+      <c r="E3" s="890" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="790" t="s">
+      <c r="F3" s="893" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="10"/>
-      <c r="H3" s="793" t="s">
+      <c r="H3" s="896" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="796" t="s">
+      <c r="I3" s="899" t="s">
         <v>46</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="799" t="s">
+      <c r="K3" s="902" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="782" t="s">
+      <c r="C4" s="885" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="785" t="s">
+      <c r="D4" s="888" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="788" t="s">
+      <c r="E4" s="891" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="791" t="s">
+      <c r="F4" s="894" t="s">
         <v>49</v>
       </c>
       <c r="G4" s="10"/>
-      <c r="H4" s="794" t="s">
+      <c r="H4" s="897" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="797" t="s">
+      <c r="I4" s="900" t="s">
         <v>51</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="800" t="s">
+      <c r="K4" s="903" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="783" t="s">
+      <c r="C5" s="886" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="786" t="s">
+      <c r="D5" s="889" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="789" t="s">
+      <c r="E5" s="892" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="792" t="s">
+      <c r="F5" s="895" t="s">
         <v>54</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="795" t="s">
+      <c r="H5" s="898" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="798" t="s">
+      <c r="I5" s="901" t="s">
         <v>56</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="801" t="s">
+      <c r="K5" s="904" t="s">
         <v>102</v>
       </c>
     </row>
@@ -9732,32 +10041,32 @@
     <row r="3" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="802" t="s">
+      <c r="C3" s="905" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="810" t="s">
+      <c r="D3" s="913" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="818" t="s">
+      <c r="E3" s="921" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="824" t="s">
+      <c r="F3" s="927" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="832" t="s">
+      <c r="G3" s="935" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="840" t="s">
+      <c r="H3" s="943" t="s">
         <v>120</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="J3" s="848" t="s">
+      <c r="J3" s="951" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="856" t="s">
+      <c r="K3" s="959" t="s">
         <v>136</v>
       </c>
-      <c r="L3" s="864" t="s">
+      <c r="L3" s="967" t="s">
         <v>144</v>
       </c>
       <c r="U3" s="6"/>
@@ -9771,32 +10080,32 @@
     <row r="4" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="803" t="s">
+      <c r="C4" s="906" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="811" t="s">
+      <c r="D4" s="914" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="819" t="s">
+      <c r="E4" s="922" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="825" t="s">
+      <c r="F4" s="928" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="833" t="s">
+      <c r="G4" s="936" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="841" t="s">
+      <c r="H4" s="944" t="s">
         <v>121</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="849" t="s">
+      <c r="J4" s="952" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="857" t="s">
+      <c r="K4" s="960" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="865" t="s">
+      <c r="L4" s="968" t="s">
         <v>145</v>
       </c>
       <c r="U4" s="6"/>
@@ -9810,30 +10119,30 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="804" t="s">
+      <c r="C5" s="907" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="812" t="s">
+      <c r="D5" s="915" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="826" t="s">
+      <c r="F5" s="929" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="834" t="s">
+      <c r="G5" s="937" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="842" t="s">
+      <c r="H5" s="945" t="s">
         <v>122</v>
       </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="850" t="s">
+      <c r="J5" s="953" t="s">
         <v>130</v>
       </c>
-      <c r="K5" s="858" t="s">
+      <c r="K5" s="961" t="s">
         <v>138</v>
       </c>
-      <c r="L5" s="866" t="s">
+      <c r="L5" s="969" t="s">
         <v>146</v>
       </c>
       <c r="U5" s="6"/>
@@ -9847,32 +10156,32 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="805" t="s">
+      <c r="C6" s="908" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="813" t="s">
+      <c r="D6" s="916" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="820" t="s">
+      <c r="E6" s="923" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="827" t="s">
+      <c r="F6" s="930" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="835" t="s">
+      <c r="G6" s="938" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="843" t="s">
+      <c r="H6" s="946" t="s">
         <v>123</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="851" t="s">
+      <c r="J6" s="954" t="s">
         <v>131</v>
       </c>
-      <c r="K6" s="859" t="s">
+      <c r="K6" s="962" t="s">
         <v>139</v>
       </c>
-      <c r="L6" s="867" t="s">
+      <c r="L6" s="970" t="s">
         <v>147</v>
       </c>
       <c r="U6" s="6"/>
@@ -9886,32 +10195,32 @@
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="806" t="s">
+      <c r="C7" s="909" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="814" t="s">
+      <c r="D7" s="917" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="821" t="s">
+      <c r="E7" s="924" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="828" t="s">
+      <c r="F7" s="931" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="836" t="s">
+      <c r="G7" s="939" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="844" t="s">
+      <c r="H7" s="947" t="s">
         <v>124</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="852" t="s">
+      <c r="J7" s="955" t="s">
         <v>132</v>
       </c>
-      <c r="K7" s="860" t="s">
+      <c r="K7" s="963" t="s">
         <v>140</v>
       </c>
-      <c r="L7" s="868" t="s">
+      <c r="L7" s="971" t="s">
         <v>148</v>
       </c>
       <c r="U7" s="6"/>
@@ -9925,30 +10234,30 @@
     <row r="8" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8"/>
-      <c r="C8" s="807" t="s">
+      <c r="C8" s="910" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="815" t="s">
+      <c r="D8" s="918" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="829" t="s">
+      <c r="F8" s="932" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="837" t="s">
+      <c r="G8" s="940" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="845" t="s">
+      <c r="H8" s="948" t="s">
         <v>125</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="853" t="s">
+      <c r="J8" s="956" t="s">
         <v>133</v>
       </c>
-      <c r="K8" s="861" t="s">
+      <c r="K8" s="964" t="s">
         <v>141</v>
       </c>
-      <c r="L8" s="869" t="s">
+      <c r="L8" s="972" t="s">
         <v>149</v>
       </c>
       <c r="U8" s="6"/>
@@ -9962,32 +10271,32 @@
     <row r="9" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9"/>
-      <c r="C9" s="808" t="s">
+      <c r="C9" s="911" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="816" t="s">
+      <c r="D9" s="919" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="822" t="s">
+      <c r="E9" s="925" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="830" t="s">
+      <c r="F9" s="933" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="838" t="s">
+      <c r="G9" s="941" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="846" t="s">
+      <c r="H9" s="949" t="s">
         <v>126</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="854" t="s">
+      <c r="J9" s="957" t="s">
         <v>134</v>
       </c>
-      <c r="K9" s="862" t="s">
+      <c r="K9" s="965" t="s">
         <v>142</v>
       </c>
-      <c r="L9" s="870" t="s">
+      <c r="L9" s="973" t="s">
         <v>150</v>
       </c>
       <c r="U9" s="6"/>
@@ -10001,32 +10310,32 @@
     <row r="10" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10"/>
-      <c r="C10" s="809" t="s">
+      <c r="C10" s="912" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="817" t="s">
+      <c r="D10" s="920" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="823" t="s">
+      <c r="E10" s="926" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="831" t="s">
+      <c r="F10" s="934" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="839" t="s">
+      <c r="G10" s="942" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="847" t="s">
+      <c r="H10" s="950" t="s">
         <v>127</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="855" t="s">
+      <c r="J10" s="958" t="s">
         <v>135</v>
       </c>
-      <c r="K10" s="863" t="s">
+      <c r="K10" s="966" t="s">
         <v>143</v>
       </c>
-      <c r="L10" s="871" t="s">
+      <c r="L10" s="974" t="s">
         <v>151</v>
       </c>
       <c r="U10" s="6"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-12 20:27:42]  "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -427,7 +427,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="153">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1202,7 +1202,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="975">
+  <cellXfs count="1696">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1609,6 +1609,2169 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -7236,44 +9399,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="872" t="s">
+      <c r="A3" s="1593" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="874" t="s">
+      <c r="B3" s="1595" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="876" t="s">
+      <c r="C3" s="1597" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="878" t="s">
+      <c r="D3" s="1599" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="880" t="s">
+      <c r="E3" s="1601" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="882" t="s">
+      <c r="G3" s="1603" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="70" x14ac:dyDescent="0.15">
-      <c r="A4" s="873" t="s">
+      <c r="A4" s="1594" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="875" t="s">
+      <c r="B4" s="1596" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="877" t="s">
+      <c r="C4" s="1598" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="879" t="s">
+      <c r="D4" s="1600" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="881" t="s">
+      <c r="E4" s="1602" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="883" t="s">
+      <c r="G4" s="1604" t="s">
         <v>99</v>
       </c>
     </row>
@@ -8427,81 +10590,81 @@
     <row r="3" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="884" t="s">
+      <c r="C3" s="1605" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="887" t="s">
+      <c r="D3" s="1608" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="890" t="s">
+      <c r="E3" s="1611" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="893" t="s">
+      <c r="F3" s="1614" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="10"/>
-      <c r="H3" s="896" t="s">
+      <c r="H3" s="1617" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="899" t="s">
+      <c r="I3" s="1620" t="s">
         <v>46</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="902" t="s">
+      <c r="K3" s="1623" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="885" t="s">
+      <c r="C4" s="1606" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="888" t="s">
+      <c r="D4" s="1609" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="891" t="s">
+      <c r="E4" s="1612" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="894" t="s">
+      <c r="F4" s="1615" t="s">
         <v>49</v>
       </c>
       <c r="G4" s="10"/>
-      <c r="H4" s="897" t="s">
+      <c r="H4" s="1618" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="900" t="s">
+      <c r="I4" s="1621" t="s">
         <v>51</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="903" t="s">
+      <c r="K4" s="1624" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="886" t="s">
+      <c r="C5" s="1607" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="889" t="s">
+      <c r="D5" s="1610" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="892" t="s">
+      <c r="E5" s="1613" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="895" t="s">
+      <c r="F5" s="1616" t="s">
         <v>54</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="898" t="s">
+      <c r="H5" s="1619" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="901" t="s">
+      <c r="I5" s="1622" t="s">
         <v>56</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="904" t="s">
+      <c r="K5" s="1625" t="s">
         <v>102</v>
       </c>
     </row>
@@ -10041,32 +12204,32 @@
     <row r="3" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="905" t="s">
+      <c r="C3" s="1626" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="913" t="s">
+      <c r="D3" s="1634" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="921" t="s">
+      <c r="E3" s="1642" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="927" t="s">
+      <c r="F3" s="1648" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="935" t="s">
+      <c r="G3" s="1656" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="943" t="s">
+      <c r="H3" s="1664" t="s">
         <v>120</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="J3" s="951" t="s">
+      <c r="J3" s="1672" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="959" t="s">
+      <c r="K3" s="1680" t="s">
         <v>136</v>
       </c>
-      <c r="L3" s="967" t="s">
+      <c r="L3" s="1688" t="s">
         <v>144</v>
       </c>
       <c r="U3" s="6"/>
@@ -10080,32 +12243,32 @@
     <row r="4" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="906" t="s">
+      <c r="C4" s="1627" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="914" t="s">
+      <c r="D4" s="1635" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="922" t="s">
+      <c r="E4" s="1643" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="928" t="s">
+      <c r="F4" s="1649" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="936" t="s">
+      <c r="G4" s="1657" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="944" t="s">
+      <c r="H4" s="1665" t="s">
         <v>121</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="952" t="s">
+      <c r="J4" s="1673" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="960" t="s">
+      <c r="K4" s="1681" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="968" t="s">
+      <c r="L4" s="1689" t="s">
         <v>145</v>
       </c>
       <c r="U4" s="6"/>
@@ -10119,30 +12282,30 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="907" t="s">
+      <c r="C5" s="1628" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="915" t="s">
+      <c r="D5" s="1636" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="929" t="s">
+      <c r="F5" s="1650" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="937" t="s">
+      <c r="G5" s="1658" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="945" t="s">
+      <c r="H5" s="1666" t="s">
         <v>122</v>
       </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="953" t="s">
+      <c r="J5" s="1674" t="s">
         <v>130</v>
       </c>
-      <c r="K5" s="961" t="s">
+      <c r="K5" s="1682" t="s">
         <v>138</v>
       </c>
-      <c r="L5" s="969" t="s">
+      <c r="L5" s="1690" t="s">
         <v>146</v>
       </c>
       <c r="U5" s="6"/>
@@ -10156,32 +12319,32 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="908" t="s">
+      <c r="C6" s="1629" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="916" t="s">
+      <c r="D6" s="1637" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="923" t="s">
+      <c r="E6" s="1644" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="930" t="s">
+      <c r="F6" s="1651" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="938" t="s">
+      <c r="G6" s="1659" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="946" t="s">
+      <c r="H6" s="1667" t="s">
         <v>123</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="954" t="s">
+      <c r="J6" s="1675" t="s">
         <v>131</v>
       </c>
-      <c r="K6" s="962" t="s">
+      <c r="K6" s="1683" t="s">
         <v>139</v>
       </c>
-      <c r="L6" s="970" t="s">
+      <c r="L6" s="1691" t="s">
         <v>147</v>
       </c>
       <c r="U6" s="6"/>
@@ -10195,32 +12358,32 @@
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="909" t="s">
+      <c r="C7" s="1630" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="917" t="s">
+      <c r="D7" s="1638" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="924" t="s">
+      <c r="E7" s="1645" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="931" t="s">
+      <c r="F7" s="1652" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="939" t="s">
+      <c r="G7" s="1660" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="947" t="s">
+      <c r="H7" s="1668" t="s">
         <v>124</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="955" t="s">
+      <c r="J7" s="1676" t="s">
         <v>132</v>
       </c>
-      <c r="K7" s="963" t="s">
+      <c r="K7" s="1684" t="s">
         <v>140</v>
       </c>
-      <c r="L7" s="971" t="s">
+      <c r="L7" s="1692" t="s">
         <v>148</v>
       </c>
       <c r="U7" s="6"/>
@@ -10234,30 +12397,30 @@
     <row r="8" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8"/>
-      <c r="C8" s="910" t="s">
+      <c r="C8" s="1631" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="918" t="s">
+      <c r="D8" s="1639" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="932" t="s">
+      <c r="F8" s="1653" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="940" t="s">
+      <c r="G8" s="1661" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="948" t="s">
+      <c r="H8" s="1669" t="s">
         <v>125</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="956" t="s">
+      <c r="J8" s="1677" t="s">
         <v>133</v>
       </c>
-      <c r="K8" s="964" t="s">
+      <c r="K8" s="1685" t="s">
         <v>141</v>
       </c>
-      <c r="L8" s="972" t="s">
+      <c r="L8" s="1693" t="s">
         <v>149</v>
       </c>
       <c r="U8" s="6"/>
@@ -10271,32 +12434,32 @@
     <row r="9" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9"/>
-      <c r="C9" s="911" t="s">
+      <c r="C9" s="1632" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="919" t="s">
+      <c r="D9" s="1640" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="925" t="s">
+      <c r="E9" s="1646" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="933" t="s">
+      <c r="F9" s="1654" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="941" t="s">
+      <c r="G9" s="1662" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="949" t="s">
+      <c r="H9" s="1670" t="s">
         <v>126</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="957" t="s">
+      <c r="J9" s="1678" t="s">
         <v>134</v>
       </c>
-      <c r="K9" s="965" t="s">
+      <c r="K9" s="1686" t="s">
         <v>142</v>
       </c>
-      <c r="L9" s="973" t="s">
+      <c r="L9" s="1694" t="s">
         <v>150</v>
       </c>
       <c r="U9" s="6"/>
@@ -10310,32 +12473,32 @@
     <row r="10" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10"/>
-      <c r="C10" s="912" t="s">
+      <c r="C10" s="1633" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="920" t="s">
+      <c r="D10" s="1641" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="926" t="s">
+      <c r="E10" s="1647" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="934" t="s">
+      <c r="F10" s="1655" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="942" t="s">
+      <c r="G10" s="1663" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="950" t="s">
+      <c r="H10" s="1671" t="s">
         <v>127</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="958" t="s">
+      <c r="J10" s="1679" t="s">
         <v>135</v>
       </c>
-      <c r="K10" s="966" t="s">
+      <c r="K10" s="1687" t="s">
         <v>143</v>
       </c>
-      <c r="L10" s="974" t="s">
+      <c r="L10" s="1695" t="s">
         <v>151</v>
       </c>
       <c r="U10" s="6"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-15 08:50:32]  "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -427,7 +427,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1779" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="153">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1202,7 +1202,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1696">
+  <cellXfs count="1799">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1609,6 +1609,315 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="1"/>
@@ -9399,44 +9708,44 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="56" x14ac:dyDescent="0.15">
-      <c r="A3" s="1593" t="s">
+      <c r="A3" s="1696" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1595" t="s">
+      <c r="B3" s="1698" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="1597" t="s">
+      <c r="C3" s="1700" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1599" t="s">
+      <c r="D3" s="1702" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="1601" t="s">
+      <c r="E3" s="1704" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="10"/>
-      <c r="G3" s="1603" t="s">
+      <c r="G3" s="1706" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="70" x14ac:dyDescent="0.15">
-      <c r="A4" s="1594" t="s">
+      <c r="A4" s="1697" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1596" t="s">
+      <c r="B4" s="1699" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1598" t="s">
+      <c r="C4" s="1701" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1600" t="s">
+      <c r="D4" s="1703" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="1602" t="s">
+      <c r="E4" s="1705" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="10"/>
-      <c r="G4" s="1604" t="s">
+      <c r="G4" s="1707" t="s">
         <v>99</v>
       </c>
     </row>
@@ -10590,81 +10899,81 @@
     <row r="3" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="1605" t="s">
+      <c r="C3" s="1708" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="1608" t="s">
+      <c r="D3" s="1711" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="1611" t="s">
+      <c r="E3" s="1714" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="1614" t="s">
+      <c r="F3" s="1717" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="10"/>
-      <c r="H3" s="1617" t="s">
+      <c r="H3" s="1720" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="1620" t="s">
+      <c r="I3" s="1723" t="s">
         <v>46</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="1623" t="s">
+      <c r="K3" s="1726" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="126" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="1606" t="s">
+      <c r="C4" s="1709" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="1609" t="s">
+      <c r="D4" s="1712" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="1612" t="s">
+      <c r="E4" s="1715" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="1615" t="s">
+      <c r="F4" s="1718" t="s">
         <v>49</v>
       </c>
       <c r="G4" s="10"/>
-      <c r="H4" s="1618" t="s">
+      <c r="H4" s="1721" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="1621" t="s">
+      <c r="I4" s="1724" t="s">
         <v>51</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1624" t="s">
+      <c r="K4" s="1727" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="112" x14ac:dyDescent="0.15">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="1607" t="s">
+      <c r="C5" s="1710" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="1610" t="s">
+      <c r="D5" s="1713" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="1613" t="s">
+      <c r="E5" s="1716" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="1616" t="s">
+      <c r="F5" s="1719" t="s">
         <v>54</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="H5" s="1619" t="s">
+      <c r="H5" s="1722" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="1622" t="s">
+      <c r="I5" s="1725" t="s">
         <v>56</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1625" t="s">
+      <c r="K5" s="1728" t="s">
         <v>102</v>
       </c>
     </row>
@@ -12204,32 +12513,32 @@
     <row r="3" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3"/>
-      <c r="C3" s="1626" t="s">
+      <c r="C3" s="1729" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="1634" t="s">
+      <c r="D3" s="1737" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="1642" t="s">
+      <c r="E3" s="1745" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="1648" t="s">
+      <c r="F3" s="1751" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="1656" t="s">
+      <c r="G3" s="1759" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="1664" t="s">
+      <c r="H3" s="1767" t="s">
         <v>120</v>
       </c>
       <c r="I3" s="10"/>
-      <c r="J3" s="1672" t="s">
+      <c r="J3" s="1775" t="s">
         <v>128</v>
       </c>
-      <c r="K3" s="1680" t="s">
+      <c r="K3" s="1783" t="s">
         <v>136</v>
       </c>
-      <c r="L3" s="1688" t="s">
+      <c r="L3" s="1791" t="s">
         <v>144</v>
       </c>
       <c r="U3" s="6"/>
@@ -12243,32 +12552,32 @@
     <row r="4" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
       <c r="B4"/>
-      <c r="C4" s="1627" t="s">
+      <c r="C4" s="1730" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="1635" t="s">
+      <c r="D4" s="1738" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="1643" t="s">
+      <c r="E4" s="1746" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="1649" t="s">
+      <c r="F4" s="1752" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="1657" t="s">
+      <c r="G4" s="1760" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="1665" t="s">
+      <c r="H4" s="1768" t="s">
         <v>121</v>
       </c>
       <c r="I4" s="10"/>
-      <c r="J4" s="1673" t="s">
+      <c r="J4" s="1776" t="s">
         <v>129</v>
       </c>
-      <c r="K4" s="1681" t="s">
+      <c r="K4" s="1784" t="s">
         <v>137</v>
       </c>
-      <c r="L4" s="1689" t="s">
+      <c r="L4" s="1792" t="s">
         <v>145</v>
       </c>
       <c r="U4" s="6"/>
@@ -12282,30 +12591,30 @@
     <row r="5" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
       <c r="B5"/>
-      <c r="C5" s="1628" t="s">
+      <c r="C5" s="1731" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="1636" t="s">
+      <c r="D5" s="1739" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="10"/>
-      <c r="F5" s="1650" t="s">
+      <c r="F5" s="1753" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="1658" t="s">
+      <c r="G5" s="1761" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="1666" t="s">
+      <c r="H5" s="1769" t="s">
         <v>122</v>
       </c>
       <c r="I5" s="10"/>
-      <c r="J5" s="1674" t="s">
+      <c r="J5" s="1777" t="s">
         <v>130</v>
       </c>
-      <c r="K5" s="1682" t="s">
+      <c r="K5" s="1785" t="s">
         <v>138</v>
       </c>
-      <c r="L5" s="1690" t="s">
+      <c r="L5" s="1793" t="s">
         <v>146</v>
       </c>
       <c r="U5" s="6"/>
@@ -12319,32 +12628,32 @@
     <row r="6" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A6" s="18"/>
       <c r="B6"/>
-      <c r="C6" s="1629" t="s">
+      <c r="C6" s="1732" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="1637" t="s">
+      <c r="D6" s="1740" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="1644" t="s">
+      <c r="E6" s="1747" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="1651" t="s">
+      <c r="F6" s="1754" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="1659" t="s">
+      <c r="G6" s="1762" t="s">
         <v>115</v>
       </c>
-      <c r="H6" s="1667" t="s">
+      <c r="H6" s="1770" t="s">
         <v>123</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="1675" t="s">
+      <c r="J6" s="1778" t="s">
         <v>131</v>
       </c>
-      <c r="K6" s="1683" t="s">
+      <c r="K6" s="1786" t="s">
         <v>139</v>
       </c>
-      <c r="L6" s="1691" t="s">
+      <c r="L6" s="1794" t="s">
         <v>147</v>
       </c>
       <c r="U6" s="6"/>
@@ -12358,32 +12667,32 @@
     <row r="7" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7"/>
-      <c r="C7" s="1630" t="s">
+      <c r="C7" s="1733" t="s">
         <v>97</v>
       </c>
-      <c r="D7" s="1638" t="s">
+      <c r="D7" s="1741" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="1645" t="s">
+      <c r="E7" s="1748" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="1652" t="s">
+      <c r="F7" s="1755" t="s">
         <v>108</v>
       </c>
-      <c r="G7" s="1660" t="s">
+      <c r="G7" s="1763" t="s">
         <v>116</v>
       </c>
-      <c r="H7" s="1668" t="s">
+      <c r="H7" s="1771" t="s">
         <v>124</v>
       </c>
       <c r="I7" s="10"/>
-      <c r="J7" s="1676" t="s">
+      <c r="J7" s="1779" t="s">
         <v>132</v>
       </c>
-      <c r="K7" s="1684" t="s">
+      <c r="K7" s="1787" t="s">
         <v>140</v>
       </c>
-      <c r="L7" s="1692" t="s">
+      <c r="L7" s="1795" t="s">
         <v>148</v>
       </c>
       <c r="U7" s="6"/>
@@ -12397,30 +12706,30 @@
     <row r="8" spans="1:31" ht="100" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8"/>
-      <c r="C8" s="1631" t="s">
+      <c r="C8" s="1734" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="1639" t="s">
+      <c r="D8" s="1742" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="1653" t="s">
+      <c r="F8" s="1756" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="1661" t="s">
+      <c r="G8" s="1764" t="s">
         <v>117</v>
       </c>
-      <c r="H8" s="1669" t="s">
+      <c r="H8" s="1772" t="s">
         <v>125</v>
       </c>
       <c r="I8" s="10"/>
-      <c r="J8" s="1677" t="s">
+      <c r="J8" s="1780" t="s">
         <v>133</v>
       </c>
-      <c r="K8" s="1685" t="s">
+      <c r="K8" s="1788" t="s">
         <v>141</v>
       </c>
-      <c r="L8" s="1693" t="s">
+      <c r="L8" s="1796" t="s">
         <v>149</v>
       </c>
       <c r="U8" s="6"/>
@@ -12434,32 +12743,32 @@
     <row r="9" spans="1:31" ht="114" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9"/>
-      <c r="C9" s="1632" t="s">
+      <c r="C9" s="1735" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="1640" t="s">
+      <c r="D9" s="1743" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="1646" t="s">
+      <c r="E9" s="1749" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="1654" t="s">
+      <c r="F9" s="1757" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="1662" t="s">
+      <c r="G9" s="1765" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="1670" t="s">
+      <c r="H9" s="1773" t="s">
         <v>126</v>
       </c>
       <c r="I9" s="10"/>
-      <c r="J9" s="1678" t="s">
+      <c r="J9" s="1781" t="s">
         <v>134</v>
       </c>
-      <c r="K9" s="1686" t="s">
+      <c r="K9" s="1789" t="s">
         <v>142</v>
       </c>
-      <c r="L9" s="1694" t="s">
+      <c r="L9" s="1797" t="s">
         <v>150</v>
       </c>
       <c r="U9" s="6"/>
@@ -12473,32 +12782,32 @@
     <row r="10" spans="1:31" ht="86" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10"/>
-      <c r="C10" s="1633" t="s">
+      <c r="C10" s="1736" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="1641" t="s">
+      <c r="D10" s="1744" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="1647" t="s">
+      <c r="E10" s="1750" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="1655" t="s">
+      <c r="F10" s="1758" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1663" t="s">
+      <c r="G10" s="1766" t="s">
         <v>119</v>
       </c>
-      <c r="H10" s="1671" t="s">
+      <c r="H10" s="1774" t="s">
         <v>127</v>
       </c>
       <c r="I10" s="10"/>
-      <c r="J10" s="1679" t="s">
+      <c r="J10" s="1782" t="s">
         <v>135</v>
       </c>
-      <c r="K10" s="1687" t="s">
+      <c r="K10" s="1790" t="s">
         <v>143</v>
       </c>
-      <c r="L10" s="1695" t="s">
+      <c r="L10" s="1798" t="s">
         <v>151</v>
       </c>
       <c r="U10" s="6"/>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-25 16:46:26]  fixed teaching-mat json indent...?"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="159">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -704,6 +704,9 @@
   <si>
     <t>For best experience, always edit in Google Sheets.</t>
   </si>
+  <si>
+    <t>(P Assessment (TEACHER))</t>
+  </si>
 </sst>
 </file>
 
@@ -1002,7 +1005,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="266">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1114,6 +1117,330 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -4531,44 +4858,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="158" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="160" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="164" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="63" t="s">
+      <c r="E3" s="166" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="65" t="s">
+      <c r="G3" s="168" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="159" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="161" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="167" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="169" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5725,81 +6052,81 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="67" t="s">
+      <c r="C3" s="170" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="173" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="176" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="179" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="13"/>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="182" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="82" t="s">
+      <c r="I3" s="185" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="85" t="s">
+      <c r="K3" s="188" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="171" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="174" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="177" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="F4" s="180" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="13"/>
-      <c r="H4" s="80" t="s">
+      <c r="H4" s="183" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="83" t="s">
+      <c r="I4" s="186" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="86" t="s">
+      <c r="K4" s="189" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="178" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="78" t="s">
+      <c r="F5" s="181" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="13"/>
-      <c r="H5" s="81" t="s">
+      <c r="H5" s="184" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="84" t="s">
+      <c r="I5" s="187" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="87" t="s">
+      <c r="K5" s="190" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7344,32 +7671,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="88" t="s">
+      <c r="C3" s="191" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="96" t="s">
+      <c r="D3" s="199" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="104" t="s">
+      <c r="E3" s="207" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="110" t="s">
+      <c r="F3" s="213" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="118" t="s">
+      <c r="G3" s="221" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="126" t="s">
+      <c r="H3" s="229" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="134" t="s">
+      <c r="J3" s="237" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="142" t="s">
+      <c r="K3" s="245" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="150" t="s">
+      <c r="L3" s="253" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -7383,32 +7710,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="89" t="s">
+      <c r="C4" s="192" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="200" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="105" t="s">
+      <c r="E4" s="208" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="111" t="s">
+      <c r="F4" s="214" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="119" t="s">
+      <c r="G4" s="222" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="127" t="s">
+      <c r="H4" s="230" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="135" t="s">
+      <c r="J4" s="238" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="143" t="s">
+      <c r="K4" s="246" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="151" t="s">
+      <c r="L4" s="254" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -7422,30 +7749,30 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="90" t="s">
+      <c r="C5" s="193" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="201" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="112" t="s">
+      <c r="F5" s="215" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="120" t="s">
+      <c r="G5" s="223" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="128" t="s">
+      <c r="H5" s="231" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="136" t="s">
+      <c r="J5" s="239" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="144" t="s">
+      <c r="K5" s="247" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="152" t="s">
+      <c r="L5" s="255" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -7459,32 +7786,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="91" t="s">
+      <c r="C6" s="194" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="99" t="s">
+      <c r="D6" s="202" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="106" t="s">
+      <c r="E6" s="209" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="113" t="s">
+      <c r="F6" s="216" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="121" t="s">
+      <c r="G6" s="224" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="129" t="s">
+      <c r="H6" s="232" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="13"/>
-      <c r="J6" s="137" t="s">
+      <c r="J6" s="240" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="145" t="s">
+      <c r="K6" s="248" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="153" t="s">
+      <c r="L6" s="256" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -7498,32 +7825,32 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="92" t="s">
+      <c r="C7" s="195" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="100" t="s">
+      <c r="D7" s="203" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="107" t="s">
+      <c r="E7" s="210" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="114" t="s">
+      <c r="F7" s="217" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="122" t="s">
+      <c r="G7" s="225" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="130" t="s">
+      <c r="H7" s="233" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="13"/>
-      <c r="J7" s="138" t="s">
+      <c r="J7" s="241" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="146" t="s">
+      <c r="K7" s="249" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="154" t="s">
+      <c r="L7" s="257" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -7537,30 +7864,30 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="196" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="204" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="22"/>
-      <c r="F8" s="115" t="s">
+      <c r="F8" s="218" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="123" t="s">
+      <c r="G8" s="226" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="131" t="s">
+      <c r="H8" s="234" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="139" t="s">
+      <c r="J8" s="242" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="147" t="s">
+      <c r="K8" s="250" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="155" t="s">
+      <c r="L8" s="258" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -7574,32 +7901,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="197" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="102" t="s">
+      <c r="D9" s="205" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="108" t="s">
+      <c r="E9" s="211" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="116" t="s">
+      <c r="F9" s="219" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="124" t="s">
+      <c r="G9" s="227" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="132" t="s">
+      <c r="H9" s="235" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="140" t="s">
+      <c r="J9" s="243" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="148" t="s">
+      <c r="K9" s="251" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="156" t="s">
+      <c r="L9" s="259" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -7613,32 +7940,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="198" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="103" t="s">
+      <c r="D10" s="206" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="109" t="s">
+      <c r="E10" s="212" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="117" t="s">
+      <c r="F10" s="220" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="125" t="s">
+      <c r="G10" s="228" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="133" t="s">
+      <c r="H10" s="236" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="141" t="s">
+      <c r="J10" s="244" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="149" t="s">
+      <c r="K10" s="252" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="157" t="s">
+      <c r="L10" s="260" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -27128,17 +27455,20 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="261" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="D3" s="13" t="s">
+      <c r="B3" s="262" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" s="263" t="s">
         <v>151</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="264" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="265" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-25 17:05:27]  fixed?"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="159">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1005,7 +1005,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="266">
+  <cellXfs count="374">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1117,6 +1117,330 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -4858,44 +5182,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="158" t="s">
+      <c r="A3" s="266" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="160" t="s">
+      <c r="B3" s="268" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="162" t="s">
+      <c r="C3" s="270" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="164" t="s">
+      <c r="D3" s="272" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="166" t="s">
+      <c r="E3" s="274" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="168" t="s">
+      <c r="G3" s="276" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="159" t="s">
+      <c r="A4" s="267" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="269" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="163" t="s">
+      <c r="C4" s="271" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="165" t="s">
+      <c r="D4" s="273" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="167" t="s">
+      <c r="E4" s="275" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="169" t="s">
+      <c r="G4" s="277" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6052,81 +6376,81 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="170" t="s">
+      <c r="C3" s="278" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="173" t="s">
+      <c r="D3" s="281" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="176" t="s">
+      <c r="E3" s="284" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="179" t="s">
+      <c r="F3" s="287" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="13"/>
-      <c r="H3" s="182" t="s">
+      <c r="H3" s="290" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="185" t="s">
+      <c r="I3" s="293" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="188" t="s">
+      <c r="K3" s="296" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="171" t="s">
+      <c r="C4" s="279" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="174" t="s">
+      <c r="D4" s="282" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="177" t="s">
+      <c r="E4" s="285" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="180" t="s">
+      <c r="F4" s="288" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="13"/>
-      <c r="H4" s="183" t="s">
+      <c r="H4" s="291" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="186" t="s">
+      <c r="I4" s="294" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="189" t="s">
+      <c r="K4" s="297" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="172" t="s">
+      <c r="C5" s="280" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="175" t="s">
+      <c r="D5" s="283" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="178" t="s">
+      <c r="E5" s="286" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="181" t="s">
+      <c r="F5" s="289" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="13"/>
-      <c r="H5" s="184" t="s">
+      <c r="H5" s="292" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="187" t="s">
+      <c r="I5" s="295" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="190" t="s">
+      <c r="K5" s="298" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7671,32 +7995,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="191" t="s">
+      <c r="C3" s="299" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="199" t="s">
+      <c r="D3" s="307" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="207" t="s">
+      <c r="E3" s="315" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="213" t="s">
+      <c r="F3" s="321" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="221" t="s">
+      <c r="G3" s="329" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="229" t="s">
+      <c r="H3" s="337" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="237" t="s">
+      <c r="J3" s="345" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="245" t="s">
+      <c r="K3" s="353" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="253" t="s">
+      <c r="L3" s="361" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -7710,32 +8034,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="192" t="s">
+      <c r="C4" s="300" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="200" t="s">
+      <c r="D4" s="308" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="208" t="s">
+      <c r="E4" s="316" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="214" t="s">
+      <c r="F4" s="322" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="222" t="s">
+      <c r="G4" s="330" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="230" t="s">
+      <c r="H4" s="338" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="238" t="s">
+      <c r="J4" s="346" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="246" t="s">
+      <c r="K4" s="354" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="254" t="s">
+      <c r="L4" s="362" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -7749,30 +8073,30 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="193" t="s">
+      <c r="C5" s="301" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="201" t="s">
+      <c r="D5" s="309" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="215" t="s">
+      <c r="F5" s="323" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="223" t="s">
+      <c r="G5" s="331" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="231" t="s">
+      <c r="H5" s="339" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="239" t="s">
+      <c r="J5" s="347" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="247" t="s">
+      <c r="K5" s="355" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="255" t="s">
+      <c r="L5" s="363" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -7786,32 +8110,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="194" t="s">
+      <c r="C6" s="302" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="202" t="s">
+      <c r="D6" s="310" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="209" t="s">
+      <c r="E6" s="317" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="216" t="s">
+      <c r="F6" s="324" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="224" t="s">
+      <c r="G6" s="332" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="232" t="s">
+      <c r="H6" s="340" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="13"/>
-      <c r="J6" s="240" t="s">
+      <c r="J6" s="348" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="248" t="s">
+      <c r="K6" s="356" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="256" t="s">
+      <c r="L6" s="364" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -7825,32 +8149,32 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="195" t="s">
+      <c r="C7" s="303" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="203" t="s">
+      <c r="D7" s="311" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="210" t="s">
+      <c r="E7" s="318" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="217" t="s">
+      <c r="F7" s="325" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="225" t="s">
+      <c r="G7" s="333" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="233" t="s">
+      <c r="H7" s="341" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="13"/>
-      <c r="J7" s="241" t="s">
+      <c r="J7" s="349" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="249" t="s">
+      <c r="K7" s="357" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="257" t="s">
+      <c r="L7" s="365" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -7864,30 +8188,30 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="196" t="s">
+      <c r="C8" s="304" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="204" t="s">
+      <c r="D8" s="312" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="22"/>
-      <c r="F8" s="218" t="s">
+      <c r="F8" s="326" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="226" t="s">
+      <c r="G8" s="334" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="234" t="s">
+      <c r="H8" s="342" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="242" t="s">
+      <c r="J8" s="350" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="250" t="s">
+      <c r="K8" s="358" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="258" t="s">
+      <c r="L8" s="366" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -7901,32 +8225,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="197" t="s">
+      <c r="C9" s="305" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="205" t="s">
+      <c r="D9" s="313" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="211" t="s">
+      <c r="E9" s="319" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="219" t="s">
+      <c r="F9" s="327" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="227" t="s">
+      <c r="G9" s="335" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="235" t="s">
+      <c r="H9" s="343" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="243" t="s">
+      <c r="J9" s="351" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="251" t="s">
+      <c r="K9" s="359" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="259" t="s">
+      <c r="L9" s="367" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -7940,32 +8264,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="198" t="s">
+      <c r="C10" s="306" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="206" t="s">
+      <c r="D10" s="314" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="212" t="s">
+      <c r="E10" s="320" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="220" t="s">
+      <c r="F10" s="328" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="228" t="s">
+      <c r="G10" s="336" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="236" t="s">
+      <c r="H10" s="344" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="244" t="s">
+      <c r="J10" s="352" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="252" t="s">
+      <c r="K10" s="360" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="260" t="s">
+      <c r="L10" s="368" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -27455,20 +27779,20 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="261" t="s">
+      <c r="A3" s="369" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="262" t="s">
+      <c r="B3" s="370" t="s">
         <v>158</v>
       </c>
       <c r="C3"/>
-      <c r="D3" s="263" t="s">
+      <c r="D3" s="371" t="s">
         <v>151</v>
       </c>
-      <c r="E3" s="264" t="s">
+      <c r="E3" s="372" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="265" t="s">
+      <c r="F3" s="373" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-26 09:30:37] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -704,6 +704,18 @@
   <si>
     <t>For best experience, always edit in Google Sheets.</t>
   </si>
+  <si>
+    <t>ColourfulSolns_Pre/Post Assessment (STUDENT)</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1hhCN2R-J_6JLJwBuNOqzuP2vZ5MXhPIPyDMgerZKNrw/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1hhCN2R-J_6JLJwBuNOqzuP2vZ5MXhPIPyDMgerZKNrw/export?format=pdf</t>
+  </si>
+  <si>
+    <t>1hhCN2R-J_6JLJwBuNOqzuP2vZ5MXhPIPyDMgerZKNrw</t>
+  </si>
 </sst>
 </file>
 
@@ -1002,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="270">
+  <cellXfs count="381">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1115,6 +1127,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -4865,44 +5210,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="163" t="s">
+      <c r="A3" s="270" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="165" t="s">
+      <c r="B3" s="272" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="167" t="s">
+      <c r="C3" s="274" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="169" t="s">
+      <c r="D3" s="276" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="171" t="s">
+      <c r="E3" s="278" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="173" t="s">
+      <c r="G3" s="280" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="164" t="s">
+      <c r="A4" s="271" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="166" t="s">
+      <c r="B4" s="273" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="168" t="s">
+      <c r="C4" s="275" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="170" t="s">
+      <c r="D4" s="277" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="172" t="s">
+      <c r="E4" s="279" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="174" t="s">
+      <c r="G4" s="281" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6059,81 +6404,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="175" t="s">
+      <c r="C3" s="282" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="178" t="s">
+      <c r="D3" s="285" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="181" t="s">
+      <c r="E3" s="288" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="184" t="s">
+      <c r="F3" s="291" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="187" t="s">
+      <c r="H3" s="294" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="190" t="s">
+      <c r="I3" s="297" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="193" t="s">
+      <c r="K3" s="300" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="176" t="s">
+      <c r="C4" s="283" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="179" t="s">
+      <c r="D4" s="286" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="182" t="s">
+      <c r="E4" s="289" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="185" t="s">
+      <c r="F4" s="292" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="188" t="s">
+      <c r="H4" s="295" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="191" t="s">
+      <c r="I4" s="298" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="194" t="s">
+      <c r="K4" s="301" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="177" t="s">
+      <c r="C5" s="284" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="180" t="s">
+      <c r="D5" s="287" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="183" t="s">
+      <c r="E5" s="290" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="186" t="s">
+      <c r="F5" s="293" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="189" t="s">
+      <c r="H5" s="296" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="192" t="s">
+      <c r="I5" s="299" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="195" t="s">
+      <c r="K5" s="302" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7678,32 +8023,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="196" t="s">
+      <c r="C3" s="303" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="204" t="s">
+      <c r="D3" s="311" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="212" t="s">
+      <c r="E3" s="319" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="218" t="s">
+      <c r="F3" s="325" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="226" t="s">
+      <c r="G3" s="333" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="234" t="s">
+      <c r="H3" s="341" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="242" t="s">
+      <c r="J3" s="349" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="250" t="s">
+      <c r="K3" s="357" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="258" t="s">
+      <c r="L3" s="365" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -7717,32 +8062,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="197" t="s">
+      <c r="C4" s="304" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="205" t="s">
+      <c r="D4" s="312" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="213" t="s">
+      <c r="E4" s="320" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="219" t="s">
+      <c r="F4" s="326" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="227" t="s">
+      <c r="G4" s="334" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="235" t="s">
+      <c r="H4" s="342" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="243" t="s">
+      <c r="J4" s="350" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="251" t="s">
+      <c r="K4" s="358" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="259" t="s">
+      <c r="L4" s="366" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -7756,30 +8101,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="198" t="s">
+      <c r="C5" s="305" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="206" t="s">
+      <c r="D5" s="313" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="220" t="s">
+      <c r="F5" s="327" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="228" t="s">
+      <c r="G5" s="335" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="236" t="s">
+      <c r="H5" s="343" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="244" t="s">
+      <c r="J5" s="351" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="252" t="s">
+      <c r="K5" s="359" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="260" t="s">
+      <c r="L5" s="367" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -7793,32 +8138,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="199" t="s">
+      <c r="C6" s="306" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="207" t="s">
+      <c r="D6" s="314" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="214" t="s">
+      <c r="E6" s="321" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="221" t="s">
+      <c r="F6" s="328" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="229" t="s">
+      <c r="G6" s="336" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="237" t="s">
+      <c r="H6" s="344" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="245" t="s">
+      <c r="J6" s="352" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="253" t="s">
+      <c r="K6" s="360" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="261" t="s">
+      <c r="L6" s="368" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -7832,32 +8177,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="200" t="s">
+      <c r="C7" s="307" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="208" t="s">
+      <c r="D7" s="315" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="215" t="s">
+      <c r="E7" s="322" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="222" t="s">
+      <c r="F7" s="329" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="230" t="s">
+      <c r="G7" s="337" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="238" t="s">
+      <c r="H7" s="345" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="246" t="s">
+      <c r="J7" s="353" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="254" t="s">
+      <c r="K7" s="361" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="262" t="s">
+      <c r="L7" s="369" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -7871,30 +8216,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="201" t="s">
+      <c r="C8" s="308" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="209" t="s">
+      <c r="D8" s="316" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="223" t="s">
+      <c r="F8" s="330" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="231" t="s">
+      <c r="G8" s="338" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="239" t="s">
+      <c r="H8" s="346" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="247" t="s">
+      <c r="J8" s="354" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="255" t="s">
+      <c r="K8" s="362" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="263" t="s">
+      <c r="L8" s="370" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -7908,32 +8253,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="202" t="s">
+      <c r="C9" s="309" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="210" t="s">
+      <c r="D9" s="317" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="216" t="s">
+      <c r="E9" s="323" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="224" t="s">
+      <c r="F9" s="331" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="232" t="s">
+      <c r="G9" s="339" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="240" t="s">
+      <c r="H9" s="347" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="248" t="s">
+      <c r="J9" s="355" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="256" t="s">
+      <c r="K9" s="363" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="264" t="s">
+      <c r="L9" s="371" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -7947,32 +8292,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="203" t="s">
+      <c r="C10" s="310" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="211" t="s">
+      <c r="D10" s="318" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="217" t="s">
+      <c r="E10" s="324" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="225" t="s">
+      <c r="F10" s="332" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="233" t="s">
+      <c r="G10" s="340" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="241" t="s">
+      <c r="H10" s="348" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="249" t="s">
+      <c r="J10" s="356" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="257" t="s">
+      <c r="K10" s="364" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="265" t="s">
+      <c r="L10" s="372" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -27426,7 +27771,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -27462,18 +27807,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="266" t="s">
-        <v>150</v>
+      <c r="A3" s="373" t="s">
+        <v>158</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="267" t="s">
+      <c r="D3" s="375" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="377" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="379" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="374">
+        <v>150</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4" t="s" s="376">
         <v>151</v>
       </c>
-      <c r="E3" s="268" t="s">
+      <c r="E4" t="s" s="378">
         <v>152</v>
       </c>
-      <c r="F3" s="269" t="s">
+      <c r="F4" t="s" s="380">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-31 12:03:49]  "Added standards, uniqueID, updated version""
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="381">
+  <cellXfs count="1047">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1127,6 +1127,2004 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -5210,44 +7208,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="270" t="s">
+      <c r="A3" s="936" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="272" t="s">
+      <c r="B3" s="938" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="274" t="s">
+      <c r="C3" s="940" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="276" t="s">
+      <c r="D3" s="942" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="278" t="s">
+      <c r="E3" s="944" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="280" t="s">
+      <c r="G3" s="946" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="271" t="s">
+      <c r="A4" s="937" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="273" t="s">
+      <c r="B4" s="939" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="275" t="s">
+      <c r="C4" s="941" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="277" t="s">
+      <c r="D4" s="943" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="279" t="s">
+      <c r="E4" s="945" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="281" t="s">
+      <c r="G4" s="947" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6404,81 +8402,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="282" t="s">
+      <c r="C3" s="948" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="285" t="s">
+      <c r="D3" s="951" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="288" t="s">
+      <c r="E3" s="954" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="291" t="s">
+      <c r="F3" s="957" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="294" t="s">
+      <c r="H3" s="960" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="297" t="s">
+      <c r="I3" s="963" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="300" t="s">
+      <c r="K3" s="966" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="283" t="s">
+      <c r="C4" s="949" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="286" t="s">
+      <c r="D4" s="952" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="289" t="s">
+      <c r="E4" s="955" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="292" t="s">
+      <c r="F4" s="958" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="295" t="s">
+      <c r="H4" s="961" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="298" t="s">
+      <c r="I4" s="964" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="301" t="s">
+      <c r="K4" s="967" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="284" t="s">
+      <c r="C5" s="950" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="287" t="s">
+      <c r="D5" s="953" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="290" t="s">
+      <c r="E5" s="956" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="293" t="s">
+      <c r="F5" s="959" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="296" t="s">
+      <c r="H5" s="962" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="299" t="s">
+      <c r="I5" s="965" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="302" t="s">
+      <c r="K5" s="968" t="s">
         <v>62</v>
       </c>
     </row>
@@ -8023,32 +10021,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="303" t="s">
+      <c r="C3" s="969" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="311" t="s">
+      <c r="D3" s="977" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="319" t="s">
+      <c r="E3" s="985" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="325" t="s">
+      <c r="F3" s="991" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="333" t="s">
+      <c r="G3" s="999" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="341" t="s">
+      <c r="H3" s="1007" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="349" t="s">
+      <c r="J3" s="1015" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="357" t="s">
+      <c r="K3" s="1023" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="365" t="s">
+      <c r="L3" s="1031" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -8062,32 +10060,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="304" t="s">
+      <c r="C4" s="970" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="312" t="s">
+      <c r="D4" s="978" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="320" t="s">
+      <c r="E4" s="986" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="326" t="s">
+      <c r="F4" s="992" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="334" t="s">
+      <c r="G4" s="1000" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="342" t="s">
+      <c r="H4" s="1008" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="350" t="s">
+      <c r="J4" s="1016" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="358" t="s">
+      <c r="K4" s="1024" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="366" t="s">
+      <c r="L4" s="1032" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -8101,30 +10099,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="305" t="s">
+      <c r="C5" s="971" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="313" t="s">
+      <c r="D5" s="979" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="327" t="s">
+      <c r="F5" s="993" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="335" t="s">
+      <c r="G5" s="1001" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="343" t="s">
+      <c r="H5" s="1009" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="351" t="s">
+      <c r="J5" s="1017" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="359" t="s">
+      <c r="K5" s="1025" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="367" t="s">
+      <c r="L5" s="1033" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -8138,32 +10136,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="306" t="s">
+      <c r="C6" s="972" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="314" t="s">
+      <c r="D6" s="980" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="321" t="s">
+      <c r="E6" s="987" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="328" t="s">
+      <c r="F6" s="994" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="336" t="s">
+      <c r="G6" s="1002" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="344" t="s">
+      <c r="H6" s="1010" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="352" t="s">
+      <c r="J6" s="1018" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="360" t="s">
+      <c r="K6" s="1026" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="368" t="s">
+      <c r="L6" s="1034" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -8177,32 +10175,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="307" t="s">
+      <c r="C7" s="973" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="315" t="s">
+      <c r="D7" s="981" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="322" t="s">
+      <c r="E7" s="988" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="329" t="s">
+      <c r="F7" s="995" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="337" t="s">
+      <c r="G7" s="1003" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="345" t="s">
+      <c r="H7" s="1011" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="353" t="s">
+      <c r="J7" s="1019" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="361" t="s">
+      <c r="K7" s="1027" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="369" t="s">
+      <c r="L7" s="1035" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -8216,30 +10214,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="308" t="s">
+      <c r="C8" s="974" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="316" t="s">
+      <c r="D8" s="982" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="330" t="s">
+      <c r="F8" s="996" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="338" t="s">
+      <c r="G8" s="1004" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="346" t="s">
+      <c r="H8" s="1012" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="354" t="s">
+      <c r="J8" s="1020" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="362" t="s">
+      <c r="K8" s="1028" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="370" t="s">
+      <c r="L8" s="1036" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -8253,32 +10251,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="309" t="s">
+      <c r="C9" s="975" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="317" t="s">
+      <c r="D9" s="983" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="323" t="s">
+      <c r="E9" s="989" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="331" t="s">
+      <c r="F9" s="997" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="339" t="s">
+      <c r="G9" s="1005" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="347" t="s">
+      <c r="H9" s="1013" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="355" t="s">
+      <c r="J9" s="1021" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="363" t="s">
+      <c r="K9" s="1029" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="371" t="s">
+      <c r="L9" s="1037" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -8292,32 +10290,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="310" t="s">
+      <c r="C10" s="976" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="318" t="s">
+      <c r="D10" s="984" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="324" t="s">
+      <c r="E10" s="990" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="332" t="s">
+      <c r="F10" s="998" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="340" t="s">
+      <c r="G10" s="1006" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="348" t="s">
+      <c r="H10" s="1014" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="356" t="s">
+      <c r="J10" s="1022" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="364" t="s">
+      <c r="K10" s="1030" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="372" t="s">
+      <c r="L10" s="1038" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -27807,34 +29805,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="373" t="s">
+      <c r="A3" s="1039" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="375" t="s">
+      <c r="D3" s="1041" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="377" t="s">
+      <c r="E3" s="1043" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="379" t="s">
+      <c r="F3" s="1045" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="374">
+      <c r="A4" t="s" s="1040">
         <v>150</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="376">
+      <c r="D4" t="s" s="1042">
         <v>151</v>
       </c>
-      <c r="E4" t="s" s="378">
+      <c r="E4" t="s" s="1044">
         <v>152</v>
       </c>
-      <c r="F4" t="s" s="380">
+      <c r="F4" t="s" s="1046">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-31 14:40:42] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1342" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1047">
+  <cellXfs count="1380">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1127,6 +1127,1005 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -7208,44 +8207,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="936" t="s">
+      <c r="A3" s="1269" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="938" t="s">
+      <c r="B3" s="1271" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="940" t="s">
+      <c r="C3" s="1273" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="942" t="s">
+      <c r="D3" s="1275" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="944" t="s">
+      <c r="E3" s="1277" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="946" t="s">
+      <c r="G3" s="1279" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="937" t="s">
+      <c r="A4" s="1270" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="939" t="s">
+      <c r="B4" s="1272" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="941" t="s">
+      <c r="C4" s="1274" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="943" t="s">
+      <c r="D4" s="1276" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="945" t="s">
+      <c r="E4" s="1278" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="947" t="s">
+      <c r="G4" s="1280" t="s">
         <v>37</v>
       </c>
     </row>
@@ -8402,81 +9401,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="948" t="s">
+      <c r="C3" s="1281" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="951" t="s">
+      <c r="D3" s="1284" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="954" t="s">
+      <c r="E3" s="1287" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="957" t="s">
+      <c r="F3" s="1290" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="960" t="s">
+      <c r="H3" s="1293" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="963" t="s">
+      <c r="I3" s="1296" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="966" t="s">
+      <c r="K3" s="1299" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="949" t="s">
+      <c r="C4" s="1282" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="952" t="s">
+      <c r="D4" s="1285" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="955" t="s">
+      <c r="E4" s="1288" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="958" t="s">
+      <c r="F4" s="1291" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="961" t="s">
+      <c r="H4" s="1294" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="964" t="s">
+      <c r="I4" s="1297" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="967" t="s">
+      <c r="K4" s="1300" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="950" t="s">
+      <c r="C5" s="1283" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="953" t="s">
+      <c r="D5" s="1286" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="956" t="s">
+      <c r="E5" s="1289" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="959" t="s">
+      <c r="F5" s="1292" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="962" t="s">
+      <c r="H5" s="1295" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="965" t="s">
+      <c r="I5" s="1298" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="968" t="s">
+      <c r="K5" s="1301" t="s">
         <v>62</v>
       </c>
     </row>
@@ -10021,32 +11020,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="969" t="s">
+      <c r="C3" s="1302" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="977" t="s">
+      <c r="D3" s="1310" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="985" t="s">
+      <c r="E3" s="1318" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="991" t="s">
+      <c r="F3" s="1324" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="999" t="s">
+      <c r="G3" s="1332" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="1007" t="s">
+      <c r="H3" s="1340" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="1015" t="s">
+      <c r="J3" s="1348" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="1023" t="s">
+      <c r="K3" s="1356" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="1031" t="s">
+      <c r="L3" s="1364" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -10060,32 +11059,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="970" t="s">
+      <c r="C4" s="1303" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="978" t="s">
+      <c r="D4" s="1311" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="986" t="s">
+      <c r="E4" s="1319" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="992" t="s">
+      <c r="F4" s="1325" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="1000" t="s">
+      <c r="G4" s="1333" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="1008" t="s">
+      <c r="H4" s="1341" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="1016" t="s">
+      <c r="J4" s="1349" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="1024" t="s">
+      <c r="K4" s="1357" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="1032" t="s">
+      <c r="L4" s="1365" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -10099,30 +11098,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="971" t="s">
+      <c r="C5" s="1304" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="979" t="s">
+      <c r="D5" s="1312" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="993" t="s">
+      <c r="F5" s="1326" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="1001" t="s">
+      <c r="G5" s="1334" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="1009" t="s">
+      <c r="H5" s="1342" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="1017" t="s">
+      <c r="J5" s="1350" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="1025" t="s">
+      <c r="K5" s="1358" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="1033" t="s">
+      <c r="L5" s="1366" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -10136,32 +11135,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="972" t="s">
+      <c r="C6" s="1305" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="980" t="s">
+      <c r="D6" s="1313" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="987" t="s">
+      <c r="E6" s="1320" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="994" t="s">
+      <c r="F6" s="1327" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="1002" t="s">
+      <c r="G6" s="1335" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="1010" t="s">
+      <c r="H6" s="1343" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="1018" t="s">
+      <c r="J6" s="1351" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="1026" t="s">
+      <c r="K6" s="1359" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="1034" t="s">
+      <c r="L6" s="1367" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -10175,32 +11174,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="973" t="s">
+      <c r="C7" s="1306" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="981" t="s">
+      <c r="D7" s="1314" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="988" t="s">
+      <c r="E7" s="1321" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="995" t="s">
+      <c r="F7" s="1328" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="1003" t="s">
+      <c r="G7" s="1336" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="1011" t="s">
+      <c r="H7" s="1344" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="1019" t="s">
+      <c r="J7" s="1352" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="1027" t="s">
+      <c r="K7" s="1360" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="1035" t="s">
+      <c r="L7" s="1368" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -10214,30 +11213,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="974" t="s">
+      <c r="C8" s="1307" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="982" t="s">
+      <c r="D8" s="1315" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="996" t="s">
+      <c r="F8" s="1329" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="1004" t="s">
+      <c r="G8" s="1337" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="1012" t="s">
+      <c r="H8" s="1345" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="1020" t="s">
+      <c r="J8" s="1353" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="1028" t="s">
+      <c r="K8" s="1361" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="1036" t="s">
+      <c r="L8" s="1369" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -10251,32 +11250,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="975" t="s">
+      <c r="C9" s="1308" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="983" t="s">
+      <c r="D9" s="1316" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="989" t="s">
+      <c r="E9" s="1322" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="997" t="s">
+      <c r="F9" s="1330" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="1005" t="s">
+      <c r="G9" s="1338" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="1013" t="s">
+      <c r="H9" s="1346" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="1021" t="s">
+      <c r="J9" s="1354" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="1029" t="s">
+      <c r="K9" s="1362" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="1037" t="s">
+      <c r="L9" s="1370" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -10290,32 +11289,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="976" t="s">
+      <c r="C10" s="1309" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="984" t="s">
+      <c r="D10" s="1317" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="990" t="s">
+      <c r="E10" s="1323" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="998" t="s">
+      <c r="F10" s="1331" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1006" t="s">
+      <c r="G10" s="1339" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1014" t="s">
+      <c r="H10" s="1347" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="1022" t="s">
+      <c r="J10" s="1355" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1030" t="s">
+      <c r="K10" s="1363" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="1038" t="s">
+      <c r="L10" s="1371" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -29805,34 +30804,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1039" t="s">
+      <c r="A3" s="1372" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="1041" t="s">
+      <c r="D3" s="1374" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="1043" t="s">
+      <c r="E3" s="1376" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="1045" t="s">
+      <c r="F3" s="1378" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="1040">
+      <c r="A4" t="s" s="1373">
         <v>150</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="1042">
+      <c r="D4" t="s" s="1375">
         <v>151</v>
       </c>
-      <c r="E4" t="s" s="1044">
+      <c r="E4" t="s" s="1377">
         <v>152</v>
       </c>
-      <c r="F4" t="s" s="1046">
+      <c r="F4" t="s" s="1379">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-31 15:07:47]  Hopefully got rid of broken standards section"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1380">
+  <cellXfs count="1491">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1127,6 +1127,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -8207,44 +8540,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1269" t="s">
+      <c r="A3" s="1380" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1271" t="s">
+      <c r="B3" s="1382" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1273" t="s">
+      <c r="C3" s="1384" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1275" t="s">
+      <c r="D3" s="1386" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1277" t="s">
+      <c r="E3" s="1388" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="1279" t="s">
+      <c r="G3" s="1390" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1270" t="s">
+      <c r="A4" s="1381" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1272" t="s">
+      <c r="B4" s="1383" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1274" t="s">
+      <c r="C4" s="1385" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1276" t="s">
+      <c r="D4" s="1387" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1278" t="s">
+      <c r="E4" s="1389" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="1280" t="s">
+      <c r="G4" s="1391" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9401,81 +9734,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1281" t="s">
+      <c r="C3" s="1392" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1284" t="s">
+      <c r="D3" s="1395" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1287" t="s">
+      <c r="E3" s="1398" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="1290" t="s">
+      <c r="F3" s="1401" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="1293" t="s">
+      <c r="H3" s="1404" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="1296" t="s">
+      <c r="I3" s="1407" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="1299" t="s">
+      <c r="K3" s="1410" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1282" t="s">
+      <c r="C4" s="1393" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1285" t="s">
+      <c r="D4" s="1396" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="1288" t="s">
+      <c r="E4" s="1399" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="1291" t="s">
+      <c r="F4" s="1402" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="1294" t="s">
+      <c r="H4" s="1405" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="1297" t="s">
+      <c r="I4" s="1408" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1300" t="s">
+      <c r="K4" s="1411" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1283" t="s">
+      <c r="C5" s="1394" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1286" t="s">
+      <c r="D5" s="1397" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="1289" t="s">
+      <c r="E5" s="1400" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="1292" t="s">
+      <c r="F5" s="1403" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="1295" t="s">
+      <c r="H5" s="1406" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="1298" t="s">
+      <c r="I5" s="1409" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1301" t="s">
+      <c r="K5" s="1412" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11020,32 +11353,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1302" t="s">
+      <c r="C3" s="1413" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1310" t="s">
+      <c r="D3" s="1421" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1318" t="s">
+      <c r="E3" s="1429" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="1324" t="s">
+      <c r="F3" s="1435" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="1332" t="s">
+      <c r="G3" s="1443" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="1340" t="s">
+      <c r="H3" s="1451" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="1348" t="s">
+      <c r="J3" s="1459" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="1356" t="s">
+      <c r="K3" s="1467" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="1364" t="s">
+      <c r="L3" s="1475" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -11059,32 +11392,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1303" t="s">
+      <c r="C4" s="1414" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1311" t="s">
+      <c r="D4" s="1422" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="1319" t="s">
+      <c r="E4" s="1430" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="1325" t="s">
+      <c r="F4" s="1436" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="1333" t="s">
+      <c r="G4" s="1444" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="1341" t="s">
+      <c r="H4" s="1452" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="1349" t="s">
+      <c r="J4" s="1460" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="1357" t="s">
+      <c r="K4" s="1468" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="1365" t="s">
+      <c r="L4" s="1476" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -11098,30 +11431,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1304" t="s">
+      <c r="C5" s="1415" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1312" t="s">
+      <c r="D5" s="1423" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="1326" t="s">
+      <c r="F5" s="1437" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="1334" t="s">
+      <c r="G5" s="1445" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="1342" t="s">
+      <c r="H5" s="1453" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="1350" t="s">
+      <c r="J5" s="1461" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="1358" t="s">
+      <c r="K5" s="1469" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="1366" t="s">
+      <c r="L5" s="1477" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -11135,32 +11468,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="1305" t="s">
+      <c r="C6" s="1416" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1313" t="s">
+      <c r="D6" s="1424" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="1320" t="s">
+      <c r="E6" s="1431" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="1327" t="s">
+      <c r="F6" s="1438" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="1335" t="s">
+      <c r="G6" s="1446" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="1343" t="s">
+      <c r="H6" s="1454" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="1351" t="s">
+      <c r="J6" s="1462" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="1359" t="s">
+      <c r="K6" s="1470" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="1367" t="s">
+      <c r="L6" s="1478" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -11174,32 +11507,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="1306" t="s">
+      <c r="C7" s="1417" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1314" t="s">
+      <c r="D7" s="1425" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1321" t="s">
+      <c r="E7" s="1432" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="1328" t="s">
+      <c r="F7" s="1439" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="1336" t="s">
+      <c r="G7" s="1447" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="1344" t="s">
+      <c r="H7" s="1455" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="1352" t="s">
+      <c r="J7" s="1463" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="1360" t="s">
+      <c r="K7" s="1471" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="1368" t="s">
+      <c r="L7" s="1479" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -11213,30 +11546,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="1307" t="s">
+      <c r="C8" s="1418" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1315" t="s">
+      <c r="D8" s="1426" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="1329" t="s">
+      <c r="F8" s="1440" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="1337" t="s">
+      <c r="G8" s="1448" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="1345" t="s">
+      <c r="H8" s="1456" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="1353" t="s">
+      <c r="J8" s="1464" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="1361" t="s">
+      <c r="K8" s="1472" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="1369" t="s">
+      <c r="L8" s="1480" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -11250,32 +11583,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="1308" t="s">
+      <c r="C9" s="1419" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1316" t="s">
+      <c r="D9" s="1427" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="1322" t="s">
+      <c r="E9" s="1433" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="1330" t="s">
+      <c r="F9" s="1441" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="1338" t="s">
+      <c r="G9" s="1449" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="1346" t="s">
+      <c r="H9" s="1457" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="1354" t="s">
+      <c r="J9" s="1465" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="1362" t="s">
+      <c r="K9" s="1473" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="1370" t="s">
+      <c r="L9" s="1481" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -11289,32 +11622,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="1309" t="s">
+      <c r="C10" s="1420" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1317" t="s">
+      <c r="D10" s="1428" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="1323" t="s">
+      <c r="E10" s="1434" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="1331" t="s">
+      <c r="F10" s="1442" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1339" t="s">
+      <c r="G10" s="1450" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1347" t="s">
+      <c r="H10" s="1458" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="1355" t="s">
+      <c r="J10" s="1466" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1363" t="s">
+      <c r="K10" s="1474" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="1371" t="s">
+      <c r="L10" s="1482" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -30804,34 +31137,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1372" t="s">
+      <c r="A3" s="1483" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="1374" t="s">
+      <c r="D3" s="1485" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="1376" t="s">
+      <c r="E3" s="1487" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="1378" t="s">
+      <c r="F3" s="1489" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="1373">
+      <c r="A4" t="s" s="1484">
         <v>150</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="1375">
+      <c r="D4" t="s" s="1486">
         <v>151</v>
       </c>
-      <c r="E4" t="s" s="1377">
+      <c r="E4" t="s" s="1488">
         <v>152</v>
       </c>
-      <c r="F4" t="s" s="1379">
+      <c r="F4" t="s" s="1490">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-31 16:16:24] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1491">
+  <cellXfs count="1602">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1127,6 +1127,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -8540,44 +8873,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1380" t="s">
+      <c r="A3" s="1491" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1382" t="s">
+      <c r="B3" s="1493" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1384" t="s">
+      <c r="C3" s="1495" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1386" t="s">
+      <c r="D3" s="1497" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1388" t="s">
+      <c r="E3" s="1499" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="1390" t="s">
+      <c r="G3" s="1501" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1381" t="s">
+      <c r="A4" s="1492" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1383" t="s">
+      <c r="B4" s="1494" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1385" t="s">
+      <c r="C4" s="1496" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1387" t="s">
+      <c r="D4" s="1498" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1389" t="s">
+      <c r="E4" s="1500" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="1391" t="s">
+      <c r="G4" s="1502" t="s">
         <v>37</v>
       </c>
     </row>
@@ -9734,81 +10067,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1392" t="s">
+      <c r="C3" s="1503" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1395" t="s">
+      <c r="D3" s="1506" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1398" t="s">
+      <c r="E3" s="1509" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="1401" t="s">
+      <c r="F3" s="1512" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="1404" t="s">
+      <c r="H3" s="1515" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="1407" t="s">
+      <c r="I3" s="1518" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="1410" t="s">
+      <c r="K3" s="1521" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1393" t="s">
+      <c r="C4" s="1504" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1396" t="s">
+      <c r="D4" s="1507" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="1399" t="s">
+      <c r="E4" s="1510" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="1402" t="s">
+      <c r="F4" s="1513" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="1405" t="s">
+      <c r="H4" s="1516" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="1408" t="s">
+      <c r="I4" s="1519" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1411" t="s">
+      <c r="K4" s="1522" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1394" t="s">
+      <c r="C5" s="1505" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1397" t="s">
+      <c r="D5" s="1508" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="1400" t="s">
+      <c r="E5" s="1511" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="1403" t="s">
+      <c r="F5" s="1514" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="1406" t="s">
+      <c r="H5" s="1517" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="1409" t="s">
+      <c r="I5" s="1520" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1412" t="s">
+      <c r="K5" s="1523" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11353,32 +11686,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1413" t="s">
+      <c r="C3" s="1524" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1421" t="s">
+      <c r="D3" s="1532" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1429" t="s">
+      <c r="E3" s="1540" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="1435" t="s">
+      <c r="F3" s="1546" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="1443" t="s">
+      <c r="G3" s="1554" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="1451" t="s">
+      <c r="H3" s="1562" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="1459" t="s">
+      <c r="J3" s="1570" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="1467" t="s">
+      <c r="K3" s="1578" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="1475" t="s">
+      <c r="L3" s="1586" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -11392,32 +11725,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1414" t="s">
+      <c r="C4" s="1525" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1422" t="s">
+      <c r="D4" s="1533" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="1430" t="s">
+      <c r="E4" s="1541" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="1436" t="s">
+      <c r="F4" s="1547" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="1444" t="s">
+      <c r="G4" s="1555" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="1452" t="s">
+      <c r="H4" s="1563" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="1460" t="s">
+      <c r="J4" s="1571" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="1468" t="s">
+      <c r="K4" s="1579" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="1476" t="s">
+      <c r="L4" s="1587" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -11431,30 +11764,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1415" t="s">
+      <c r="C5" s="1526" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1423" t="s">
+      <c r="D5" s="1534" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="1437" t="s">
+      <c r="F5" s="1548" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="1445" t="s">
+      <c r="G5" s="1556" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="1453" t="s">
+      <c r="H5" s="1564" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="1461" t="s">
+      <c r="J5" s="1572" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="1469" t="s">
+      <c r="K5" s="1580" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="1477" t="s">
+      <c r="L5" s="1588" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -11468,32 +11801,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="1416" t="s">
+      <c r="C6" s="1527" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1424" t="s">
+      <c r="D6" s="1535" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="1431" t="s">
+      <c r="E6" s="1542" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="1438" t="s">
+      <c r="F6" s="1549" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="1446" t="s">
+      <c r="G6" s="1557" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="1454" t="s">
+      <c r="H6" s="1565" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="1462" t="s">
+      <c r="J6" s="1573" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="1470" t="s">
+      <c r="K6" s="1581" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="1478" t="s">
+      <c r="L6" s="1589" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -11507,32 +11840,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="1417" t="s">
+      <c r="C7" s="1528" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1425" t="s">
+      <c r="D7" s="1536" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1432" t="s">
+      <c r="E7" s="1543" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="1439" t="s">
+      <c r="F7" s="1550" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="1447" t="s">
+      <c r="G7" s="1558" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="1455" t="s">
+      <c r="H7" s="1566" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="1463" t="s">
+      <c r="J7" s="1574" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="1471" t="s">
+      <c r="K7" s="1582" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="1479" t="s">
+      <c r="L7" s="1590" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -11546,30 +11879,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="1418" t="s">
+      <c r="C8" s="1529" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1426" t="s">
+      <c r="D8" s="1537" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="1440" t="s">
+      <c r="F8" s="1551" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="1448" t="s">
+      <c r="G8" s="1559" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="1456" t="s">
+      <c r="H8" s="1567" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="1464" t="s">
+      <c r="J8" s="1575" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="1472" t="s">
+      <c r="K8" s="1583" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="1480" t="s">
+      <c r="L8" s="1591" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -11583,32 +11916,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="1419" t="s">
+      <c r="C9" s="1530" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1427" t="s">
+      <c r="D9" s="1538" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="1433" t="s">
+      <c r="E9" s="1544" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="1441" t="s">
+      <c r="F9" s="1552" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="1449" t="s">
+      <c r="G9" s="1560" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="1457" t="s">
+      <c r="H9" s="1568" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="1465" t="s">
+      <c r="J9" s="1576" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="1473" t="s">
+      <c r="K9" s="1584" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="1481" t="s">
+      <c r="L9" s="1592" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -11622,32 +11955,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="1420" t="s">
+      <c r="C10" s="1531" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1428" t="s">
+      <c r="D10" s="1539" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="1434" t="s">
+      <c r="E10" s="1545" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="1442" t="s">
+      <c r="F10" s="1553" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1450" t="s">
+      <c r="G10" s="1561" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1458" t="s">
+      <c r="H10" s="1569" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="1466" t="s">
+      <c r="J10" s="1577" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1474" t="s">
+      <c r="K10" s="1585" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="1482" t="s">
+      <c r="L10" s="1593" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -31137,34 +31470,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1483" t="s">
+      <c r="A3" s="1594" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="1485" t="s">
+      <c r="D3" s="1596" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="1487" t="s">
+      <c r="E3" s="1598" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="1489" t="s">
+      <c r="F3" s="1600" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="1484">
+      <c r="A4" t="s" s="1595">
         <v>150</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="1486">
+      <c r="D4" t="s" s="1597">
         <v>151</v>
       </c>
-      <c r="E4" t="s" s="1488">
+      <c r="E4" t="s" s="1599">
         <v>152</v>
       </c>
-      <c r="F4" t="s" s="1490">
+      <c r="F4" t="s" s="1601">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-31 21:27:52]  hopefully all set for launch"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1602">
+  <cellXfs count="1824">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1127,6 +1127,672 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -8873,44 +9539,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1491" t="s">
+      <c r="A3" s="1713" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1493" t="s">
+      <c r="B3" s="1715" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1495" t="s">
+      <c r="C3" s="1717" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1497" t="s">
+      <c r="D3" s="1719" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1499" t="s">
+      <c r="E3" s="1721" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="1501" t="s">
+      <c r="G3" s="1723" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1492" t="s">
+      <c r="A4" s="1714" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1494" t="s">
+      <c r="B4" s="1716" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1496" t="s">
+      <c r="C4" s="1718" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1498" t="s">
+      <c r="D4" s="1720" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1500" t="s">
+      <c r="E4" s="1722" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="1502" t="s">
+      <c r="G4" s="1724" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10067,81 +10733,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1503" t="s">
+      <c r="C3" s="1725" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1506" t="s">
+      <c r="D3" s="1728" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1509" t="s">
+      <c r="E3" s="1731" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="1512" t="s">
+      <c r="F3" s="1734" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="1515" t="s">
+      <c r="H3" s="1737" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="1518" t="s">
+      <c r="I3" s="1740" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="1521" t="s">
+      <c r="K3" s="1743" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1504" t="s">
+      <c r="C4" s="1726" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1507" t="s">
+      <c r="D4" s="1729" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="1510" t="s">
+      <c r="E4" s="1732" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="1513" t="s">
+      <c r="F4" s="1735" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="1516" t="s">
+      <c r="H4" s="1738" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="1519" t="s">
+      <c r="I4" s="1741" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1522" t="s">
+      <c r="K4" s="1744" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1505" t="s">
+      <c r="C5" s="1727" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1508" t="s">
+      <c r="D5" s="1730" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="1511" t="s">
+      <c r="E5" s="1733" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="1514" t="s">
+      <c r="F5" s="1736" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="1517" t="s">
+      <c r="H5" s="1739" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="1520" t="s">
+      <c r="I5" s="1742" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1523" t="s">
+      <c r="K5" s="1745" t="s">
         <v>62</v>
       </c>
     </row>
@@ -11686,32 +12352,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1524" t="s">
+      <c r="C3" s="1746" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1532" t="s">
+      <c r="D3" s="1754" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1540" t="s">
+      <c r="E3" s="1762" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="1546" t="s">
+      <c r="F3" s="1768" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="1554" t="s">
+      <c r="G3" s="1776" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="1562" t="s">
+      <c r="H3" s="1784" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="1570" t="s">
+      <c r="J3" s="1792" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="1578" t="s">
+      <c r="K3" s="1800" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="1586" t="s">
+      <c r="L3" s="1808" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -11725,32 +12391,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1525" t="s">
+      <c r="C4" s="1747" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1533" t="s">
+      <c r="D4" s="1755" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="1541" t="s">
+      <c r="E4" s="1763" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="1547" t="s">
+      <c r="F4" s="1769" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="1555" t="s">
+      <c r="G4" s="1777" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="1563" t="s">
+      <c r="H4" s="1785" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="1571" t="s">
+      <c r="J4" s="1793" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="1579" t="s">
+      <c r="K4" s="1801" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="1587" t="s">
+      <c r="L4" s="1809" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -11764,30 +12430,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1526" t="s">
+      <c r="C5" s="1748" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1534" t="s">
+      <c r="D5" s="1756" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="1548" t="s">
+      <c r="F5" s="1770" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="1556" t="s">
+      <c r="G5" s="1778" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="1564" t="s">
+      <c r="H5" s="1786" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="1572" t="s">
+      <c r="J5" s="1794" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="1580" t="s">
+      <c r="K5" s="1802" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="1588" t="s">
+      <c r="L5" s="1810" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -11801,32 +12467,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="1527" t="s">
+      <c r="C6" s="1749" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1535" t="s">
+      <c r="D6" s="1757" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="1542" t="s">
+      <c r="E6" s="1764" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="1549" t="s">
+      <c r="F6" s="1771" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="1557" t="s">
+      <c r="G6" s="1779" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="1565" t="s">
+      <c r="H6" s="1787" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="1573" t="s">
+      <c r="J6" s="1795" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="1581" t="s">
+      <c r="K6" s="1803" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="1589" t="s">
+      <c r="L6" s="1811" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -11840,32 +12506,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="1528" t="s">
+      <c r="C7" s="1750" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1536" t="s">
+      <c r="D7" s="1758" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1543" t="s">
+      <c r="E7" s="1765" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="1550" t="s">
+      <c r="F7" s="1772" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="1558" t="s">
+      <c r="G7" s="1780" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="1566" t="s">
+      <c r="H7" s="1788" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="1574" t="s">
+      <c r="J7" s="1796" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="1582" t="s">
+      <c r="K7" s="1804" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="1590" t="s">
+      <c r="L7" s="1812" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -11879,30 +12545,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="1529" t="s">
+      <c r="C8" s="1751" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1537" t="s">
+      <c r="D8" s="1759" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="1551" t="s">
+      <c r="F8" s="1773" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="1559" t="s">
+      <c r="G8" s="1781" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="1567" t="s">
+      <c r="H8" s="1789" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="1575" t="s">
+      <c r="J8" s="1797" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="1583" t="s">
+      <c r="K8" s="1805" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="1591" t="s">
+      <c r="L8" s="1813" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -11916,32 +12582,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="1530" t="s">
+      <c r="C9" s="1752" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1538" t="s">
+      <c r="D9" s="1760" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="1544" t="s">
+      <c r="E9" s="1766" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="1552" t="s">
+      <c r="F9" s="1774" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="1560" t="s">
+      <c r="G9" s="1782" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="1568" t="s">
+      <c r="H9" s="1790" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="1576" t="s">
+      <c r="J9" s="1798" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="1584" t="s">
+      <c r="K9" s="1806" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="1592" t="s">
+      <c r="L9" s="1814" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -11955,32 +12621,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="1531" t="s">
+      <c r="C10" s="1753" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1539" t="s">
+      <c r="D10" s="1761" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="1545" t="s">
+      <c r="E10" s="1767" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="1553" t="s">
+      <c r="F10" s="1775" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1561" t="s">
+      <c r="G10" s="1783" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1569" t="s">
+      <c r="H10" s="1791" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="1577" t="s">
+      <c r="J10" s="1799" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1585" t="s">
+      <c r="K10" s="1807" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="1593" t="s">
+      <c r="L10" s="1815" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -31470,34 +32136,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1594" t="s">
+      <c r="A3" s="1816" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="1596" t="s">
+      <c r="D3" s="1818" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="1598" t="s">
+      <c r="E3" s="1820" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="1600" t="s">
+      <c r="F3" s="1822" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="1595">
+      <c r="A4" t="s" s="1817">
         <v>150</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="1597">
+      <c r="D4" t="s" s="1819">
         <v>151</v>
       </c>
-      <c r="E4" t="s" s="1599">
+      <c r="E4" t="s" s="1821">
         <v>152</v>
       </c>
-      <c r="F4" t="s" s="1601">
+      <c r="F4" t="s" s="1823">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-31 22:42:02]  fixed minor issue with social studies standards"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1824">
+  <cellXfs count="1935">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1127,6 +1127,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -9539,44 +9872,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1713" t="s">
+      <c r="A3" s="1824" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1715" t="s">
+      <c r="B3" s="1826" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1717" t="s">
+      <c r="C3" s="1828" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1719" t="s">
+      <c r="D3" s="1830" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1721" t="s">
+      <c r="E3" s="1832" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="1723" t="s">
+      <c r="G3" s="1834" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1714" t="s">
+      <c r="A4" s="1825" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1716" t="s">
+      <c r="B4" s="1827" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1718" t="s">
+      <c r="C4" s="1829" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1720" t="s">
+      <c r="D4" s="1831" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1722" t="s">
+      <c r="E4" s="1833" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="1724" t="s">
+      <c r="G4" s="1835" t="s">
         <v>37</v>
       </c>
     </row>
@@ -10733,81 +11066,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1725" t="s">
+      <c r="C3" s="1836" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1728" t="s">
+      <c r="D3" s="1839" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1731" t="s">
+      <c r="E3" s="1842" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="1734" t="s">
+      <c r="F3" s="1845" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="1737" t="s">
+      <c r="H3" s="1848" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="1740" t="s">
+      <c r="I3" s="1851" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="1743" t="s">
+      <c r="K3" s="1854" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1726" t="s">
+      <c r="C4" s="1837" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1729" t="s">
+      <c r="D4" s="1840" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="1732" t="s">
+      <c r="E4" s="1843" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="1735" t="s">
+      <c r="F4" s="1846" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="1738" t="s">
+      <c r="H4" s="1849" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="1741" t="s">
+      <c r="I4" s="1852" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1744" t="s">
+      <c r="K4" s="1855" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1727" t="s">
+      <c r="C5" s="1838" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1730" t="s">
+      <c r="D5" s="1841" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="1733" t="s">
+      <c r="E5" s="1844" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="1736" t="s">
+      <c r="F5" s="1847" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="1739" t="s">
+      <c r="H5" s="1850" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="1742" t="s">
+      <c r="I5" s="1853" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1745" t="s">
+      <c r="K5" s="1856" t="s">
         <v>62</v>
       </c>
     </row>
@@ -12352,32 +12685,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1746" t="s">
+      <c r="C3" s="1857" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1754" t="s">
+      <c r="D3" s="1865" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1762" t="s">
+      <c r="E3" s="1873" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="1768" t="s">
+      <c r="F3" s="1879" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="1776" t="s">
+      <c r="G3" s="1887" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="1784" t="s">
+      <c r="H3" s="1895" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="1792" t="s">
+      <c r="J3" s="1903" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="1800" t="s">
+      <c r="K3" s="1911" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="1808" t="s">
+      <c r="L3" s="1919" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -12391,32 +12724,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1747" t="s">
+      <c r="C4" s="1858" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1755" t="s">
+      <c r="D4" s="1866" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="1763" t="s">
+      <c r="E4" s="1874" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="1769" t="s">
+      <c r="F4" s="1880" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="1777" t="s">
+      <c r="G4" s="1888" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="1785" t="s">
+      <c r="H4" s="1896" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="1793" t="s">
+      <c r="J4" s="1904" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="1801" t="s">
+      <c r="K4" s="1912" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="1809" t="s">
+      <c r="L4" s="1920" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -12430,30 +12763,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1748" t="s">
+      <c r="C5" s="1859" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1756" t="s">
+      <c r="D5" s="1867" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="1770" t="s">
+      <c r="F5" s="1881" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="1778" t="s">
+      <c r="G5" s="1889" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="1786" t="s">
+      <c r="H5" s="1897" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="1794" t="s">
+      <c r="J5" s="1905" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="1802" t="s">
+      <c r="K5" s="1913" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="1810" t="s">
+      <c r="L5" s="1921" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -12467,32 +12800,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="1749" t="s">
+      <c r="C6" s="1860" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1757" t="s">
+      <c r="D6" s="1868" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="1764" t="s">
+      <c r="E6" s="1875" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="1771" t="s">
+      <c r="F6" s="1882" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="1779" t="s">
+      <c r="G6" s="1890" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="1787" t="s">
+      <c r="H6" s="1898" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="1795" t="s">
+      <c r="J6" s="1906" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="1803" t="s">
+      <c r="K6" s="1914" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="1811" t="s">
+      <c r="L6" s="1922" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -12506,32 +12839,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="1750" t="s">
+      <c r="C7" s="1861" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1758" t="s">
+      <c r="D7" s="1869" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1765" t="s">
+      <c r="E7" s="1876" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="1772" t="s">
+      <c r="F7" s="1883" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="1780" t="s">
+      <c r="G7" s="1891" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="1788" t="s">
+      <c r="H7" s="1899" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="1796" t="s">
+      <c r="J7" s="1907" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="1804" t="s">
+      <c r="K7" s="1915" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="1812" t="s">
+      <c r="L7" s="1923" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -12545,30 +12878,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="1751" t="s">
+      <c r="C8" s="1862" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1759" t="s">
+      <c r="D8" s="1870" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="1773" t="s">
+      <c r="F8" s="1884" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="1781" t="s">
+      <c r="G8" s="1892" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="1789" t="s">
+      <c r="H8" s="1900" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="1797" t="s">
+      <c r="J8" s="1908" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="1805" t="s">
+      <c r="K8" s="1916" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="1813" t="s">
+      <c r="L8" s="1924" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -12582,32 +12915,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="1752" t="s">
+      <c r="C9" s="1863" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1760" t="s">
+      <c r="D9" s="1871" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="1766" t="s">
+      <c r="E9" s="1877" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="1774" t="s">
+      <c r="F9" s="1885" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="1782" t="s">
+      <c r="G9" s="1893" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="1790" t="s">
+      <c r="H9" s="1901" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="1798" t="s">
+      <c r="J9" s="1909" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="1806" t="s">
+      <c r="K9" s="1917" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="1814" t="s">
+      <c r="L9" s="1925" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -12621,32 +12954,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="1753" t="s">
+      <c r="C10" s="1864" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1761" t="s">
+      <c r="D10" s="1872" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="1767" t="s">
+      <c r="E10" s="1878" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="1775" t="s">
+      <c r="F10" s="1886" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1783" t="s">
+      <c r="G10" s="1894" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1791" t="s">
+      <c r="H10" s="1902" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="1799" t="s">
+      <c r="J10" s="1910" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1807" t="s">
+      <c r="K10" s="1918" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="1815" t="s">
+      <c r="L10" s="1926" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -32136,34 +32469,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1816" t="s">
+      <c r="A3" s="1927" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="1818" t="s">
+      <c r="D3" s="1929" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="1820" t="s">
+      <c r="E3" s="1931" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="1822" t="s">
+      <c r="F3" s="1933" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="1817">
+      <c r="A4" t="s" s="1928">
         <v>150</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="1819">
+      <c r="D4" t="s" s="1930">
         <v>151</v>
       </c>
-      <c r="E4" t="s" s="1821">
+      <c r="E4" t="s" s="1932">
         <v>152</v>
       </c>
-      <c r="F4" t="s" s="1823">
+      <c r="F4" t="s" s="1934">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-08-31 22:55:53]  added Madelyn to credits ... again??"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2341" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1935">
+  <cellXfs count="2046">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1127,6 +1127,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -9872,44 +10205,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1824" t="s">
+      <c r="A3" s="1935" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1826" t="s">
+      <c r="B3" s="1937" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1828" t="s">
+      <c r="C3" s="1939" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1830" t="s">
+      <c r="D3" s="1941" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1832" t="s">
+      <c r="E3" s="1943" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="1834" t="s">
+      <c r="G3" s="1945" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1825" t="s">
+      <c r="A4" s="1936" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1827" t="s">
+      <c r="B4" s="1938" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1829" t="s">
+      <c r="C4" s="1940" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1831" t="s">
+      <c r="D4" s="1942" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1833" t="s">
+      <c r="E4" s="1944" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="1835" t="s">
+      <c r="G4" s="1946" t="s">
         <v>37</v>
       </c>
     </row>
@@ -11066,81 +11399,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1836" t="s">
+      <c r="C3" s="1947" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1839" t="s">
+      <c r="D3" s="1950" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1842" t="s">
+      <c r="E3" s="1953" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="1845" t="s">
+      <c r="F3" s="1956" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="1848" t="s">
+      <c r="H3" s="1959" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="1851" t="s">
+      <c r="I3" s="1962" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="1854" t="s">
+      <c r="K3" s="1965" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1837" t="s">
+      <c r="C4" s="1948" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1840" t="s">
+      <c r="D4" s="1951" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="1843" t="s">
+      <c r="E4" s="1954" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="1846" t="s">
+      <c r="F4" s="1957" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="1849" t="s">
+      <c r="H4" s="1960" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="1852" t="s">
+      <c r="I4" s="1963" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1855" t="s">
+      <c r="K4" s="1966" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1838" t="s">
+      <c r="C5" s="1949" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1841" t="s">
+      <c r="D5" s="1952" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="1844" t="s">
+      <c r="E5" s="1955" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="1847" t="s">
+      <c r="F5" s="1958" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="1850" t="s">
+      <c r="H5" s="1961" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="1853" t="s">
+      <c r="I5" s="1964" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1856" t="s">
+      <c r="K5" s="1967" t="s">
         <v>62</v>
       </c>
     </row>
@@ -12685,32 +13018,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1857" t="s">
+      <c r="C3" s="1968" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1865" t="s">
+      <c r="D3" s="1976" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1873" t="s">
+      <c r="E3" s="1984" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="1879" t="s">
+      <c r="F3" s="1990" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="1887" t="s">
+      <c r="G3" s="1998" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="1895" t="s">
+      <c r="H3" s="2006" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="1903" t="s">
+      <c r="J3" s="2014" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="1911" t="s">
+      <c r="K3" s="2022" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="1919" t="s">
+      <c r="L3" s="2030" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -12724,32 +13057,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1858" t="s">
+      <c r="C4" s="1969" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1866" t="s">
+      <c r="D4" s="1977" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="1874" t="s">
+      <c r="E4" s="1985" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="1880" t="s">
+      <c r="F4" s="1991" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="1888" t="s">
+      <c r="G4" s="1999" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="1896" t="s">
+      <c r="H4" s="2007" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="1904" t="s">
+      <c r="J4" s="2015" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="1912" t="s">
+      <c r="K4" s="2023" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="1920" t="s">
+      <c r="L4" s="2031" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -12763,30 +13096,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1859" t="s">
+      <c r="C5" s="1970" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1867" t="s">
+      <c r="D5" s="1978" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="1881" t="s">
+      <c r="F5" s="1992" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="1889" t="s">
+      <c r="G5" s="2000" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="1897" t="s">
+      <c r="H5" s="2008" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="1905" t="s">
+      <c r="J5" s="2016" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="1913" t="s">
+      <c r="K5" s="2024" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="1921" t="s">
+      <c r="L5" s="2032" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -12800,32 +13133,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="1860" t="s">
+      <c r="C6" s="1971" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1868" t="s">
+      <c r="D6" s="1979" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="1875" t="s">
+      <c r="E6" s="1986" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="1882" t="s">
+      <c r="F6" s="1993" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="1890" t="s">
+      <c r="G6" s="2001" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="1898" t="s">
+      <c r="H6" s="2009" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="1906" t="s">
+      <c r="J6" s="2017" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="1914" t="s">
+      <c r="K6" s="2025" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="1922" t="s">
+      <c r="L6" s="2033" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -12839,32 +13172,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="1861" t="s">
+      <c r="C7" s="1972" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1869" t="s">
+      <c r="D7" s="1980" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1876" t="s">
+      <c r="E7" s="1987" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="1883" t="s">
+      <c r="F7" s="1994" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="1891" t="s">
+      <c r="G7" s="2002" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="1899" t="s">
+      <c r="H7" s="2010" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="1907" t="s">
+      <c r="J7" s="2018" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="1915" t="s">
+      <c r="K7" s="2026" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="1923" t="s">
+      <c r="L7" s="2034" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -12878,30 +13211,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="1862" t="s">
+      <c r="C8" s="1973" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1870" t="s">
+      <c r="D8" s="1981" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="1884" t="s">
+      <c r="F8" s="1995" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="1892" t="s">
+      <c r="G8" s="2003" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="1900" t="s">
+      <c r="H8" s="2011" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="1908" t="s">
+      <c r="J8" s="2019" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="1916" t="s">
+      <c r="K8" s="2027" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="1924" t="s">
+      <c r="L8" s="2035" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -12915,32 +13248,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="1863" t="s">
+      <c r="C9" s="1974" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1871" t="s">
+      <c r="D9" s="1982" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="1877" t="s">
+      <c r="E9" s="1988" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="1885" t="s">
+      <c r="F9" s="1996" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="1893" t="s">
+      <c r="G9" s="2004" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="1901" t="s">
+      <c r="H9" s="2012" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="1909" t="s">
+      <c r="J9" s="2020" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="1917" t="s">
+      <c r="K9" s="2028" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="1925" t="s">
+      <c r="L9" s="2036" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -12954,32 +13287,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="1864" t="s">
+      <c r="C10" s="1975" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1872" t="s">
+      <c r="D10" s="1983" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="1878" t="s">
+      <c r="E10" s="1989" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="1886" t="s">
+      <c r="F10" s="1997" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="1894" t="s">
+      <c r="G10" s="2005" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="1902" t="s">
+      <c r="H10" s="2013" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="1910" t="s">
+      <c r="J10" s="2021" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="1918" t="s">
+      <c r="K10" s="2029" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="1926" t="s">
+      <c r="L10" s="2037" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -32469,34 +32802,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1927" t="s">
+      <c r="A3" s="2038" t="s">
         <v>158</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="1929" t="s">
+      <c r="D3" s="2040" t="s">
         <v>159</v>
       </c>
-      <c r="E3" s="1931" t="s">
+      <c r="E3" s="2042" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="1933" t="s">
+      <c r="F3" s="2044" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="1928">
+      <c r="A4" t="s" s="2039">
         <v>150</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="1930">
+      <c r="D4" t="s" s="2041">
         <v>151</v>
       </c>
-      <c r="E4" t="s" s="1932">
+      <c r="E4" t="s" s="2043">
         <v>152</v>
       </c>
-      <c r="F4" t="s" s="1934">
+      <c r="F4" t="s" s="2045">
         <v>153</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-05 19:58:31]  "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2341" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="230">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -716,6 +716,210 @@
   <si>
     <t>1hhCN2R-J_6JLJwBuNOqzuP2vZ5MXhPIPyDMgerZKNrw</t>
   </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1XG-42nE5qCOHpUyCJ9LqoN0GAvycTZRj</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1Vhyr8y-3xQBR9XNFzh6EG-y7SeXhEjW5</t>
+  </si>
+  <si>
+    <t>1XG-42nE5qCOHpUyCJ9LqoN0GAvycTZRj</t>
+  </si>
+  <si>
+    <t>1Vhyr8y-3xQBR9XNFzh6EG-y7SeXhEjW5</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P1_Presentation_classroom</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P2_Presentation_classroom</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P3_Presentation_classroom</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1Ms756WmF4viacoZCqjxcl0cuFzIhT2LOfxvhgqNyvJk/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1uD6KT1aHFXo0pwSXTDLi9Jo-t0-Nr4pRF9aL1wdJ79k/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1kqA1GbcsvtVidaA6UvEMX6Zh1eFg_sK4AnUlcxe5j-A/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1Ms756WmF4viacoZCqjxcl0cuFzIhT2LOfxvhgqNyvJk/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1uD6KT1aHFXo0pwSXTDLi9Jo-t0-Nr4pRF9aL1wdJ79k/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1kqA1GbcsvtVidaA6UvEMX6Zh1eFg_sK4AnUlcxe5j-A/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1Ms756WmF4viacoZCqjxcl0cuFzIhT2LOfxvhgqNyvJk/present</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1uD6KT1aHFXo0pwSXTDLi9Jo-t0-Nr4pRF9aL1wdJ79k/present</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1kqA1GbcsvtVidaA6UvEMX6Zh1eFg_sK4AnUlcxe5j-A/present</t>
+  </si>
+  <si>
+    <t>1Ms756WmF4viacoZCqjxcl0cuFzIhT2LOfxvhgqNyvJk</t>
+  </si>
+  <si>
+    <t>1uD6KT1aHFXo0pwSXTDLi9Jo-t0-Nr4pRF9aL1wdJ79k</t>
+  </si>
+  <si>
+    <t>1kqA1GbcsvtVidaA6UvEMX6Zh1eFg_sK4AnUlcxe5j-A</t>
+  </si>
+  <si>
+    <t>Worksheet (P1)</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P1_Worksheet (STUDENT)</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P1_Worksheet (TEACHER)</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P1_Reading Handout</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P2_Worksheet (STUDENT)</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P2_Worksheet (TEACHER)</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P2_Cost Cards</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P3_Worksheet (STUDENT)</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_P3_Worksheet (TEACHER)</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/19ITdnilpOCnlm2tbuAMnW9P11vp6yPKk0golN4uneto/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1ELVmQoPqO45dsYTB3x4dUb9eF1XEiEnOZHsYXooBS30/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1kHi7f7gxlMjL_FKWn-lgeqjmC5VlSx2_KJQ3w1cftVw/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1RABNcunP2cTVlksvQ9j_WrLXsXn0o_0Wv-yvS2qOdiQ/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1YqsH7Dgc0gZrWZ7uMu7Q8ak_zLLZdNmPZ2kSTkE3ug4/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1jWUl4_HDbz822WH1Nbrvc0uNei31BjXzO0oZIhwJDtA/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1CE9qh0YPkk9X6rZY4ylKBR3Ch1ch3Rw2R68cLwAifL8/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1-V56RE816HL1VXByPkEj4TW2v3TOMX6GN-5fhowhK0U/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/19ITdnilpOCnlm2tbuAMnW9P11vp6yPKk0golN4uneto/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1ELVmQoPqO45dsYTB3x4dUb9eF1XEiEnOZHsYXooBS30/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1kHi7f7gxlMjL_FKWn-lgeqjmC5VlSx2_KJQ3w1cftVw/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1RABNcunP2cTVlksvQ9j_WrLXsXn0o_0Wv-yvS2qOdiQ/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1YqsH7Dgc0gZrWZ7uMu7Q8ak_zLLZdNmPZ2kSTkE3ug4/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1jWUl4_HDbz822WH1Nbrvc0uNei31BjXzO0oZIhwJDtA/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1CE9qh0YPkk9X6rZY4ylKBR3Ch1ch3Rw2R68cLwAifL8/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1-V56RE816HL1VXByPkEj4TW2v3TOMX6GN-5fhowhK0U/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/19ITdnilpOCnlm2tbuAMnW9P11vp6yPKk0golN4uneto/export?format=pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1ELVmQoPqO45dsYTB3x4dUb9eF1XEiEnOZHsYXooBS30/export?format=pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1kHi7f7gxlMjL_FKWn-lgeqjmC5VlSx2_KJQ3w1cftVw/export?format=pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1RABNcunP2cTVlksvQ9j_WrLXsXn0o_0Wv-yvS2qOdiQ/export?format=pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1YqsH7Dgc0gZrWZ7uMu7Q8ak_zLLZdNmPZ2kSTkE3ug4/export?format=pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/presentation/d/1jWUl4_HDbz822WH1Nbrvc0uNei31BjXzO0oZIhwJDtA/export/pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1CE9qh0YPkk9X6rZY4ylKBR3Ch1ch3Rw2R68cLwAifL8/export?format=pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1-V56RE816HL1VXByPkEj4TW2v3TOMX6GN-5fhowhK0U/export?format=pdf</t>
+  </si>
+  <si>
+    <t>19ITdnilpOCnlm2tbuAMnW9P11vp6yPKk0golN4uneto</t>
+  </si>
+  <si>
+    <t>1ELVmQoPqO45dsYTB3x4dUb9eF1XEiEnOZHsYXooBS30</t>
+  </si>
+  <si>
+    <t>1kHi7f7gxlMjL_FKWn-lgeqjmC5VlSx2_KJQ3w1cftVw</t>
+  </si>
+  <si>
+    <t>1RABNcunP2cTVlksvQ9j_WrLXsXn0o_0Wv-yvS2qOdiQ</t>
+  </si>
+  <si>
+    <t>1YqsH7Dgc0gZrWZ7uMu7Q8ak_zLLZdNmPZ2kSTkE3ug4</t>
+  </si>
+  <si>
+    <t>1jWUl4_HDbz822WH1Nbrvc0uNei31BjXzO0oZIhwJDtA</t>
+  </si>
+  <si>
+    <t>1CE9qh0YPkk9X6rZY4ylKBR3Ch1ch3Rw2R68cLwAifL8</t>
+  </si>
+  <si>
+    <t>1-V56RE816HL1VXByPkEj4TW2v3TOMX6GN-5fhowhK0U</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_Pre Post Assessment (STUDENT)</t>
+  </si>
+  <si>
+    <t>ColorfulSolns_Pre Post Assessment (TEACHER)</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1YW3X4Ku06z2hrvZFIFbDmJ6miTlqGnikzbodZ-9E6ZU/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1PvwVv5paQYzWHC2A021tWgCnBLW6a5E8H5EZcdDkB9g/template/preview</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1YW3X4Ku06z2hrvZFIFbDmJ6miTlqGnikzbodZ-9E6ZU/export?format=pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/1PvwVv5paQYzWHC2A021tWgCnBLW6a5E8H5EZcdDkB9g/export?format=pdf</t>
+  </si>
+  <si>
+    <t>1YW3X4Ku06z2hrvZFIFbDmJ6miTlqGnikzbodZ-9E6ZU</t>
+  </si>
+  <si>
+    <t>1PvwVv5paQYzWHC2A021tWgCnBLW6a5E8H5EZcdDkB9g</t>
+  </si>
 </sst>
 </file>
 
@@ -1014,7 +1218,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2046">
+  <cellXfs count="2268">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1127,6 +1331,672 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -10205,45 +11075,45 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="1935" t="s">
+      <c r="A3" s="2157" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1937" t="s">
+      <c r="B3" s="2159" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1939" t="s">
+      <c r="C3" s="2161" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1941" t="s">
+      <c r="D3" s="2163" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1943" t="s">
-        <v>33</v>
+      <c r="E3" s="2165" t="s">
+        <v>162</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="1945" t="s">
-        <v>34</v>
+      <c r="G3" s="2167" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1936" t="s">
+      <c r="A4" s="2158" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1938" t="s">
+      <c r="B4" s="2160" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="1940" t="s">
+      <c r="C4" s="2162" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="1942" t="s">
+      <c r="D4" s="2164" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="1944" t="s">
-        <v>36</v>
+      <c r="E4" s="2166" t="s">
+        <v>163</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="1946" t="s">
-        <v>37</v>
+      <c r="G4" s="2168" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="5">
@@ -11399,82 +12269,82 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1947" t="s">
+      <c r="C3" s="2169" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1950" t="s">
+      <c r="D3" s="2172" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1953" t="s">
-        <v>46</v>
+      <c r="E3" s="2175" t="s">
+        <v>166</v>
       </c>
-      <c r="F3" s="1956" t="s">
-        <v>47</v>
+      <c r="F3" s="2178" t="s">
+        <v>169</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="1959" t="s">
-        <v>48</v>
+      <c r="H3" s="2181" t="s">
+        <v>172</v>
       </c>
-      <c r="I3" s="1962" t="s">
-        <v>49</v>
+      <c r="I3" s="2184" t="s">
+        <v>175</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="1965" t="s">
-        <v>50</v>
+      <c r="K3" s="2187" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1948" t="s">
+      <c r="C4" s="2170" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1951" t="s">
+      <c r="D4" s="2173" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="1954" t="s">
-        <v>52</v>
+      <c r="E4" s="2176" t="s">
+        <v>167</v>
       </c>
-      <c r="F4" s="1957" t="s">
-        <v>53</v>
+      <c r="F4" s="2179" t="s">
+        <v>170</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="1960" t="s">
-        <v>54</v>
+      <c r="H4" s="2182" t="s">
+        <v>173</v>
       </c>
-      <c r="I4" s="1963" t="s">
-        <v>55</v>
+      <c r="I4" s="2185" t="s">
+        <v>176</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="1966" t="s">
-        <v>56</v>
+      <c r="K4" s="2188" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1949" t="s">
+      <c r="C5" s="2171" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1952" t="s">
+      <c r="D5" s="2174" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="1955" t="s">
-        <v>58</v>
+      <c r="E5" s="2177" t="s">
+        <v>168</v>
       </c>
-      <c r="F5" s="1958" t="s">
-        <v>59</v>
+      <c r="F5" s="2180" t="s">
+        <v>171</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="1961" t="s">
-        <v>60</v>
+      <c r="H5" s="2183" t="s">
+        <v>174</v>
       </c>
-      <c r="I5" s="1964" t="s">
-        <v>61</v>
+      <c r="I5" s="2186" t="s">
+        <v>177</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="1967" t="s">
-        <v>62</v>
+      <c r="K5" s="2189" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="6">
@@ -13018,33 +13888,33 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="1968" t="s">
+      <c r="C3" s="2190" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1976" t="s">
+      <c r="D3" s="2198" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="1984" t="s">
+      <c r="E3" s="2206" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="1990" t="s">
+      <c r="F3" s="2212" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="1998" t="s">
-        <v>69</v>
+      <c r="G3" s="2220" t="s">
+        <v>182</v>
       </c>
-      <c r="H3" s="2006" t="s">
-        <v>70</v>
+      <c r="H3" s="2228" t="s">
+        <v>190</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="2014" t="s">
-        <v>71</v>
+      <c r="J3" s="2236" t="s">
+        <v>198</v>
       </c>
-      <c r="K3" s="2022" t="s">
-        <v>72</v>
+      <c r="K3" s="2244" t="s">
+        <v>206</v>
       </c>
-      <c r="L3" s="2030" t="s">
-        <v>73</v>
+      <c r="L3" s="2252" t="s">
+        <v>214</v>
       </c>
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
@@ -13057,33 +13927,33 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="1969" t="s">
+      <c r="C4" s="2191" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="1977" t="s">
+      <c r="D4" s="2199" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="1985" t="s">
+      <c r="E4" s="2207" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="1991" t="s">
+      <c r="F4" s="2213" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="1999" t="s">
-        <v>76</v>
+      <c r="G4" s="2221" t="s">
+        <v>183</v>
       </c>
-      <c r="H4" s="2007" t="s">
-        <v>77</v>
+      <c r="H4" s="2229" t="s">
+        <v>191</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="2015" t="s">
-        <v>78</v>
+      <c r="J4" s="2237" t="s">
+        <v>199</v>
       </c>
-      <c r="K4" s="2023" t="s">
-        <v>79</v>
+      <c r="K4" s="2245" t="s">
+        <v>207</v>
       </c>
-      <c r="L4" s="2031" t="s">
-        <v>80</v>
+      <c r="L4" s="2253" t="s">
+        <v>215</v>
       </c>
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
@@ -13096,31 +13966,31 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="1970" t="s">
+      <c r="C5" s="2192" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="1978" t="s">
+      <c r="D5" s="2200" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="1992" t="s">
-        <v>81</v>
+      <c r="F5" s="2214" t="s">
+        <v>181</v>
       </c>
-      <c r="G5" s="2000" t="s">
-        <v>82</v>
+      <c r="G5" s="2222" t="s">
+        <v>184</v>
       </c>
-      <c r="H5" s="2008" t="s">
-        <v>83</v>
+      <c r="H5" s="2230" t="s">
+        <v>192</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="2016" t="s">
-        <v>84</v>
+      <c r="J5" s="2238" t="s">
+        <v>200</v>
       </c>
-      <c r="K5" s="2024" t="s">
-        <v>85</v>
+      <c r="K5" s="2246" t="s">
+        <v>208</v>
       </c>
-      <c r="L5" s="2032" t="s">
-        <v>86</v>
+      <c r="L5" s="2254" t="s">
+        <v>216</v>
       </c>
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
@@ -13133,33 +14003,33 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="1971" t="s">
+      <c r="C6" s="2193" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1979" t="s">
+      <c r="D6" s="2201" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="1986" t="s">
+      <c r="E6" s="2208" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="1993" t="s">
+      <c r="F6" s="2215" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="2001" t="s">
-        <v>88</v>
+      <c r="G6" s="2223" t="s">
+        <v>185</v>
       </c>
-      <c r="H6" s="2009" t="s">
-        <v>89</v>
+      <c r="H6" s="2231" t="s">
+        <v>193</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="2017" t="s">
-        <v>90</v>
+      <c r="J6" s="2239" t="s">
+        <v>201</v>
       </c>
-      <c r="K6" s="2025" t="s">
-        <v>91</v>
+      <c r="K6" s="2247" t="s">
+        <v>209</v>
       </c>
-      <c r="L6" s="2033" t="s">
-        <v>92</v>
+      <c r="L6" s="2255" t="s">
+        <v>217</v>
       </c>
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
@@ -13172,33 +14042,33 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="1972" t="s">
+      <c r="C7" s="2194" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1980" t="s">
+      <c r="D7" s="2202" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="1987" t="s">
+      <c r="E7" s="2209" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="1994" t="s">
+      <c r="F7" s="2216" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="2002" t="s">
-        <v>94</v>
+      <c r="G7" s="2224" t="s">
+        <v>186</v>
       </c>
-      <c r="H7" s="2010" t="s">
-        <v>95</v>
+      <c r="H7" s="2232" t="s">
+        <v>194</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="2018" t="s">
-        <v>96</v>
+      <c r="J7" s="2240" t="s">
+        <v>202</v>
       </c>
-      <c r="K7" s="2026" t="s">
-        <v>97</v>
+      <c r="K7" s="2248" t="s">
+        <v>210</v>
       </c>
-      <c r="L7" s="2034" t="s">
-        <v>98</v>
+      <c r="L7" s="2256" t="s">
+        <v>218</v>
       </c>
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
@@ -13211,31 +14081,31 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="1973" t="s">
+      <c r="C8" s="2195" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="1981" t="s">
+      <c r="D8" s="2203" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="1995" t="s">
+      <c r="F8" s="2217" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="2003" t="s">
-        <v>100</v>
+      <c r="G8" s="2225" t="s">
+        <v>187</v>
       </c>
-      <c r="H8" s="2011" t="s">
-        <v>101</v>
+      <c r="H8" s="2233" t="s">
+        <v>195</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="2019" t="s">
-        <v>102</v>
+      <c r="J8" s="2241" t="s">
+        <v>203</v>
       </c>
-      <c r="K8" s="2027" t="s">
-        <v>103</v>
+      <c r="K8" s="2249" t="s">
+        <v>211</v>
       </c>
-      <c r="L8" s="2035" t="s">
-        <v>104</v>
+      <c r="L8" s="2257" t="s">
+        <v>219</v>
       </c>
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
@@ -13248,33 +14118,33 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="1974" t="s">
+      <c r="C9" s="2196" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="1982" t="s">
+      <c r="D9" s="2204" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="1988" t="s">
+      <c r="E9" s="2210" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="1996" t="s">
+      <c r="F9" s="2218" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="2004" t="s">
-        <v>106</v>
+      <c r="G9" s="2226" t="s">
+        <v>188</v>
       </c>
-      <c r="H9" s="2012" t="s">
-        <v>107</v>
+      <c r="H9" s="2234" t="s">
+        <v>196</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="2020" t="s">
-        <v>108</v>
+      <c r="J9" s="2242" t="s">
+        <v>204</v>
       </c>
-      <c r="K9" s="2028" t="s">
-        <v>109</v>
+      <c r="K9" s="2250" t="s">
+        <v>212</v>
       </c>
-      <c r="L9" s="2036" t="s">
-        <v>110</v>
+      <c r="L9" s="2258" t="s">
+        <v>220</v>
       </c>
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
@@ -13287,33 +14157,33 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="1975" t="s">
+      <c r="C10" s="2197" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1983" t="s">
+      <c r="D10" s="2205" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="1989" t="s">
+      <c r="E10" s="2211" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="1997" t="s">
+      <c r="F10" s="2219" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="2005" t="s">
-        <v>112</v>
+      <c r="G10" s="2227" t="s">
+        <v>189</v>
       </c>
-      <c r="H10" s="2013" t="s">
-        <v>113</v>
+      <c r="H10" s="2235" t="s">
+        <v>197</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="2021" t="s">
-        <v>114</v>
+      <c r="J10" s="2243" t="s">
+        <v>205</v>
       </c>
-      <c r="K10" s="2029" t="s">
-        <v>115</v>
+      <c r="K10" s="2251" t="s">
+        <v>213</v>
       </c>
-      <c r="L10" s="2037" t="s">
-        <v>116</v>
+      <c r="L10" s="2259" t="s">
+        <v>221</v>
       </c>
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
@@ -32802,35 +33672,35 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2038" t="s">
-        <v>158</v>
+      <c r="A3" s="2260" t="s">
+        <v>222</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="2040" t="s">
-        <v>159</v>
+      <c r="D3" s="2262" t="s">
+        <v>224</v>
       </c>
-      <c r="E3" s="2042" t="s">
-        <v>160</v>
+      <c r="E3" s="2264" t="s">
+        <v>226</v>
       </c>
-      <c r="F3" s="2044" t="s">
-        <v>161</v>
+      <c r="F3" s="2266" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="2039">
-        <v>150</v>
+      <c r="A4" t="s" s="2261">
+        <v>223</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="2041">
-        <v>151</v>
+      <c r="D4" t="s" s="2263">
+        <v>225</v>
       </c>
-      <c r="E4" t="s" s="2043">
-        <v>152</v>
+      <c r="E4" t="s" s="2265">
+        <v>227</v>
       </c>
-      <c r="F4" t="s" s="2045">
-        <v>153</v>
+      <c r="F4" t="s" s="2267">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-05 22:59:19]  added epaulette; fixed Pangaia link"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2563" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="232">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -920,6 +920,12 @@
   <si>
     <t>1PvwVv5paQYzWHC2A021tWgCnBLW6a5E8H5EZcdDkB9g</t>
   </si>
+  <si>
+    <t>8-12</t>
+  </si>
+  <si>
+    <t>/classroom/classroom_g8-12/</t>
+  </si>
 </sst>
 </file>
 
@@ -1218,7 +1224,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2268">
+  <cellXfs count="2601">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1331,6 +1337,1005 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -11075,44 +12080,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="2157" t="s">
+      <c r="A3" s="2490" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2159" t="s">
-        <v>30</v>
+      <c r="B3" s="2492" t="s">
+        <v>230</v>
       </c>
-      <c r="C3" s="2161" t="s">
+      <c r="C3" s="2494" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2163" t="s">
-        <v>32</v>
+      <c r="D3" s="2496" t="s">
+        <v>231</v>
       </c>
-      <c r="E3" s="2165" t="s">
+      <c r="E3" s="2498" t="s">
         <v>162</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="2167" t="s">
+      <c r="G3" s="2500" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2158" t="s">
+      <c r="A4" s="2491" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2160" t="s">
+      <c r="B4" s="2493" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2162" t="s">
+      <c r="C4" s="2495" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2164" t="s">
+      <c r="D4" s="2497" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="2166" t="s">
+      <c r="E4" s="2499" t="s">
         <v>163</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="2168" t="s">
+      <c r="G4" s="2501" t="s">
         <v>165</v>
       </c>
     </row>
@@ -12269,81 +13274,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2169" t="s">
-        <v>30</v>
+      <c r="C3" s="2502" t="s">
+        <v>230</v>
       </c>
-      <c r="D3" s="2172" t="s">
+      <c r="D3" s="2505" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2175" t="s">
+      <c r="E3" s="2508" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="2178" t="s">
+      <c r="F3" s="2511" t="s">
         <v>169</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="2181" t="s">
+      <c r="H3" s="2514" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="2184" t="s">
+      <c r="I3" s="2517" t="s">
         <v>175</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="2187" t="s">
+      <c r="K3" s="2520" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2170" t="s">
-        <v>30</v>
+      <c r="C4" s="2503" t="s">
+        <v>230</v>
       </c>
-      <c r="D4" s="2173" t="s">
+      <c r="D4" s="2506" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="2176" t="s">
+      <c r="E4" s="2509" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="2179" t="s">
+      <c r="F4" s="2512" t="s">
         <v>170</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="2182" t="s">
+      <c r="H4" s="2515" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="2185" t="s">
+      <c r="I4" s="2518" t="s">
         <v>176</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="2188" t="s">
+      <c r="K4" s="2521" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2171" t="s">
-        <v>30</v>
+      <c r="C5" s="2504" t="s">
+        <v>230</v>
       </c>
-      <c r="D5" s="2174" t="s">
+      <c r="D5" s="2507" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="2177" t="s">
+      <c r="E5" s="2510" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="2180" t="s">
+      <c r="F5" s="2513" t="s">
         <v>171</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="2183" t="s">
+      <c r="H5" s="2516" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="2186" t="s">
+      <c r="I5" s="2519" t="s">
         <v>177</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="2189" t="s">
+      <c r="K5" s="2522" t="s">
         <v>180</v>
       </c>
     </row>
@@ -13888,32 +14893,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2190" t="s">
-        <v>30</v>
+      <c r="C3" s="2523" t="s">
+        <v>230</v>
       </c>
-      <c r="D3" s="2198" t="s">
+      <c r="D3" s="2531" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2206" t="s">
+      <c r="E3" s="2539" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="2212" t="s">
+      <c r="F3" s="2545" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="2220" t="s">
+      <c r="G3" s="2553" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="2228" t="s">
+      <c r="H3" s="2561" t="s">
         <v>190</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="2236" t="s">
+      <c r="J3" s="2569" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="2244" t="s">
+      <c r="K3" s="2577" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="2252" t="s">
+      <c r="L3" s="2585" t="s">
         <v>214</v>
       </c>
       <c r="U3" s="8"/>
@@ -13927,32 +14932,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2191" t="s">
-        <v>30</v>
+      <c r="C4" s="2524" t="s">
+        <v>230</v>
       </c>
-      <c r="D4" s="2199" t="s">
+      <c r="D4" s="2532" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="2207" t="s">
+      <c r="E4" s="2540" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="2213" t="s">
+      <c r="F4" s="2546" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="2221" t="s">
+      <c r="G4" s="2554" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="2229" t="s">
+      <c r="H4" s="2562" t="s">
         <v>191</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="2237" t="s">
+      <c r="J4" s="2570" t="s">
         <v>199</v>
       </c>
-      <c r="K4" s="2245" t="s">
+      <c r="K4" s="2578" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="2253" t="s">
+      <c r="L4" s="2586" t="s">
         <v>215</v>
       </c>
       <c r="U4" s="8"/>
@@ -13966,30 +14971,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2192" t="s">
-        <v>30</v>
+      <c r="C5" s="2525" t="s">
+        <v>230</v>
       </c>
-      <c r="D5" s="2200" t="s">
+      <c r="D5" s="2533" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="2214" t="s">
+      <c r="F5" s="2547" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="2222" t="s">
+      <c r="G5" s="2555" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="2230" t="s">
+      <c r="H5" s="2563" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="2238" t="s">
+      <c r="J5" s="2571" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="2246" t="s">
+      <c r="K5" s="2579" t="s">
         <v>208</v>
       </c>
-      <c r="L5" s="2254" t="s">
+      <c r="L5" s="2587" t="s">
         <v>216</v>
       </c>
       <c r="U5" s="8"/>
@@ -14003,32 +15008,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="2193" t="s">
-        <v>30</v>
+      <c r="C6" s="2526" t="s">
+        <v>230</v>
       </c>
-      <c r="D6" s="2201" t="s">
+      <c r="D6" s="2534" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2208" t="s">
+      <c r="E6" s="2541" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="2215" t="s">
+      <c r="F6" s="2548" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="2223" t="s">
+      <c r="G6" s="2556" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="2231" t="s">
+      <c r="H6" s="2564" t="s">
         <v>193</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="2239" t="s">
+      <c r="J6" s="2572" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="2247" t="s">
+      <c r="K6" s="2580" t="s">
         <v>209</v>
       </c>
-      <c r="L6" s="2255" t="s">
+      <c r="L6" s="2588" t="s">
         <v>217</v>
       </c>
       <c r="U6" s="8"/>
@@ -14042,32 +15047,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="2194" t="s">
-        <v>30</v>
+      <c r="C7" s="2527" t="s">
+        <v>230</v>
       </c>
-      <c r="D7" s="2202" t="s">
+      <c r="D7" s="2535" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="2209" t="s">
+      <c r="E7" s="2542" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="2216" t="s">
+      <c r="F7" s="2549" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="2224" t="s">
+      <c r="G7" s="2557" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="2232" t="s">
+      <c r="H7" s="2565" t="s">
         <v>194</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="2240" t="s">
+      <c r="J7" s="2573" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="2248" t="s">
+      <c r="K7" s="2581" t="s">
         <v>210</v>
       </c>
-      <c r="L7" s="2256" t="s">
+      <c r="L7" s="2589" t="s">
         <v>218</v>
       </c>
       <c r="U7" s="8"/>
@@ -14081,30 +15086,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="2195" t="s">
-        <v>30</v>
+      <c r="C8" s="2528" t="s">
+        <v>230</v>
       </c>
-      <c r="D8" s="2203" t="s">
+      <c r="D8" s="2536" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="2217" t="s">
+      <c r="F8" s="2550" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="2225" t="s">
+      <c r="G8" s="2558" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="2233" t="s">
+      <c r="H8" s="2566" t="s">
         <v>195</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="2241" t="s">
+      <c r="J8" s="2574" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="2249" t="s">
+      <c r="K8" s="2582" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="2257" t="s">
+      <c r="L8" s="2590" t="s">
         <v>219</v>
       </c>
       <c r="U8" s="8"/>
@@ -14118,32 +15123,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="2196" t="s">
-        <v>30</v>
+      <c r="C9" s="2529" t="s">
+        <v>230</v>
       </c>
-      <c r="D9" s="2204" t="s">
+      <c r="D9" s="2537" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="2210" t="s">
+      <c r="E9" s="2543" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="2218" t="s">
+      <c r="F9" s="2551" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="2226" t="s">
+      <c r="G9" s="2559" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="2234" t="s">
+      <c r="H9" s="2567" t="s">
         <v>196</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="2242" t="s">
+      <c r="J9" s="2575" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="2250" t="s">
+      <c r="K9" s="2583" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="2258" t="s">
+      <c r="L9" s="2591" t="s">
         <v>220</v>
       </c>
       <c r="U9" s="8"/>
@@ -14157,32 +15162,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="2197" t="s">
-        <v>30</v>
+      <c r="C10" s="2530" t="s">
+        <v>230</v>
       </c>
-      <c r="D10" s="2205" t="s">
+      <c r="D10" s="2538" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="2211" t="s">
+      <c r="E10" s="2544" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="2219" t="s">
+      <c r="F10" s="2552" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="2227" t="s">
+      <c r="G10" s="2560" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="2235" t="s">
+      <c r="H10" s="2568" t="s">
         <v>197</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="2243" t="s">
+      <c r="J10" s="2576" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="2251" t="s">
+      <c r="K10" s="2584" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="2259" t="s">
+      <c r="L10" s="2592" t="s">
         <v>221</v>
       </c>
       <c r="U10" s="8"/>
@@ -33672,34 +34677,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2260" t="s">
+      <c r="A3" s="2593" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="2262" t="s">
+      <c r="D3" s="2595" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="2264" t="s">
+      <c r="E3" s="2597" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="2266" t="s">
+      <c r="F3" s="2599" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="2261">
+      <c r="A4" t="s" s="2594">
         <v>223</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="2263">
+      <c r="D4" t="s" s="2596">
         <v>225</v>
       </c>
-      <c r="E4" t="s" s="2265">
+      <c r="E4" t="s" s="2598">
         <v>227</v>
       </c>
-      <c r="F4" t="s" s="2267">
+      <c r="F4" t="s" s="2600">
         <v>229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-05 23:09:21]  changed years to grades"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3007" uniqueCount="232">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1224,7 +1224,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2601">
+  <cellXfs count="2712">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1337,6 +1337,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -12080,44 +12413,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="2490" t="s">
+      <c r="A3" s="2601" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2492" t="s">
+      <c r="B3" s="2603" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="2494" t="s">
+      <c r="C3" s="2605" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2496" t="s">
+      <c r="D3" s="2607" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="2498" t="s">
+      <c r="E3" s="2609" t="s">
         <v>162</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="2500" t="s">
+      <c r="G3" s="2611" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2491" t="s">
+      <c r="A4" s="2602" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2493" t="s">
+      <c r="B4" s="2604" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2495" t="s">
+      <c r="C4" s="2606" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2497" t="s">
+      <c r="D4" s="2608" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="2499" t="s">
+      <c r="E4" s="2610" t="s">
         <v>163</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="2501" t="s">
+      <c r="G4" s="2612" t="s">
         <v>165</v>
       </c>
     </row>
@@ -13274,81 +13607,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2502" t="s">
+      <c r="C3" s="2613" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="2505" t="s">
+      <c r="D3" s="2616" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2508" t="s">
+      <c r="E3" s="2619" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="2511" t="s">
+      <c r="F3" s="2622" t="s">
         <v>169</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="2514" t="s">
+      <c r="H3" s="2625" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="2517" t="s">
+      <c r="I3" s="2628" t="s">
         <v>175</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="2520" t="s">
+      <c r="K3" s="2631" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2503" t="s">
+      <c r="C4" s="2614" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="2506" t="s">
+      <c r="D4" s="2617" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="2509" t="s">
+      <c r="E4" s="2620" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="2512" t="s">
+      <c r="F4" s="2623" t="s">
         <v>170</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="2515" t="s">
+      <c r="H4" s="2626" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="2518" t="s">
+      <c r="I4" s="2629" t="s">
         <v>176</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="2521" t="s">
+      <c r="K4" s="2632" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2504" t="s">
+      <c r="C5" s="2615" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="2507" t="s">
+      <c r="D5" s="2618" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="2510" t="s">
+      <c r="E5" s="2621" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="2513" t="s">
+      <c r="F5" s="2624" t="s">
         <v>171</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="2516" t="s">
+      <c r="H5" s="2627" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="2519" t="s">
+      <c r="I5" s="2630" t="s">
         <v>177</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="2522" t="s">
+      <c r="K5" s="2633" t="s">
         <v>180</v>
       </c>
     </row>
@@ -14893,32 +15226,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2523" t="s">
+      <c r="C3" s="2634" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="2531" t="s">
+      <c r="D3" s="2642" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2539" t="s">
+      <c r="E3" s="2650" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="2545" t="s">
+      <c r="F3" s="2656" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="2553" t="s">
+      <c r="G3" s="2664" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="2561" t="s">
+      <c r="H3" s="2672" t="s">
         <v>190</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="2569" t="s">
+      <c r="J3" s="2680" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="2577" t="s">
+      <c r="K3" s="2688" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="2585" t="s">
+      <c r="L3" s="2696" t="s">
         <v>214</v>
       </c>
       <c r="U3" s="8"/>
@@ -14932,32 +15265,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2524" t="s">
+      <c r="C4" s="2635" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="2532" t="s">
+      <c r="D4" s="2643" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="2540" t="s">
+      <c r="E4" s="2651" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="2546" t="s">
+      <c r="F4" s="2657" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="2554" t="s">
+      <c r="G4" s="2665" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="2562" t="s">
+      <c r="H4" s="2673" t="s">
         <v>191</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="2570" t="s">
+      <c r="J4" s="2681" t="s">
         <v>199</v>
       </c>
-      <c r="K4" s="2578" t="s">
+      <c r="K4" s="2689" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="2586" t="s">
+      <c r="L4" s="2697" t="s">
         <v>215</v>
       </c>
       <c r="U4" s="8"/>
@@ -14971,30 +15304,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2525" t="s">
+      <c r="C5" s="2636" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="2533" t="s">
+      <c r="D5" s="2644" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="2547" t="s">
+      <c r="F5" s="2658" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="2555" t="s">
+      <c r="G5" s="2666" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="2563" t="s">
+      <c r="H5" s="2674" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="2571" t="s">
+      <c r="J5" s="2682" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="2579" t="s">
+      <c r="K5" s="2690" t="s">
         <v>208</v>
       </c>
-      <c r="L5" s="2587" t="s">
+      <c r="L5" s="2698" t="s">
         <v>216</v>
       </c>
       <c r="U5" s="8"/>
@@ -15008,32 +15341,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="2526" t="s">
+      <c r="C6" s="2637" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="2534" t="s">
+      <c r="D6" s="2645" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2541" t="s">
+      <c r="E6" s="2652" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="2548" t="s">
+      <c r="F6" s="2659" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="2556" t="s">
+      <c r="G6" s="2667" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="2564" t="s">
+      <c r="H6" s="2675" t="s">
         <v>193</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="2572" t="s">
+      <c r="J6" s="2683" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="2580" t="s">
+      <c r="K6" s="2691" t="s">
         <v>209</v>
       </c>
-      <c r="L6" s="2588" t="s">
+      <c r="L6" s="2699" t="s">
         <v>217</v>
       </c>
       <c r="U6" s="8"/>
@@ -15047,32 +15380,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="2527" t="s">
+      <c r="C7" s="2638" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="2535" t="s">
+      <c r="D7" s="2646" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="2542" t="s">
+      <c r="E7" s="2653" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="2549" t="s">
+      <c r="F7" s="2660" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="2557" t="s">
+      <c r="G7" s="2668" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="2565" t="s">
+      <c r="H7" s="2676" t="s">
         <v>194</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="2573" t="s">
+      <c r="J7" s="2684" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="2581" t="s">
+      <c r="K7" s="2692" t="s">
         <v>210</v>
       </c>
-      <c r="L7" s="2589" t="s">
+      <c r="L7" s="2700" t="s">
         <v>218</v>
       </c>
       <c r="U7" s="8"/>
@@ -15086,30 +15419,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="2528" t="s">
+      <c r="C8" s="2639" t="s">
         <v>230</v>
       </c>
-      <c r="D8" s="2536" t="s">
+      <c r="D8" s="2647" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="2550" t="s">
+      <c r="F8" s="2661" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="2558" t="s">
+      <c r="G8" s="2669" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="2566" t="s">
+      <c r="H8" s="2677" t="s">
         <v>195</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="2574" t="s">
+      <c r="J8" s="2685" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="2582" t="s">
+      <c r="K8" s="2693" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="2590" t="s">
+      <c r="L8" s="2701" t="s">
         <v>219</v>
       </c>
       <c r="U8" s="8"/>
@@ -15123,32 +15456,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="2529" t="s">
+      <c r="C9" s="2640" t="s">
         <v>230</v>
       </c>
-      <c r="D9" s="2537" t="s">
+      <c r="D9" s="2648" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="2543" t="s">
+      <c r="E9" s="2654" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="2551" t="s">
+      <c r="F9" s="2662" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="2559" t="s">
+      <c r="G9" s="2670" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="2567" t="s">
+      <c r="H9" s="2678" t="s">
         <v>196</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="2575" t="s">
+      <c r="J9" s="2686" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="2583" t="s">
+      <c r="K9" s="2694" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="2591" t="s">
+      <c r="L9" s="2702" t="s">
         <v>220</v>
       </c>
       <c r="U9" s="8"/>
@@ -15162,32 +15495,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="2530" t="s">
+      <c r="C10" s="2641" t="s">
         <v>230</v>
       </c>
-      <c r="D10" s="2538" t="s">
+      <c r="D10" s="2649" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="2544" t="s">
+      <c r="E10" s="2655" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="2552" t="s">
+      <c r="F10" s="2663" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="2560" t="s">
+      <c r="G10" s="2671" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="2568" t="s">
+      <c r="H10" s="2679" t="s">
         <v>197</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="2576" t="s">
+      <c r="J10" s="2687" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="2584" t="s">
+      <c r="K10" s="2695" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="2592" t="s">
+      <c r="L10" s="2703" t="s">
         <v>221</v>
       </c>
       <c r="U10" s="8"/>
@@ -34677,34 +35010,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2593" t="s">
+      <c r="A3" s="2704" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="2595" t="s">
+      <c r="D3" s="2706" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="2597" t="s">
+      <c r="E3" s="2708" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="2599" t="s">
+      <c r="F3" s="2710" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="2594">
+      <c r="A4" t="s" s="2705">
         <v>223</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="2596">
+      <c r="D4" t="s" s="2707">
         <v>225</v>
       </c>
-      <c r="E4" t="s" s="2598">
+      <c r="E4" t="s" s="2709">
         <v>227</v>
       </c>
-      <c r="F4" t="s" s="2600">
+      <c r="F4" t="s" s="2711">
         <v>229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-06 18:49:00]  updated to US standards alignment"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3007" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3118" uniqueCount="232">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1224,7 +1224,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2712">
+  <cellXfs count="2823">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1337,6 +1337,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -12413,44 +12746,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="2601" t="s">
+      <c r="A3" s="2712" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2603" t="s">
+      <c r="B3" s="2714" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="2605" t="s">
+      <c r="C3" s="2716" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2607" t="s">
+      <c r="D3" s="2718" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="2609" t="s">
+      <c r="E3" s="2720" t="s">
         <v>162</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="2611" t="s">
+      <c r="G3" s="2722" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2602" t="s">
+      <c r="A4" s="2713" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2604" t="s">
+      <c r="B4" s="2715" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2606" t="s">
+      <c r="C4" s="2717" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2608" t="s">
+      <c r="D4" s="2719" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="2610" t="s">
+      <c r="E4" s="2721" t="s">
         <v>163</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="2612" t="s">
+      <c r="G4" s="2723" t="s">
         <v>165</v>
       </c>
     </row>
@@ -13607,81 +13940,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2613" t="s">
+      <c r="C3" s="2724" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="2616" t="s">
+      <c r="D3" s="2727" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2619" t="s">
+      <c r="E3" s="2730" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="2622" t="s">
+      <c r="F3" s="2733" t="s">
         <v>169</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="2625" t="s">
+      <c r="H3" s="2736" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="2628" t="s">
+      <c r="I3" s="2739" t="s">
         <v>175</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="2631" t="s">
+      <c r="K3" s="2742" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2614" t="s">
+      <c r="C4" s="2725" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="2617" t="s">
+      <c r="D4" s="2728" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="2620" t="s">
+      <c r="E4" s="2731" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="2623" t="s">
+      <c r="F4" s="2734" t="s">
         <v>170</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="2626" t="s">
+      <c r="H4" s="2737" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="2629" t="s">
+      <c r="I4" s="2740" t="s">
         <v>176</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="2632" t="s">
+      <c r="K4" s="2743" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2615" t="s">
+      <c r="C5" s="2726" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="2618" t="s">
+      <c r="D5" s="2729" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="2621" t="s">
+      <c r="E5" s="2732" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="2624" t="s">
+      <c r="F5" s="2735" t="s">
         <v>171</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="2627" t="s">
+      <c r="H5" s="2738" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="2630" t="s">
+      <c r="I5" s="2741" t="s">
         <v>177</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="2633" t="s">
+      <c r="K5" s="2744" t="s">
         <v>180</v>
       </c>
     </row>
@@ -15226,32 +15559,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2634" t="s">
+      <c r="C3" s="2745" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="2642" t="s">
+      <c r="D3" s="2753" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2650" t="s">
+      <c r="E3" s="2761" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="2656" t="s">
+      <c r="F3" s="2767" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="2664" t="s">
+      <c r="G3" s="2775" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="2672" t="s">
+      <c r="H3" s="2783" t="s">
         <v>190</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="2680" t="s">
+      <c r="J3" s="2791" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="2688" t="s">
+      <c r="K3" s="2799" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="2696" t="s">
+      <c r="L3" s="2807" t="s">
         <v>214</v>
       </c>
       <c r="U3" s="8"/>
@@ -15265,32 +15598,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2635" t="s">
+      <c r="C4" s="2746" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="2643" t="s">
+      <c r="D4" s="2754" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="2651" t="s">
+      <c r="E4" s="2762" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="2657" t="s">
+      <c r="F4" s="2768" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="2665" t="s">
+      <c r="G4" s="2776" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="2673" t="s">
+      <c r="H4" s="2784" t="s">
         <v>191</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="2681" t="s">
+      <c r="J4" s="2792" t="s">
         <v>199</v>
       </c>
-      <c r="K4" s="2689" t="s">
+      <c r="K4" s="2800" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="2697" t="s">
+      <c r="L4" s="2808" t="s">
         <v>215</v>
       </c>
       <c r="U4" s="8"/>
@@ -15304,30 +15637,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2636" t="s">
+      <c r="C5" s="2747" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="2644" t="s">
+      <c r="D5" s="2755" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="2658" t="s">
+      <c r="F5" s="2769" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="2666" t="s">
+      <c r="G5" s="2777" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="2674" t="s">
+      <c r="H5" s="2785" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="2682" t="s">
+      <c r="J5" s="2793" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="2690" t="s">
+      <c r="K5" s="2801" t="s">
         <v>208</v>
       </c>
-      <c r="L5" s="2698" t="s">
+      <c r="L5" s="2809" t="s">
         <v>216</v>
       </c>
       <c r="U5" s="8"/>
@@ -15341,32 +15674,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="2637" t="s">
+      <c r="C6" s="2748" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="2645" t="s">
+      <c r="D6" s="2756" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2652" t="s">
+      <c r="E6" s="2763" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="2659" t="s">
+      <c r="F6" s="2770" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="2667" t="s">
+      <c r="G6" s="2778" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="2675" t="s">
+      <c r="H6" s="2786" t="s">
         <v>193</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="2683" t="s">
+      <c r="J6" s="2794" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="2691" t="s">
+      <c r="K6" s="2802" t="s">
         <v>209</v>
       </c>
-      <c r="L6" s="2699" t="s">
+      <c r="L6" s="2810" t="s">
         <v>217</v>
       </c>
       <c r="U6" s="8"/>
@@ -15380,32 +15713,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="2638" t="s">
+      <c r="C7" s="2749" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="2646" t="s">
+      <c r="D7" s="2757" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="2653" t="s">
+      <c r="E7" s="2764" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="2660" t="s">
+      <c r="F7" s="2771" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="2668" t="s">
+      <c r="G7" s="2779" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="2676" t="s">
+      <c r="H7" s="2787" t="s">
         <v>194</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="2684" t="s">
+      <c r="J7" s="2795" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="2692" t="s">
+      <c r="K7" s="2803" t="s">
         <v>210</v>
       </c>
-      <c r="L7" s="2700" t="s">
+      <c r="L7" s="2811" t="s">
         <v>218</v>
       </c>
       <c r="U7" s="8"/>
@@ -15419,30 +15752,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="2639" t="s">
+      <c r="C8" s="2750" t="s">
         <v>230</v>
       </c>
-      <c r="D8" s="2647" t="s">
+      <c r="D8" s="2758" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="2661" t="s">
+      <c r="F8" s="2772" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="2669" t="s">
+      <c r="G8" s="2780" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="2677" t="s">
+      <c r="H8" s="2788" t="s">
         <v>195</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="2685" t="s">
+      <c r="J8" s="2796" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="2693" t="s">
+      <c r="K8" s="2804" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="2701" t="s">
+      <c r="L8" s="2812" t="s">
         <v>219</v>
       </c>
       <c r="U8" s="8"/>
@@ -15456,32 +15789,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="2640" t="s">
+      <c r="C9" s="2751" t="s">
         <v>230</v>
       </c>
-      <c r="D9" s="2648" t="s">
+      <c r="D9" s="2759" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="2654" t="s">
+      <c r="E9" s="2765" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="2662" t="s">
+      <c r="F9" s="2773" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="2670" t="s">
+      <c r="G9" s="2781" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="2678" t="s">
+      <c r="H9" s="2789" t="s">
         <v>196</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="2686" t="s">
+      <c r="J9" s="2797" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="2694" t="s">
+      <c r="K9" s="2805" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="2702" t="s">
+      <c r="L9" s="2813" t="s">
         <v>220</v>
       </c>
       <c r="U9" s="8"/>
@@ -15495,32 +15828,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="2641" t="s">
+      <c r="C10" s="2752" t="s">
         <v>230</v>
       </c>
-      <c r="D10" s="2649" t="s">
+      <c r="D10" s="2760" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="2655" t="s">
+      <c r="E10" s="2766" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="2663" t="s">
+      <c r="F10" s="2774" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="2671" t="s">
+      <c r="G10" s="2782" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="2679" t="s">
+      <c r="H10" s="2790" t="s">
         <v>197</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="2687" t="s">
+      <c r="J10" s="2798" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="2695" t="s">
+      <c r="K10" s="2806" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="2703" t="s">
+      <c r="L10" s="2814" t="s">
         <v>221</v>
       </c>
       <c r="U10" s="8"/>
@@ -35010,34 +35343,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2704" t="s">
+      <c r="A3" s="2815" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="2706" t="s">
+      <c r="D3" s="2817" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="2708" t="s">
+      <c r="E3" s="2819" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="2710" t="s">
+      <c r="F3" s="2821" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="2705">
+      <c r="A4" t="s" s="2816">
         <v>223</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="2707">
+      <c r="D4" t="s" s="2818">
         <v>225</v>
       </c>
-      <c r="E4" t="s" s="2709">
+      <c r="E4" t="s" s="2820">
         <v>227</v>
       </c>
-      <c r="F4" t="s" s="2711">
+      <c r="F4" t="s" s="2822">
         <v>229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-06 21:29:41]  add learning chart?"
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3118" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3229" uniqueCount="232">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1224,7 +1224,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2823">
+  <cellXfs count="2934">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1337,6 +1337,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -12746,44 +13079,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="2712" t="s">
+      <c r="A3" s="2823" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2714" t="s">
+      <c r="B3" s="2825" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="2716" t="s">
+      <c r="C3" s="2827" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2718" t="s">
+      <c r="D3" s="2829" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="2720" t="s">
+      <c r="E3" s="2831" t="s">
         <v>162</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="2722" t="s">
+      <c r="G3" s="2833" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2713" t="s">
+      <c r="A4" s="2824" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2715" t="s">
+      <c r="B4" s="2826" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2717" t="s">
+      <c r="C4" s="2828" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2719" t="s">
+      <c r="D4" s="2830" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="2721" t="s">
+      <c r="E4" s="2832" t="s">
         <v>163</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="2723" t="s">
+      <c r="G4" s="2834" t="s">
         <v>165</v>
       </c>
     </row>
@@ -13940,81 +14273,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2724" t="s">
+      <c r="C3" s="2835" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="2727" t="s">
+      <c r="D3" s="2838" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2730" t="s">
+      <c r="E3" s="2841" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="2733" t="s">
+      <c r="F3" s="2844" t="s">
         <v>169</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="2736" t="s">
+      <c r="H3" s="2847" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="2739" t="s">
+      <c r="I3" s="2850" t="s">
         <v>175</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="2742" t="s">
+      <c r="K3" s="2853" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2725" t="s">
+      <c r="C4" s="2836" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="2728" t="s">
+      <c r="D4" s="2839" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="2731" t="s">
+      <c r="E4" s="2842" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="2734" t="s">
+      <c r="F4" s="2845" t="s">
         <v>170</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="2737" t="s">
+      <c r="H4" s="2848" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="2740" t="s">
+      <c r="I4" s="2851" t="s">
         <v>176</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="2743" t="s">
+      <c r="K4" s="2854" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2726" t="s">
+      <c r="C5" s="2837" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="2729" t="s">
+      <c r="D5" s="2840" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="2732" t="s">
+      <c r="E5" s="2843" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="2735" t="s">
+      <c r="F5" s="2846" t="s">
         <v>171</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="2738" t="s">
+      <c r="H5" s="2849" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="2741" t="s">
+      <c r="I5" s="2852" t="s">
         <v>177</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="2744" t="s">
+      <c r="K5" s="2855" t="s">
         <v>180</v>
       </c>
     </row>
@@ -15559,32 +15892,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2745" t="s">
+      <c r="C3" s="2856" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="2753" t="s">
+      <c r="D3" s="2864" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2761" t="s">
+      <c r="E3" s="2872" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="2767" t="s">
+      <c r="F3" s="2878" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="2775" t="s">
+      <c r="G3" s="2886" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="2783" t="s">
+      <c r="H3" s="2894" t="s">
         <v>190</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="2791" t="s">
+      <c r="J3" s="2902" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="2799" t="s">
+      <c r="K3" s="2910" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="2807" t="s">
+      <c r="L3" s="2918" t="s">
         <v>214</v>
       </c>
       <c r="U3" s="8"/>
@@ -15598,32 +15931,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2746" t="s">
+      <c r="C4" s="2857" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="2754" t="s">
+      <c r="D4" s="2865" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="2762" t="s">
+      <c r="E4" s="2873" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="2768" t="s">
+      <c r="F4" s="2879" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="2776" t="s">
+      <c r="G4" s="2887" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="2784" t="s">
+      <c r="H4" s="2895" t="s">
         <v>191</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="2792" t="s">
+      <c r="J4" s="2903" t="s">
         <v>199</v>
       </c>
-      <c r="K4" s="2800" t="s">
+      <c r="K4" s="2911" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="2808" t="s">
+      <c r="L4" s="2919" t="s">
         <v>215</v>
       </c>
       <c r="U4" s="8"/>
@@ -15637,30 +15970,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2747" t="s">
+      <c r="C5" s="2858" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="2755" t="s">
+      <c r="D5" s="2866" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="2769" t="s">
+      <c r="F5" s="2880" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="2777" t="s">
+      <c r="G5" s="2888" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="2785" t="s">
+      <c r="H5" s="2896" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="2793" t="s">
+      <c r="J5" s="2904" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="2801" t="s">
+      <c r="K5" s="2912" t="s">
         <v>208</v>
       </c>
-      <c r="L5" s="2809" t="s">
+      <c r="L5" s="2920" t="s">
         <v>216</v>
       </c>
       <c r="U5" s="8"/>
@@ -15674,32 +16007,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="2748" t="s">
+      <c r="C6" s="2859" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="2756" t="s">
+      <c r="D6" s="2867" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2763" t="s">
+      <c r="E6" s="2874" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="2770" t="s">
+      <c r="F6" s="2881" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="2778" t="s">
+      <c r="G6" s="2889" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="2786" t="s">
+      <c r="H6" s="2897" t="s">
         <v>193</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="2794" t="s">
+      <c r="J6" s="2905" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="2802" t="s">
+      <c r="K6" s="2913" t="s">
         <v>209</v>
       </c>
-      <c r="L6" s="2810" t="s">
+      <c r="L6" s="2921" t="s">
         <v>217</v>
       </c>
       <c r="U6" s="8"/>
@@ -15713,32 +16046,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="2749" t="s">
+      <c r="C7" s="2860" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="2757" t="s">
+      <c r="D7" s="2868" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="2764" t="s">
+      <c r="E7" s="2875" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="2771" t="s">
+      <c r="F7" s="2882" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="2779" t="s">
+      <c r="G7" s="2890" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="2787" t="s">
+      <c r="H7" s="2898" t="s">
         <v>194</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="2795" t="s">
+      <c r="J7" s="2906" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="2803" t="s">
+      <c r="K7" s="2914" t="s">
         <v>210</v>
       </c>
-      <c r="L7" s="2811" t="s">
+      <c r="L7" s="2922" t="s">
         <v>218</v>
       </c>
       <c r="U7" s="8"/>
@@ -15752,30 +16085,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="2750" t="s">
+      <c r="C8" s="2861" t="s">
         <v>230</v>
       </c>
-      <c r="D8" s="2758" t="s">
+      <c r="D8" s="2869" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="2772" t="s">
+      <c r="F8" s="2883" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="2780" t="s">
+      <c r="G8" s="2891" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="2788" t="s">
+      <c r="H8" s="2899" t="s">
         <v>195</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="2796" t="s">
+      <c r="J8" s="2907" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="2804" t="s">
+      <c r="K8" s="2915" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="2812" t="s">
+      <c r="L8" s="2923" t="s">
         <v>219</v>
       </c>
       <c r="U8" s="8"/>
@@ -15789,32 +16122,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="2751" t="s">
+      <c r="C9" s="2862" t="s">
         <v>230</v>
       </c>
-      <c r="D9" s="2759" t="s">
+      <c r="D9" s="2870" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="2765" t="s">
+      <c r="E9" s="2876" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="2773" t="s">
+      <c r="F9" s="2884" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="2781" t="s">
+      <c r="G9" s="2892" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="2789" t="s">
+      <c r="H9" s="2900" t="s">
         <v>196</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="2797" t="s">
+      <c r="J9" s="2908" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="2805" t="s">
+      <c r="K9" s="2916" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="2813" t="s">
+      <c r="L9" s="2924" t="s">
         <v>220</v>
       </c>
       <c r="U9" s="8"/>
@@ -15828,32 +16161,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="2752" t="s">
+      <c r="C10" s="2863" t="s">
         <v>230</v>
       </c>
-      <c r="D10" s="2760" t="s">
+      <c r="D10" s="2871" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="2766" t="s">
+      <c r="E10" s="2877" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="2774" t="s">
+      <c r="F10" s="2885" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="2782" t="s">
+      <c r="G10" s="2893" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="2790" t="s">
+      <c r="H10" s="2901" t="s">
         <v>197</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="2798" t="s">
+      <c r="J10" s="2909" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="2806" t="s">
+      <c r="K10" s="2917" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="2814" t="s">
+      <c r="L10" s="2925" t="s">
         <v>221</v>
       </c>
       <c r="U10" s="8"/>
@@ -35343,34 +35676,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2815" t="s">
+      <c r="A3" s="2926" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="2817" t="s">
+      <c r="D3" s="2928" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="2819" t="s">
+      <c r="E3" s="2930" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="2821" t="s">
+      <c r="F3" s="2932" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="2816">
+      <c r="A4" t="s" s="2927">
         <v>223</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="2818">
+      <c r="D4" t="s" s="2929">
         <v>225</v>
       </c>
-      <c r="E4" t="s" s="2820">
+      <c r="E4" t="s" s="2931">
         <v>227</v>
       </c>
-      <c r="F4" t="s" s="2822">
+      <c r="F4" t="s" s="2933">
         <v>229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-08 21:51:35] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3229" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="232">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1224,7 +1224,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2934">
+  <cellXfs count="3267">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1337,6 +1337,1005 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -13079,44 +14078,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="2823" t="s">
+      <c r="A3" s="3156" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2825" t="s">
+      <c r="B3" s="3158" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="2827" t="s">
+      <c r="C3" s="3160" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2829" t="s">
+      <c r="D3" s="3162" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="2831" t="s">
+      <c r="E3" s="3164" t="s">
         <v>162</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="2833" t="s">
+      <c r="G3" s="3166" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2824" t="s">
+      <c r="A4" s="3157" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2826" t="s">
+      <c r="B4" s="3159" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2828" t="s">
+      <c r="C4" s="3161" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="2830" t="s">
+      <c r="D4" s="3163" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="2832" t="s">
+      <c r="E4" s="3165" t="s">
         <v>163</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="2834" t="s">
+      <c r="G4" s="3167" t="s">
         <v>165</v>
       </c>
     </row>
@@ -14273,81 +15272,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2835" t="s">
+      <c r="C3" s="3168" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="2838" t="s">
+      <c r="D3" s="3171" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2841" t="s">
+      <c r="E3" s="3174" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="2844" t="s">
+      <c r="F3" s="3177" t="s">
         <v>169</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="2847" t="s">
+      <c r="H3" s="3180" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="2850" t="s">
+      <c r="I3" s="3183" t="s">
         <v>175</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="2853" t="s">
+      <c r="K3" s="3186" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2836" t="s">
+      <c r="C4" s="3169" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="2839" t="s">
+      <c r="D4" s="3172" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="2842" t="s">
+      <c r="E4" s="3175" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="2845" t="s">
+      <c r="F4" s="3178" t="s">
         <v>170</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="2848" t="s">
+      <c r="H4" s="3181" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="2851" t="s">
+      <c r="I4" s="3184" t="s">
         <v>176</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="2854" t="s">
+      <c r="K4" s="3187" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2837" t="s">
+      <c r="C5" s="3170" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="2840" t="s">
+      <c r="D5" s="3173" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="2843" t="s">
+      <c r="E5" s="3176" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="2846" t="s">
+      <c r="F5" s="3179" t="s">
         <v>171</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="2849" t="s">
+      <c r="H5" s="3182" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="2852" t="s">
+      <c r="I5" s="3185" t="s">
         <v>177</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="2855" t="s">
+      <c r="K5" s="3188" t="s">
         <v>180</v>
       </c>
     </row>
@@ -15892,32 +16891,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="2856" t="s">
+      <c r="C3" s="3189" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="2864" t="s">
+      <c r="D3" s="3197" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="2872" t="s">
+      <c r="E3" s="3205" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="2878" t="s">
+      <c r="F3" s="3211" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="2886" t="s">
+      <c r="G3" s="3219" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="2894" t="s">
+      <c r="H3" s="3227" t="s">
         <v>190</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="2902" t="s">
+      <c r="J3" s="3235" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="2910" t="s">
+      <c r="K3" s="3243" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="2918" t="s">
+      <c r="L3" s="3251" t="s">
         <v>214</v>
       </c>
       <c r="U3" s="8"/>
@@ -15931,32 +16930,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="2857" t="s">
+      <c r="C4" s="3190" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="2865" t="s">
+      <c r="D4" s="3198" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="2873" t="s">
+      <c r="E4" s="3206" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="2879" t="s">
+      <c r="F4" s="3212" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="2887" t="s">
+      <c r="G4" s="3220" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="2895" t="s">
+      <c r="H4" s="3228" t="s">
         <v>191</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="2903" t="s">
+      <c r="J4" s="3236" t="s">
         <v>199</v>
       </c>
-      <c r="K4" s="2911" t="s">
+      <c r="K4" s="3244" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="2919" t="s">
+      <c r="L4" s="3252" t="s">
         <v>215</v>
       </c>
       <c r="U4" s="8"/>
@@ -15970,30 +16969,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="2858" t="s">
+      <c r="C5" s="3191" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="2866" t="s">
+      <c r="D5" s="3199" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="2880" t="s">
+      <c r="F5" s="3213" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="2888" t="s">
+      <c r="G5" s="3221" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="2896" t="s">
+      <c r="H5" s="3229" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="2904" t="s">
+      <c r="J5" s="3237" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="2912" t="s">
+      <c r="K5" s="3245" t="s">
         <v>208</v>
       </c>
-      <c r="L5" s="2920" t="s">
+      <c r="L5" s="3253" t="s">
         <v>216</v>
       </c>
       <c r="U5" s="8"/>
@@ -16007,32 +17006,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="2859" t="s">
+      <c r="C6" s="3192" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="2867" t="s">
+      <c r="D6" s="3200" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="2874" t="s">
+      <c r="E6" s="3207" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="2881" t="s">
+      <c r="F6" s="3214" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="2889" t="s">
+      <c r="G6" s="3222" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="2897" t="s">
+      <c r="H6" s="3230" t="s">
         <v>193</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="2905" t="s">
+      <c r="J6" s="3238" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="2913" t="s">
+      <c r="K6" s="3246" t="s">
         <v>209</v>
       </c>
-      <c r="L6" s="2921" t="s">
+      <c r="L6" s="3254" t="s">
         <v>217</v>
       </c>
       <c r="U6" s="8"/>
@@ -16046,32 +17045,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="2860" t="s">
+      <c r="C7" s="3193" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="2868" t="s">
+      <c r="D7" s="3201" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="2875" t="s">
+      <c r="E7" s="3208" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="2882" t="s">
+      <c r="F7" s="3215" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="2890" t="s">
+      <c r="G7" s="3223" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="2898" t="s">
+      <c r="H7" s="3231" t="s">
         <v>194</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="2906" t="s">
+      <c r="J7" s="3239" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="2914" t="s">
+      <c r="K7" s="3247" t="s">
         <v>210</v>
       </c>
-      <c r="L7" s="2922" t="s">
+      <c r="L7" s="3255" t="s">
         <v>218</v>
       </c>
       <c r="U7" s="8"/>
@@ -16085,30 +17084,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="2861" t="s">
+      <c r="C8" s="3194" t="s">
         <v>230</v>
       </c>
-      <c r="D8" s="2869" t="s">
+      <c r="D8" s="3202" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="2883" t="s">
+      <c r="F8" s="3216" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="2891" t="s">
+      <c r="G8" s="3224" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="2899" t="s">
+      <c r="H8" s="3232" t="s">
         <v>195</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="2907" t="s">
+      <c r="J8" s="3240" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="2915" t="s">
+      <c r="K8" s="3248" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="2923" t="s">
+      <c r="L8" s="3256" t="s">
         <v>219</v>
       </c>
       <c r="U8" s="8"/>
@@ -16122,32 +17121,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="2862" t="s">
+      <c r="C9" s="3195" t="s">
         <v>230</v>
       </c>
-      <c r="D9" s="2870" t="s">
+      <c r="D9" s="3203" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="2876" t="s">
+      <c r="E9" s="3209" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="2884" t="s">
+      <c r="F9" s="3217" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="2892" t="s">
+      <c r="G9" s="3225" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="2900" t="s">
+      <c r="H9" s="3233" t="s">
         <v>196</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="2908" t="s">
+      <c r="J9" s="3241" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="2916" t="s">
+      <c r="K9" s="3249" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="2924" t="s">
+      <c r="L9" s="3257" t="s">
         <v>220</v>
       </c>
       <c r="U9" s="8"/>
@@ -16161,32 +17160,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="2863" t="s">
+      <c r="C10" s="3196" t="s">
         <v>230</v>
       </c>
-      <c r="D10" s="2871" t="s">
+      <c r="D10" s="3204" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="2877" t="s">
+      <c r="E10" s="3210" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="2885" t="s">
+      <c r="F10" s="3218" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="2893" t="s">
+      <c r="G10" s="3226" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="2901" t="s">
+      <c r="H10" s="3234" t="s">
         <v>197</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="2909" t="s">
+      <c r="J10" s="3242" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="2917" t="s">
+      <c r="K10" s="3250" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="2925" t="s">
+      <c r="L10" s="3258" t="s">
         <v>221</v>
       </c>
       <c r="U10" s="8"/>
@@ -35676,34 +36675,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2926" t="s">
+      <c r="A3" s="3259" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="2928" t="s">
+      <c r="D3" s="3261" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="2930" t="s">
+      <c r="E3" s="3263" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="2932" t="s">
+      <c r="F3" s="3265" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="2927">
+      <c r="A4" t="s" s="3260">
         <v>223</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="2929">
+      <c r="D4" t="s" s="3262">
         <v>225</v>
       </c>
-      <c r="E4" t="s" s="2931">
+      <c r="E4" t="s" s="3264">
         <v>227</v>
       </c>
-      <c r="F4" t="s" s="2933">
+      <c r="F4" t="s" s="3266">
         <v>229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-08 23:19:17] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3562" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3673" uniqueCount="232">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1224,7 +1224,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3267">
+  <cellXfs count="3378">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1337,6 +1337,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -14078,44 +14411,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="3156" t="s">
+      <c r="A3" s="3267" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3158" t="s">
+      <c r="B3" s="3269" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="3160" t="s">
+      <c r="C3" s="3271" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3162" t="s">
+      <c r="D3" s="3273" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="3164" t="s">
+      <c r="E3" s="3275" t="s">
         <v>162</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="3166" t="s">
+      <c r="G3" s="3277" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3157" t="s">
+      <c r="A4" s="3268" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3159" t="s">
+      <c r="B4" s="3270" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3161" t="s">
+      <c r="C4" s="3272" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3163" t="s">
+      <c r="D4" s="3274" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="3165" t="s">
+      <c r="E4" s="3276" t="s">
         <v>163</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="3167" t="s">
+      <c r="G4" s="3278" t="s">
         <v>165</v>
       </c>
     </row>
@@ -15272,81 +15605,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="3168" t="s">
+      <c r="C3" s="3279" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="3171" t="s">
+      <c r="D3" s="3282" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3174" t="s">
+      <c r="E3" s="3285" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="3177" t="s">
+      <c r="F3" s="3288" t="s">
         <v>169</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="3180" t="s">
+      <c r="H3" s="3291" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="3183" t="s">
+      <c r="I3" s="3294" t="s">
         <v>175</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="3186" t="s">
+      <c r="K3" s="3297" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="3169" t="s">
+      <c r="C4" s="3280" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="3172" t="s">
+      <c r="D4" s="3283" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="3175" t="s">
+      <c r="E4" s="3286" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="3178" t="s">
+      <c r="F4" s="3289" t="s">
         <v>170</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="3181" t="s">
+      <c r="H4" s="3292" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="3184" t="s">
+      <c r="I4" s="3295" t="s">
         <v>176</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="3187" t="s">
+      <c r="K4" s="3298" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="3170" t="s">
+      <c r="C5" s="3281" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="3173" t="s">
+      <c r="D5" s="3284" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="3176" t="s">
+      <c r="E5" s="3287" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="3179" t="s">
+      <c r="F5" s="3290" t="s">
         <v>171</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="3182" t="s">
+      <c r="H5" s="3293" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="3185" t="s">
+      <c r="I5" s="3296" t="s">
         <v>177</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="3188" t="s">
+      <c r="K5" s="3299" t="s">
         <v>180</v>
       </c>
     </row>
@@ -16891,32 +17224,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="3189" t="s">
+      <c r="C3" s="3300" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="3197" t="s">
+      <c r="D3" s="3308" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3205" t="s">
+      <c r="E3" s="3316" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="3211" t="s">
+      <c r="F3" s="3322" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="3219" t="s">
+      <c r="G3" s="3330" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="3227" t="s">
+      <c r="H3" s="3338" t="s">
         <v>190</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="3235" t="s">
+      <c r="J3" s="3346" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="3243" t="s">
+      <c r="K3" s="3354" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="3251" t="s">
+      <c r="L3" s="3362" t="s">
         <v>214</v>
       </c>
       <c r="U3" s="8"/>
@@ -16930,32 +17263,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="3190" t="s">
+      <c r="C4" s="3301" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="3198" t="s">
+      <c r="D4" s="3309" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="3206" t="s">
+      <c r="E4" s="3317" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="3212" t="s">
+      <c r="F4" s="3323" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="3220" t="s">
+      <c r="G4" s="3331" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="3228" t="s">
+      <c r="H4" s="3339" t="s">
         <v>191</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="3236" t="s">
+      <c r="J4" s="3347" t="s">
         <v>199</v>
       </c>
-      <c r="K4" s="3244" t="s">
+      <c r="K4" s="3355" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="3252" t="s">
+      <c r="L4" s="3363" t="s">
         <v>215</v>
       </c>
       <c r="U4" s="8"/>
@@ -16969,30 +17302,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="3191" t="s">
+      <c r="C5" s="3302" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="3199" t="s">
+      <c r="D5" s="3310" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="3213" t="s">
+      <c r="F5" s="3324" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="3221" t="s">
+      <c r="G5" s="3332" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="3229" t="s">
+      <c r="H5" s="3340" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="3237" t="s">
+      <c r="J5" s="3348" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="3245" t="s">
+      <c r="K5" s="3356" t="s">
         <v>208</v>
       </c>
-      <c r="L5" s="3253" t="s">
+      <c r="L5" s="3364" t="s">
         <v>216</v>
       </c>
       <c r="U5" s="8"/>
@@ -17006,32 +17339,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="3192" t="s">
+      <c r="C6" s="3303" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="3200" t="s">
+      <c r="D6" s="3311" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="3207" t="s">
+      <c r="E6" s="3318" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="3214" t="s">
+      <c r="F6" s="3325" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="3222" t="s">
+      <c r="G6" s="3333" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="3230" t="s">
+      <c r="H6" s="3341" t="s">
         <v>193</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="3238" t="s">
+      <c r="J6" s="3349" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="3246" t="s">
+      <c r="K6" s="3357" t="s">
         <v>209</v>
       </c>
-      <c r="L6" s="3254" t="s">
+      <c r="L6" s="3365" t="s">
         <v>217</v>
       </c>
       <c r="U6" s="8"/>
@@ -17045,32 +17378,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="3193" t="s">
+      <c r="C7" s="3304" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="3201" t="s">
+      <c r="D7" s="3312" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="3208" t="s">
+      <c r="E7" s="3319" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="3215" t="s">
+      <c r="F7" s="3326" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="3223" t="s">
+      <c r="G7" s="3334" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="3231" t="s">
+      <c r="H7" s="3342" t="s">
         <v>194</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="3239" t="s">
+      <c r="J7" s="3350" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="3247" t="s">
+      <c r="K7" s="3358" t="s">
         <v>210</v>
       </c>
-      <c r="L7" s="3255" t="s">
+      <c r="L7" s="3366" t="s">
         <v>218</v>
       </c>
       <c r="U7" s="8"/>
@@ -17084,30 +17417,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="3194" t="s">
+      <c r="C8" s="3305" t="s">
         <v>230</v>
       </c>
-      <c r="D8" s="3202" t="s">
+      <c r="D8" s="3313" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="3216" t="s">
+      <c r="F8" s="3327" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="3224" t="s">
+      <c r="G8" s="3335" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="3232" t="s">
+      <c r="H8" s="3343" t="s">
         <v>195</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="3240" t="s">
+      <c r="J8" s="3351" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="3248" t="s">
+      <c r="K8" s="3359" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="3256" t="s">
+      <c r="L8" s="3367" t="s">
         <v>219</v>
       </c>
       <c r="U8" s="8"/>
@@ -17121,32 +17454,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="3195" t="s">
+      <c r="C9" s="3306" t="s">
         <v>230</v>
       </c>
-      <c r="D9" s="3203" t="s">
+      <c r="D9" s="3314" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="3209" t="s">
+      <c r="E9" s="3320" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="3217" t="s">
+      <c r="F9" s="3328" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="3225" t="s">
+      <c r="G9" s="3336" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="3233" t="s">
+      <c r="H9" s="3344" t="s">
         <v>196</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="3241" t="s">
+      <c r="J9" s="3352" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="3249" t="s">
+      <c r="K9" s="3360" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="3257" t="s">
+      <c r="L9" s="3368" t="s">
         <v>220</v>
       </c>
       <c r="U9" s="8"/>
@@ -17160,32 +17493,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="3196" t="s">
+      <c r="C10" s="3307" t="s">
         <v>230</v>
       </c>
-      <c r="D10" s="3204" t="s">
+      <c r="D10" s="3315" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="3210" t="s">
+      <c r="E10" s="3321" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="3218" t="s">
+      <c r="F10" s="3329" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="3226" t="s">
+      <c r="G10" s="3337" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="3234" t="s">
+      <c r="H10" s="3345" t="s">
         <v>197</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="3242" t="s">
+      <c r="J10" s="3353" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="3250" t="s">
+      <c r="K10" s="3361" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="3258" t="s">
+      <c r="L10" s="3369" t="s">
         <v>221</v>
       </c>
       <c r="U10" s="8"/>
@@ -36675,34 +37008,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3259" t="s">
+      <c r="A3" s="3370" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="3261" t="s">
+      <c r="D3" s="3372" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="3263" t="s">
+      <c r="E3" s="3374" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="3265" t="s">
+      <c r="F3" s="3376" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="3260">
+      <c r="A4" t="s" s="3371">
         <v>223</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="3262">
+      <c r="D4" t="s" s="3373">
         <v>225</v>
       </c>
-      <c r="E4" t="s" s="3264">
+      <c r="E4" t="s" s="3375">
         <v>227</v>
       </c>
-      <c r="F4" t="s" s="3266">
+      <c r="F4" t="s" s="3377">
         <v>229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-09 00:21:48] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3673" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3784" uniqueCount="232">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1224,7 +1224,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3378">
+  <cellXfs count="3489">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1337,6 +1337,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -14411,44 +14744,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="3267" t="s">
+      <c r="A3" s="3378" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3269" t="s">
+      <c r="B3" s="3380" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="3271" t="s">
+      <c r="C3" s="3382" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3273" t="s">
+      <c r="D3" s="3384" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="3275" t="s">
+      <c r="E3" s="3386" t="s">
         <v>162</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="3277" t="s">
+      <c r="G3" s="3388" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3268" t="s">
+      <c r="A4" s="3379" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3270" t="s">
+      <c r="B4" s="3381" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3272" t="s">
+      <c r="C4" s="3383" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3274" t="s">
+      <c r="D4" s="3385" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="3276" t="s">
+      <c r="E4" s="3387" t="s">
         <v>163</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="3278" t="s">
+      <c r="G4" s="3389" t="s">
         <v>165</v>
       </c>
     </row>
@@ -15605,81 +15938,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="3279" t="s">
+      <c r="C3" s="3390" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="3282" t="s">
+      <c r="D3" s="3393" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3285" t="s">
+      <c r="E3" s="3396" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="3288" t="s">
+      <c r="F3" s="3399" t="s">
         <v>169</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="3291" t="s">
+      <c r="H3" s="3402" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="3294" t="s">
+      <c r="I3" s="3405" t="s">
         <v>175</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="3297" t="s">
+      <c r="K3" s="3408" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="3280" t="s">
+      <c r="C4" s="3391" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="3283" t="s">
+      <c r="D4" s="3394" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="3286" t="s">
+      <c r="E4" s="3397" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="3289" t="s">
+      <c r="F4" s="3400" t="s">
         <v>170</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="3292" t="s">
+      <c r="H4" s="3403" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="3295" t="s">
+      <c r="I4" s="3406" t="s">
         <v>176</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="3298" t="s">
+      <c r="K4" s="3409" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="3281" t="s">
+      <c r="C5" s="3392" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="3284" t="s">
+      <c r="D5" s="3395" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="3287" t="s">
+      <c r="E5" s="3398" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="3290" t="s">
+      <c r="F5" s="3401" t="s">
         <v>171</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="3293" t="s">
+      <c r="H5" s="3404" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="3296" t="s">
+      <c r="I5" s="3407" t="s">
         <v>177</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="3299" t="s">
+      <c r="K5" s="3410" t="s">
         <v>180</v>
       </c>
     </row>
@@ -17224,32 +17557,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="3300" t="s">
+      <c r="C3" s="3411" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="3308" t="s">
+      <c r="D3" s="3419" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3316" t="s">
+      <c r="E3" s="3427" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="3322" t="s">
+      <c r="F3" s="3433" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="3330" t="s">
+      <c r="G3" s="3441" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="3338" t="s">
+      <c r="H3" s="3449" t="s">
         <v>190</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="3346" t="s">
+      <c r="J3" s="3457" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="3354" t="s">
+      <c r="K3" s="3465" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="3362" t="s">
+      <c r="L3" s="3473" t="s">
         <v>214</v>
       </c>
       <c r="U3" s="8"/>
@@ -17263,32 +17596,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="3301" t="s">
+      <c r="C4" s="3412" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="3309" t="s">
+      <c r="D4" s="3420" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="3317" t="s">
+      <c r="E4" s="3428" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="3323" t="s">
+      <c r="F4" s="3434" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="3331" t="s">
+      <c r="G4" s="3442" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="3339" t="s">
+      <c r="H4" s="3450" t="s">
         <v>191</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="3347" t="s">
+      <c r="J4" s="3458" t="s">
         <v>199</v>
       </c>
-      <c r="K4" s="3355" t="s">
+      <c r="K4" s="3466" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="3363" t="s">
+      <c r="L4" s="3474" t="s">
         <v>215</v>
       </c>
       <c r="U4" s="8"/>
@@ -17302,30 +17635,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="3302" t="s">
+      <c r="C5" s="3413" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="3310" t="s">
+      <c r="D5" s="3421" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="3324" t="s">
+      <c r="F5" s="3435" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="3332" t="s">
+      <c r="G5" s="3443" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="3340" t="s">
+      <c r="H5" s="3451" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="3348" t="s">
+      <c r="J5" s="3459" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="3356" t="s">
+      <c r="K5" s="3467" t="s">
         <v>208</v>
       </c>
-      <c r="L5" s="3364" t="s">
+      <c r="L5" s="3475" t="s">
         <v>216</v>
       </c>
       <c r="U5" s="8"/>
@@ -17339,32 +17672,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="3303" t="s">
+      <c r="C6" s="3414" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="3311" t="s">
+      <c r="D6" s="3422" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="3318" t="s">
+      <c r="E6" s="3429" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="3325" t="s">
+      <c r="F6" s="3436" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="3333" t="s">
+      <c r="G6" s="3444" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="3341" t="s">
+      <c r="H6" s="3452" t="s">
         <v>193</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="3349" t="s">
+      <c r="J6" s="3460" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="3357" t="s">
+      <c r="K6" s="3468" t="s">
         <v>209</v>
       </c>
-      <c r="L6" s="3365" t="s">
+      <c r="L6" s="3476" t="s">
         <v>217</v>
       </c>
       <c r="U6" s="8"/>
@@ -17378,32 +17711,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="3304" t="s">
+      <c r="C7" s="3415" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="3312" t="s">
+      <c r="D7" s="3423" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="3319" t="s">
+      <c r="E7" s="3430" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="3326" t="s">
+      <c r="F7" s="3437" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="3334" t="s">
+      <c r="G7" s="3445" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="3342" t="s">
+      <c r="H7" s="3453" t="s">
         <v>194</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="3350" t="s">
+      <c r="J7" s="3461" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="3358" t="s">
+      <c r="K7" s="3469" t="s">
         <v>210</v>
       </c>
-      <c r="L7" s="3366" t="s">
+      <c r="L7" s="3477" t="s">
         <v>218</v>
       </c>
       <c r="U7" s="8"/>
@@ -17417,30 +17750,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="3305" t="s">
+      <c r="C8" s="3416" t="s">
         <v>230</v>
       </c>
-      <c r="D8" s="3313" t="s">
+      <c r="D8" s="3424" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="3327" t="s">
+      <c r="F8" s="3438" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="3335" t="s">
+      <c r="G8" s="3446" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="3343" t="s">
+      <c r="H8" s="3454" t="s">
         <v>195</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="3351" t="s">
+      <c r="J8" s="3462" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="3359" t="s">
+      <c r="K8" s="3470" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="3367" t="s">
+      <c r="L8" s="3478" t="s">
         <v>219</v>
       </c>
       <c r="U8" s="8"/>
@@ -17454,32 +17787,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="3306" t="s">
+      <c r="C9" s="3417" t="s">
         <v>230</v>
       </c>
-      <c r="D9" s="3314" t="s">
+      <c r="D9" s="3425" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="3320" t="s">
+      <c r="E9" s="3431" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="3328" t="s">
+      <c r="F9" s="3439" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="3336" t="s">
+      <c r="G9" s="3447" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="3344" t="s">
+      <c r="H9" s="3455" t="s">
         <v>196</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="3352" t="s">
+      <c r="J9" s="3463" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="3360" t="s">
+      <c r="K9" s="3471" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="3368" t="s">
+      <c r="L9" s="3479" t="s">
         <v>220</v>
       </c>
       <c r="U9" s="8"/>
@@ -17493,32 +17826,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="3307" t="s">
+      <c r="C10" s="3418" t="s">
         <v>230</v>
       </c>
-      <c r="D10" s="3315" t="s">
+      <c r="D10" s="3426" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="3321" t="s">
+      <c r="E10" s="3432" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="3329" t="s">
+      <c r="F10" s="3440" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="3337" t="s">
+      <c r="G10" s="3448" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="3345" t="s">
+      <c r="H10" s="3456" t="s">
         <v>197</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="3353" t="s">
+      <c r="J10" s="3464" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="3361" t="s">
+      <c r="K10" s="3472" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="3369" t="s">
+      <c r="L10" s="3480" t="s">
         <v>221</v>
       </c>
       <c r="U10" s="8"/>
@@ -37008,34 +37341,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3370" t="s">
+      <c r="A3" s="3481" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="3372" t="s">
+      <c r="D3" s="3483" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="3374" t="s">
+      <c r="E3" s="3485" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="3376" t="s">
+      <c r="F3" s="3487" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="3371">
+      <c r="A4" t="s" s="3482">
         <v>223</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="3373">
+      <c r="D4" t="s" s="3484">
         <v>225</v>
       </c>
-      <c r="E4" t="s" s="3375">
+      <c r="E4" t="s" s="3486">
         <v>227</v>
       </c>
-      <c r="F4" t="s" s="3377">
+      <c r="F4" t="s" s="3488">
         <v>229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-09 10:35:51] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3784" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3895" uniqueCount="232">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1224,7 +1224,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3489">
+  <cellXfs count="3600">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1337,6 +1337,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -14744,44 +15077,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="3378" t="s">
+      <c r="A3" s="3489" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3380" t="s">
+      <c r="B3" s="3491" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="3382" t="s">
+      <c r="C3" s="3493" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="3384" t="s">
+      <c r="D3" s="3495" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="3386" t="s">
+      <c r="E3" s="3497" t="s">
         <v>162</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="3388" t="s">
+      <c r="G3" s="3499" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3379" t="s">
+      <c r="A4" s="3490" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3381" t="s">
+      <c r="B4" s="3492" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3383" t="s">
+      <c r="C4" s="3494" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="3385" t="s">
+      <c r="D4" s="3496" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="3387" t="s">
+      <c r="E4" s="3498" t="s">
         <v>163</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="3389" t="s">
+      <c r="G4" s="3500" t="s">
         <v>165</v>
       </c>
     </row>
@@ -15938,81 +16271,81 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="3390" t="s">
+      <c r="C3" s="3501" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="3393" t="s">
+      <c r="D3" s="3504" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3396" t="s">
+      <c r="E3" s="3507" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="3399" t="s">
+      <c r="F3" s="3510" t="s">
         <v>169</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="3402" t="s">
+      <c r="H3" s="3513" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="3405" t="s">
+      <c r="I3" s="3516" t="s">
         <v>175</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="3408" t="s">
+      <c r="K3" s="3519" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="3391" t="s">
+      <c r="C4" s="3502" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="3394" t="s">
+      <c r="D4" s="3505" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="3397" t="s">
+      <c r="E4" s="3508" t="s">
         <v>167</v>
       </c>
-      <c r="F4" s="3400" t="s">
+      <c r="F4" s="3511" t="s">
         <v>170</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="3403" t="s">
+      <c r="H4" s="3514" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="3406" t="s">
+      <c r="I4" s="3517" t="s">
         <v>176</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="3409" t="s">
+      <c r="K4" s="3520" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="3392" t="s">
+      <c r="C5" s="3503" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="3395" t="s">
+      <c r="D5" s="3506" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="3398" t="s">
+      <c r="E5" s="3509" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="3401" t="s">
+      <c r="F5" s="3512" t="s">
         <v>171</v>
       </c>
       <c r="G5" s="14"/>
-      <c r="H5" s="3404" t="s">
+      <c r="H5" s="3515" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="3407" t="s">
+      <c r="I5" s="3518" t="s">
         <v>177</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="3410" t="s">
+      <c r="K5" s="3521" t="s">
         <v>180</v>
       </c>
     </row>
@@ -17557,32 +17890,32 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="3411" t="s">
+      <c r="C3" s="3522" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="3419" t="s">
+      <c r="D3" s="3530" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3427" t="s">
+      <c r="E3" s="3538" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="3433" t="s">
+      <c r="F3" s="3544" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="3441" t="s">
+      <c r="G3" s="3552" t="s">
         <v>182</v>
       </c>
-      <c r="H3" s="3449" t="s">
+      <c r="H3" s="3560" t="s">
         <v>190</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="3457" t="s">
+      <c r="J3" s="3568" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="3465" t="s">
+      <c r="K3" s="3576" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="3473" t="s">
+      <c r="L3" s="3584" t="s">
         <v>214</v>
       </c>
       <c r="U3" s="8"/>
@@ -17596,32 +17929,32 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="3412" t="s">
+      <c r="C4" s="3523" t="s">
         <v>230</v>
       </c>
-      <c r="D4" s="3420" t="s">
+      <c r="D4" s="3531" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="3428" t="s">
+      <c r="E4" s="3539" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="3434" t="s">
+      <c r="F4" s="3545" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="3442" t="s">
+      <c r="G4" s="3553" t="s">
         <v>183</v>
       </c>
-      <c r="H4" s="3450" t="s">
+      <c r="H4" s="3561" t="s">
         <v>191</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="3458" t="s">
+      <c r="J4" s="3569" t="s">
         <v>199</v>
       </c>
-      <c r="K4" s="3466" t="s">
+      <c r="K4" s="3577" t="s">
         <v>207</v>
       </c>
-      <c r="L4" s="3474" t="s">
+      <c r="L4" s="3585" t="s">
         <v>215</v>
       </c>
       <c r="U4" s="8"/>
@@ -17635,30 +17968,30 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="3413" t="s">
+      <c r="C5" s="3524" t="s">
         <v>230</v>
       </c>
-      <c r="D5" s="3421" t="s">
+      <c r="D5" s="3532" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="3435" t="s">
+      <c r="F5" s="3546" t="s">
         <v>181</v>
       </c>
-      <c r="G5" s="3443" t="s">
+      <c r="G5" s="3554" t="s">
         <v>184</v>
       </c>
-      <c r="H5" s="3451" t="s">
+      <c r="H5" s="3562" t="s">
         <v>192</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="3459" t="s">
+      <c r="J5" s="3570" t="s">
         <v>200</v>
       </c>
-      <c r="K5" s="3467" t="s">
+      <c r="K5" s="3578" t="s">
         <v>208</v>
       </c>
-      <c r="L5" s="3475" t="s">
+      <c r="L5" s="3586" t="s">
         <v>216</v>
       </c>
       <c r="U5" s="8"/>
@@ -17672,32 +18005,32 @@
     <row r="6">
       <c r="A6" s="23"/>
       <c r="B6"/>
-      <c r="C6" s="3414" t="s">
+      <c r="C6" s="3525" t="s">
         <v>230</v>
       </c>
-      <c r="D6" s="3422" t="s">
+      <c r="D6" s="3533" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="3429" t="s">
+      <c r="E6" s="3540" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="3436" t="s">
+      <c r="F6" s="3547" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="3444" t="s">
+      <c r="G6" s="3555" t="s">
         <v>185</v>
       </c>
-      <c r="H6" s="3452" t="s">
+      <c r="H6" s="3563" t="s">
         <v>193</v>
       </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="3460" t="s">
+      <c r="J6" s="3571" t="s">
         <v>201</v>
       </c>
-      <c r="K6" s="3468" t="s">
+      <c r="K6" s="3579" t="s">
         <v>209</v>
       </c>
-      <c r="L6" s="3476" t="s">
+      <c r="L6" s="3587" t="s">
         <v>217</v>
       </c>
       <c r="U6" s="8"/>
@@ -17711,32 +18044,32 @@
     <row r="7">
       <c r="A7" s="23"/>
       <c r="B7"/>
-      <c r="C7" s="3415" t="s">
+      <c r="C7" s="3526" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="3423" t="s">
+      <c r="D7" s="3534" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="3430" t="s">
+      <c r="E7" s="3541" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="3437" t="s">
+      <c r="F7" s="3548" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="3445" t="s">
+      <c r="G7" s="3556" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="3453" t="s">
+      <c r="H7" s="3564" t="s">
         <v>194</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="3461" t="s">
+      <c r="J7" s="3572" t="s">
         <v>202</v>
       </c>
-      <c r="K7" s="3469" t="s">
+      <c r="K7" s="3580" t="s">
         <v>210</v>
       </c>
-      <c r="L7" s="3477" t="s">
+      <c r="L7" s="3588" t="s">
         <v>218</v>
       </c>
       <c r="U7" s="8"/>
@@ -17750,30 +18083,30 @@
     <row r="8">
       <c r="A8" s="23"/>
       <c r="B8"/>
-      <c r="C8" s="3416" t="s">
+      <c r="C8" s="3527" t="s">
         <v>230</v>
       </c>
-      <c r="D8" s="3424" t="s">
+      <c r="D8" s="3535" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="23"/>
-      <c r="F8" s="3438" t="s">
+      <c r="F8" s="3549" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="3446" t="s">
+      <c r="G8" s="3557" t="s">
         <v>187</v>
       </c>
-      <c r="H8" s="3454" t="s">
+      <c r="H8" s="3565" t="s">
         <v>195</v>
       </c>
       <c r="I8" s="14"/>
-      <c r="J8" s="3462" t="s">
+      <c r="J8" s="3573" t="s">
         <v>203</v>
       </c>
-      <c r="K8" s="3470" t="s">
+      <c r="K8" s="3581" t="s">
         <v>211</v>
       </c>
-      <c r="L8" s="3478" t="s">
+      <c r="L8" s="3589" t="s">
         <v>219</v>
       </c>
       <c r="U8" s="8"/>
@@ -17787,32 +18120,32 @@
     <row r="9">
       <c r="A9" s="23"/>
       <c r="B9"/>
-      <c r="C9" s="3417" t="s">
+      <c r="C9" s="3528" t="s">
         <v>230</v>
       </c>
-      <c r="D9" s="3425" t="s">
+      <c r="D9" s="3536" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="3431" t="s">
+      <c r="E9" s="3542" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="3439" t="s">
+      <c r="F9" s="3550" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="3447" t="s">
+      <c r="G9" s="3558" t="s">
         <v>188</v>
       </c>
-      <c r="H9" s="3455" t="s">
+      <c r="H9" s="3566" t="s">
         <v>196</v>
       </c>
       <c r="I9" s="14"/>
-      <c r="J9" s="3463" t="s">
+      <c r="J9" s="3574" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="3471" t="s">
+      <c r="K9" s="3582" t="s">
         <v>212</v>
       </c>
-      <c r="L9" s="3479" t="s">
+      <c r="L9" s="3590" t="s">
         <v>220</v>
       </c>
       <c r="U9" s="8"/>
@@ -17826,32 +18159,32 @@
     <row r="10">
       <c r="A10" s="23"/>
       <c r="B10"/>
-      <c r="C10" s="3418" t="s">
+      <c r="C10" s="3529" t="s">
         <v>230</v>
       </c>
-      <c r="D10" s="3426" t="s">
+      <c r="D10" s="3537" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="3432" t="s">
+      <c r="E10" s="3543" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="3440" t="s">
+      <c r="F10" s="3551" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="3448" t="s">
+      <c r="G10" s="3559" t="s">
         <v>189</v>
       </c>
-      <c r="H10" s="3456" t="s">
+      <c r="H10" s="3567" t="s">
         <v>197</v>
       </c>
       <c r="I10" s="14"/>
-      <c r="J10" s="3464" t="s">
+      <c r="J10" s="3575" t="s">
         <v>205</v>
       </c>
-      <c r="K10" s="3472" t="s">
+      <c r="K10" s="3583" t="s">
         <v>213</v>
       </c>
-      <c r="L10" s="3480" t="s">
+      <c r="L10" s="3591" t="s">
         <v>221</v>
       </c>
       <c r="U10" s="8"/>
@@ -37341,34 +37674,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3481" t="s">
+      <c r="A3" s="3592" t="s">
         <v>222</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3"/>
-      <c r="D3" s="3483" t="s">
+      <c r="D3" s="3594" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="3485" t="s">
+      <c r="E3" s="3596" t="s">
         <v>226</v>
       </c>
-      <c r="F3" s="3487" t="s">
+      <c r="F3" s="3598" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="3482">
+      <c r="A4" t="s" s="3593">
         <v>223</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" t="s" s="3484">
+      <c r="D4" t="s" s="3595">
         <v>225</v>
       </c>
-      <c r="E4" t="s" s="3486">
+      <c r="E4" t="s" s="3597">
         <v>227</v>
       </c>
-      <c r="F4" t="s" s="3488">
+      <c r="F4" t="s" s="3599">
         <v>229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-09 12:47:55] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="168">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1130,6 +1130,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1441,13 +1774,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="29.63" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="27.13" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="8.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="25.63" collapsed="false"/>
-    <col min="6" max="25" customWidth="true" width="10.63" collapsed="false"/>
-    <col min="26" max="26" customWidth="true" width="14.38" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.63" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.13" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.63" collapsed="true"/>
+    <col min="6" max="25" customWidth="true" width="10.63" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="14.38" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
@@ -4178,13 +4511,13 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.13" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.63" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="22.88" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="21.63" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="112.38" collapsed="false"/>
-    <col min="7" max="26" customWidth="true" width="10.63" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.13" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.63" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.88" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.63" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="112.38" collapsed="true"/>
+    <col min="7" max="26" customWidth="true" width="10.63" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -4238,44 +4571,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="53" t="s">
+      <c r="B3" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="65" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="67" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="66" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="68" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5345,20 +5678,20 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.63" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.38" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.38" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="8.38" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="28.38" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.38" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="8" max="9" customWidth="true" width="21.38" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="35.13" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="14.38" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="16.63" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="14.38" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="21.63" collapsed="false"/>
-    <col min="15" max="30" customWidth="true" width="14.38" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="9.63" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.38" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.38" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.38" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.38" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.38" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="21.38" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="35.13" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.38" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.63" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.38" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="21.63" collapsed="true"/>
+    <col min="15" max="30" customWidth="true" width="14.38" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -5432,81 +5765,81 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="78" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="13"/>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="53" t="s">
+      <c r="I3" s="84" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="53" t="s">
+      <c r="K3" s="87" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="79" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="13"/>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="82" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="53" t="s">
+      <c r="I4" s="85" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="53" t="s">
+      <c r="K4" s="88" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="80" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="13"/>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="86" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="89" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6944,18 +7277,18 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.13" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="11.63" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.38" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="9.38" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="13.88" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.88" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="29.63" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="16.38" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="19.13" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="21.38" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="19.0" collapsed="false"/>
-    <col min="12" max="31" customWidth="true" width="10.63" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.13" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.63" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.38" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.38" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.88" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.63" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.38" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.13" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.38" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="12" max="31" customWidth="true" width="10.63" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -7051,32 +7384,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="112" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="53" t="s">
+      <c r="G3" s="120" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="53" t="s">
+      <c r="H3" s="128" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="53" t="s">
+      <c r="J3" s="136" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="53" t="s">
+      <c r="K3" s="144" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="53" t="s">
+      <c r="L3" s="152" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -7090,32 +7423,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="53" t="s">
+      <c r="C4" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="99" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="107" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="53" t="s">
+      <c r="G4" s="121" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="53" t="s">
+      <c r="H4" s="129" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="53" t="s">
+      <c r="J4" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="53" t="s">
+      <c r="K4" s="145" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="53" t="s">
+      <c r="L4" s="153" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -7129,30 +7462,30 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="53" t="s">
+      <c r="D5" s="100" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="114" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="53" t="s">
+      <c r="G5" s="122" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="53" t="s">
+      <c r="H5" s="130" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="53" t="s">
+      <c r="J5" s="138" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="53" t="s">
+      <c r="K5" s="146" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="53" t="s">
+      <c r="L5" s="154" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -7166,32 +7499,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="53" t="s">
+      <c r="E6" s="108" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="115" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="53" t="s">
+      <c r="G6" s="123" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="131" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="13"/>
-      <c r="J6" s="53" t="s">
+      <c r="J6" s="139" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="53" t="s">
+      <c r="K6" s="147" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="53" t="s">
+      <c r="L6" s="155" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -7205,32 +7538,32 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="53" t="s">
+      <c r="F7" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="53" t="s">
+      <c r="G7" s="124" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="53" t="s">
+      <c r="H7" s="132" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="13"/>
-      <c r="J7" s="53" t="s">
+      <c r="J7" s="140" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="53" t="s">
+      <c r="K7" s="148" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="53" t="s">
+      <c r="L7" s="156" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -7244,30 +7577,30 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="95" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="103" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="22"/>
-      <c r="F8" s="53" t="s">
+      <c r="F8" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="G8" s="125" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="53" t="s">
+      <c r="H8" s="133" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="53" t="s">
+      <c r="J8" s="141" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="53" t="s">
+      <c r="K8" s="149" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="53" t="s">
+      <c r="L8" s="157" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -7281,32 +7614,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="D9" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="110" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="F9" s="118" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="53" t="s">
+      <c r="G9" s="126" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="53" t="s">
+      <c r="H9" s="134" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="53" t="s">
+      <c r="J9" s="142" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="53" t="s">
+      <c r="K9" s="150" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="53" t="s">
+      <c r="L9" s="158" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -7320,32 +7653,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="119" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="53" t="s">
+      <c r="G10" s="127" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="53" t="s">
+      <c r="H10" s="135" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="53" t="s">
+      <c r="J10" s="143" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="53" t="s">
+      <c r="K10" s="151" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="53" t="s">
+      <c r="L10" s="159" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -9368,22 +9701,22 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.13" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.88" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.38" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="7.13" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="19.38" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.63" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.38" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="19.13" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.13" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="21.88" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="28.13" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="14.38" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="16.63" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="14.38" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="21.63" collapsed="false"/>
-    <col min="16" max="31" customWidth="true" width="14.38" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.13" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.88" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.38" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="7.13" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.38" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.63" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.38" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.13" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.13" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.88" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.13" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.38" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.63" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="14.38" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="21.63" collapsed="true"/>
+    <col min="16" max="31" customWidth="true" width="14.38" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="21.75" customHeight="1">
@@ -11010,19 +11343,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="7.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="8.13" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.13" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="9.38" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="10.13" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="39.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="22.38" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="17.38" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.38" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="16.38" collapsed="false"/>
-    <col min="12" max="13" customWidth="true" width="10.88" collapsed="false"/>
-    <col min="14" max="31" customWidth="true" width="10.63" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.13" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.13" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.38" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.13" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.38" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.38" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.38" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.38" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="10.88" collapsed="true"/>
+    <col min="14" max="31" customWidth="true" width="10.63" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -13352,17 +13685,17 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.88" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="10.13" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.13" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="13.63" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="15.38" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="47.38" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="34.13" collapsed="false"/>
-    <col min="8" max="9" customWidth="true" width="12.13" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="16.63" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="16.13" collapsed="false"/>
-    <col min="12" max="31" customWidth="true" width="14.38" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="11.88" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.13" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.13" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.63" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.38" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="47.38" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="34.13" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="12.13" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.63" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.13" collapsed="true"/>
+    <col min="12" max="31" customWidth="true" width="14.38" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.0" customHeight="1">
@@ -26805,7 +27138,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.75" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="23.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -26835,34 +27168,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="160" t="s">
         <v>150</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3"/>
-      <c r="D3" s="53" t="s">
+      <c r="D3" s="162" t="s">
         <v>151</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="164" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="53" t="s">
+      <c r="F3" s="166" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="161" t="s">
         <v>154</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" s="53" t="s">
+      <c r="D4" s="163" t="s">
         <v>155</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="165" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="167" t="s">
         <v>157</v>
       </c>
     </row>
@@ -26885,9 +27218,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="150.0" collapsed="false"/>
-    <col min="2" max="6" customWidth="true" width="10.63" collapsed="false"/>
-    <col min="7" max="26" customWidth="true" width="14.38" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="150.0" collapsed="true"/>
+    <col min="2" max="6" customWidth="true" width="10.63" collapsed="true"/>
+    <col min="7" max="26" customWidth="true" width="14.38" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="26.25" customHeight="1">

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-09-16 18:16:44] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="279">
+  <cellXfs count="390">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1130,6 +1130,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -4904,44 +5237,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="279" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="170" t="s">
+      <c r="B3" s="281" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="172" t="s">
+      <c r="C3" s="283" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="174" t="s">
+      <c r="D3" s="285" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="176" t="s">
+      <c r="E3" s="287" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="178" t="s">
+      <c r="G3" s="289" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="169" t="s">
+      <c r="A4" s="280" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="171" t="s">
+      <c r="B4" s="282" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="173" t="s">
+      <c r="C4" s="284" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="175" t="s">
+      <c r="D4" s="286" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="177" t="s">
+      <c r="E4" s="288" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="179" t="s">
+      <c r="G4" s="290" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6098,81 +6431,81 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="180" t="s">
+      <c r="C3" s="291" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="183" t="s">
+      <c r="D3" s="294" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="186" t="s">
+      <c r="E3" s="297" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="189" t="s">
+      <c r="F3" s="300" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="13"/>
-      <c r="H3" s="192" t="s">
+      <c r="H3" s="303" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="195" t="s">
+      <c r="I3" s="306" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="198" t="s">
+      <c r="K3" s="309" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="181" t="s">
+      <c r="C4" s="292" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="184" t="s">
+      <c r="D4" s="295" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="187" t="s">
+      <c r="E4" s="298" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="190" t="s">
+      <c r="F4" s="301" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="13"/>
-      <c r="H4" s="193" t="s">
+      <c r="H4" s="304" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="196" t="s">
+      <c r="I4" s="307" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="199" t="s">
+      <c r="K4" s="310" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="182" t="s">
+      <c r="C5" s="293" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="185" t="s">
+      <c r="D5" s="296" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="188" t="s">
+      <c r="E5" s="299" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="191" t="s">
+      <c r="F5" s="302" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="13"/>
-      <c r="H5" s="194" t="s">
+      <c r="H5" s="305" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="197" t="s">
+      <c r="I5" s="308" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="200" t="s">
+      <c r="K5" s="311" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7717,32 +8050,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="201" t="s">
+      <c r="C3" s="312" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="209" t="s">
+      <c r="D3" s="320" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="217" t="s">
+      <c r="E3" s="328" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="223" t="s">
+      <c r="F3" s="334" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="231" t="s">
+      <c r="G3" s="342" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="239" t="s">
+      <c r="H3" s="350" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="247" t="s">
+      <c r="J3" s="358" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="255" t="s">
+      <c r="K3" s="366" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="263" t="s">
+      <c r="L3" s="374" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -7756,32 +8089,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="202" t="s">
+      <c r="C4" s="313" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="210" t="s">
+      <c r="D4" s="321" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="218" t="s">
+      <c r="E4" s="329" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="224" t="s">
+      <c r="F4" s="335" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="232" t="s">
+      <c r="G4" s="343" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="240" t="s">
+      <c r="H4" s="351" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="248" t="s">
+      <c r="J4" s="359" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="256" t="s">
+      <c r="K4" s="367" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="264" t="s">
+      <c r="L4" s="375" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -7795,30 +8128,30 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="203" t="s">
+      <c r="C5" s="314" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="211" t="s">
+      <c r="D5" s="322" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="225" t="s">
+      <c r="F5" s="336" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="233" t="s">
+      <c r="G5" s="344" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="241" t="s">
+      <c r="H5" s="352" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="249" t="s">
+      <c r="J5" s="360" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="257" t="s">
+      <c r="K5" s="368" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="265" t="s">
+      <c r="L5" s="376" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -7832,32 +8165,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="204" t="s">
+      <c r="C6" s="315" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="212" t="s">
+      <c r="D6" s="323" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="219" t="s">
+      <c r="E6" s="330" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="226" t="s">
+      <c r="F6" s="337" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="234" t="s">
+      <c r="G6" s="345" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="242" t="s">
+      <c r="H6" s="353" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="13"/>
-      <c r="J6" s="250" t="s">
+      <c r="J6" s="361" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="258" t="s">
+      <c r="K6" s="369" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="266" t="s">
+      <c r="L6" s="377" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -7871,32 +8204,32 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="205" t="s">
+      <c r="C7" s="316" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="213" t="s">
+      <c r="D7" s="324" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="220" t="s">
+      <c r="E7" s="331" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="227" t="s">
+      <c r="F7" s="338" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="235" t="s">
+      <c r="G7" s="346" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="243" t="s">
+      <c r="H7" s="354" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="13"/>
-      <c r="J7" s="251" t="s">
+      <c r="J7" s="362" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="259" t="s">
+      <c r="K7" s="370" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="267" t="s">
+      <c r="L7" s="378" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -7910,30 +8243,30 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="206" t="s">
+      <c r="C8" s="317" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="214" t="s">
+      <c r="D8" s="325" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="22"/>
-      <c r="F8" s="228" t="s">
+      <c r="F8" s="339" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="236" t="s">
+      <c r="G8" s="347" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="244" t="s">
+      <c r="H8" s="355" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="252" t="s">
+      <c r="J8" s="363" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="260" t="s">
+      <c r="K8" s="371" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="268" t="s">
+      <c r="L8" s="379" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -7947,32 +8280,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="207" t="s">
+      <c r="C9" s="318" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="215" t="s">
+      <c r="D9" s="326" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="221" t="s">
+      <c r="E9" s="332" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="229" t="s">
+      <c r="F9" s="340" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="237" t="s">
+      <c r="G9" s="348" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="245" t="s">
+      <c r="H9" s="356" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="253" t="s">
+      <c r="J9" s="364" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="261" t="s">
+      <c r="K9" s="372" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="269" t="s">
+      <c r="L9" s="380" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -7986,32 +8319,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="208" t="s">
+      <c r="C10" s="319" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="216" t="s">
+      <c r="D10" s="327" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="222" t="s">
+      <c r="E10" s="333" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="230" t="s">
+      <c r="F10" s="341" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="238" t="s">
+      <c r="G10" s="349" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="246" t="s">
+      <c r="H10" s="357" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="254" t="s">
+      <c r="J10" s="365" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="262" t="s">
+      <c r="K10" s="373" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="270" t="s">
+      <c r="L10" s="381" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -27501,34 +27834,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="271" t="s">
+      <c r="A3" s="382" t="s">
         <v>150</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3"/>
-      <c r="D3" s="273" t="s">
+      <c r="D3" s="384" t="s">
         <v>151</v>
       </c>
-      <c r="E3" s="275" t="s">
+      <c r="E3" s="386" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="277" t="s">
+      <c r="F3" s="388" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="272" t="s">
+      <c r="A4" s="383" t="s">
         <v>154</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" s="274" t="s">
+      <c r="D4" s="385" t="s">
         <v>155</v>
       </c>
-      <c r="E4" s="276" t="s">
+      <c r="E4" s="387" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="278" t="s">
+      <c r="F4" s="389" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"galacticPubs::publish() [2022-11-17 12:00:05] "
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -229,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="162">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1014,7 +1014,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="390">
+  <cellXfs count="501">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1130,6 +1130,339 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -5237,44 +5570,44 @@
       <c r="Z2" s="6"/>
     </row>
     <row r="3">
-      <c r="A3" s="279" t="s">
+      <c r="A3" s="390" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="281" t="s">
+      <c r="B3" s="392" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="283" t="s">
+      <c r="C3" s="394" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="285" t="s">
+      <c r="D3" s="396" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="287" t="s">
+      <c r="E3" s="398" t="s">
         <v>33</v>
       </c>
       <c r="F3" s="13"/>
-      <c r="G3" s="289" t="s">
+      <c r="G3" s="400" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="280" t="s">
+      <c r="A4" s="391" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="282" t="s">
+      <c r="B4" s="393" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="284" t="s">
+      <c r="C4" s="395" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="286" t="s">
+      <c r="D4" s="397" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="288" t="s">
+      <c r="E4" s="399" t="s">
         <v>36</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="290" t="s">
+      <c r="G4" s="401" t="s">
         <v>37</v>
       </c>
     </row>
@@ -6431,81 +6764,81 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="291" t="s">
+      <c r="C3" s="402" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="294" t="s">
+      <c r="D3" s="405" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="297" t="s">
+      <c r="E3" s="408" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="300" t="s">
+      <c r="F3" s="411" t="s">
         <v>47</v>
       </c>
       <c r="G3" s="13"/>
-      <c r="H3" s="303" t="s">
+      <c r="H3" s="414" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="306" t="s">
+      <c r="I3" s="417" t="s">
         <v>49</v>
       </c>
       <c r="J3"/>
-      <c r="K3" s="309" t="s">
+      <c r="K3" s="420" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="292" t="s">
+      <c r="C4" s="403" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="295" t="s">
+      <c r="D4" s="406" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="298" t="s">
+      <c r="E4" s="409" t="s">
         <v>52</v>
       </c>
-      <c r="F4" s="301" t="s">
+      <c r="F4" s="412" t="s">
         <v>53</v>
       </c>
       <c r="G4" s="13"/>
-      <c r="H4" s="304" t="s">
+      <c r="H4" s="415" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="307" t="s">
+      <c r="I4" s="418" t="s">
         <v>55</v>
       </c>
       <c r="J4"/>
-      <c r="K4" s="310" t="s">
+      <c r="K4" s="421" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="293" t="s">
+      <c r="C5" s="404" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="296" t="s">
+      <c r="D5" s="407" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="299" t="s">
+      <c r="E5" s="410" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="302" t="s">
+      <c r="F5" s="413" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="13"/>
-      <c r="H5" s="305" t="s">
+      <c r="H5" s="416" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="308" t="s">
+      <c r="I5" s="419" t="s">
         <v>61</v>
       </c>
       <c r="J5"/>
-      <c r="K5" s="311" t="s">
+      <c r="K5" s="422" t="s">
         <v>62</v>
       </c>
     </row>
@@ -8050,32 +8383,32 @@
     <row r="3">
       <c r="A3" s="22"/>
       <c r="B3"/>
-      <c r="C3" s="312" t="s">
+      <c r="C3" s="423" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="320" t="s">
+      <c r="D3" s="431" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="328" t="s">
+      <c r="E3" s="439" t="s">
         <v>67</v>
       </c>
-      <c r="F3" s="334" t="s">
+      <c r="F3" s="445" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="342" t="s">
+      <c r="G3" s="453" t="s">
         <v>69</v>
       </c>
-      <c r="H3" s="350" t="s">
+      <c r="H3" s="461" t="s">
         <v>70</v>
       </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="358" t="s">
+      <c r="J3" s="469" t="s">
         <v>71</v>
       </c>
-      <c r="K3" s="366" t="s">
+      <c r="K3" s="477" t="s">
         <v>72</v>
       </c>
-      <c r="L3" s="374" t="s">
+      <c r="L3" s="485" t="s">
         <v>73</v>
       </c>
       <c r="U3" s="8"/>
@@ -8089,32 +8422,32 @@
     <row r="4">
       <c r="A4" s="22"/>
       <c r="B4"/>
-      <c r="C4" s="313" t="s">
+      <c r="C4" s="424" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="321" t="s">
+      <c r="D4" s="432" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="329" t="s">
+      <c r="E4" s="440" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="335" t="s">
+      <c r="F4" s="446" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="343" t="s">
+      <c r="G4" s="454" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="351" t="s">
+      <c r="H4" s="462" t="s">
         <v>77</v>
       </c>
       <c r="I4" s="13"/>
-      <c r="J4" s="359" t="s">
+      <c r="J4" s="470" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="367" t="s">
+      <c r="K4" s="478" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="375" t="s">
+      <c r="L4" s="486" t="s">
         <v>80</v>
       </c>
       <c r="U4" s="8"/>
@@ -8128,30 +8461,30 @@
     <row r="5">
       <c r="A5" s="22"/>
       <c r="B5"/>
-      <c r="C5" s="314" t="s">
+      <c r="C5" s="425" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="322" t="s">
+      <c r="D5" s="433" t="s">
         <v>45</v>
       </c>
       <c r="E5" s="13"/>
-      <c r="F5" s="336" t="s">
+      <c r="F5" s="447" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="344" t="s">
+      <c r="G5" s="455" t="s">
         <v>82</v>
       </c>
-      <c r="H5" s="352" t="s">
+      <c r="H5" s="463" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="360" t="s">
+      <c r="J5" s="471" t="s">
         <v>84</v>
       </c>
-      <c r="K5" s="368" t="s">
+      <c r="K5" s="479" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="376" t="s">
+      <c r="L5" s="487" t="s">
         <v>86</v>
       </c>
       <c r="U5" s="8"/>
@@ -8165,32 +8498,32 @@
     <row r="6">
       <c r="A6" s="22"/>
       <c r="B6"/>
-      <c r="C6" s="315" t="s">
+      <c r="C6" s="426" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="323" t="s">
+      <c r="D6" s="434" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="330" t="s">
+      <c r="E6" s="441" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="337" t="s">
+      <c r="F6" s="448" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="345" t="s">
+      <c r="G6" s="456" t="s">
         <v>88</v>
       </c>
-      <c r="H6" s="353" t="s">
+      <c r="H6" s="464" t="s">
         <v>89</v>
       </c>
       <c r="I6" s="13"/>
-      <c r="J6" s="361" t="s">
+      <c r="J6" s="472" t="s">
         <v>90</v>
       </c>
-      <c r="K6" s="369" t="s">
+      <c r="K6" s="480" t="s">
         <v>91</v>
       </c>
-      <c r="L6" s="377" t="s">
+      <c r="L6" s="488" t="s">
         <v>92</v>
       </c>
       <c r="U6" s="8"/>
@@ -8204,32 +8537,32 @@
     <row r="7">
       <c r="A7" s="22"/>
       <c r="B7"/>
-      <c r="C7" s="316" t="s">
+      <c r="C7" s="427" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="324" t="s">
+      <c r="D7" s="435" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="331" t="s">
+      <c r="E7" s="442" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="338" t="s">
+      <c r="F7" s="449" t="s">
         <v>93</v>
       </c>
-      <c r="G7" s="346" t="s">
+      <c r="G7" s="457" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="354" t="s">
+      <c r="H7" s="465" t="s">
         <v>95</v>
       </c>
       <c r="I7" s="13"/>
-      <c r="J7" s="362" t="s">
+      <c r="J7" s="473" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="370" t="s">
+      <c r="K7" s="481" t="s">
         <v>97</v>
       </c>
-      <c r="L7" s="378" t="s">
+      <c r="L7" s="489" t="s">
         <v>98</v>
       </c>
       <c r="U7" s="8"/>
@@ -8243,30 +8576,30 @@
     <row r="8">
       <c r="A8" s="22"/>
       <c r="B8"/>
-      <c r="C8" s="317" t="s">
+      <c r="C8" s="428" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="325" t="s">
+      <c r="D8" s="436" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="22"/>
-      <c r="F8" s="339" t="s">
+      <c r="F8" s="450" t="s">
         <v>99</v>
       </c>
-      <c r="G8" s="347" t="s">
+      <c r="G8" s="458" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="355" t="s">
+      <c r="H8" s="466" t="s">
         <v>101</v>
       </c>
       <c r="I8" s="13"/>
-      <c r="J8" s="363" t="s">
+      <c r="J8" s="474" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="371" t="s">
+      <c r="K8" s="482" t="s">
         <v>103</v>
       </c>
-      <c r="L8" s="379" t="s">
+      <c r="L8" s="490" t="s">
         <v>104</v>
       </c>
       <c r="U8" s="8"/>
@@ -8280,32 +8613,32 @@
     <row r="9">
       <c r="A9" s="22"/>
       <c r="B9"/>
-      <c r="C9" s="318" t="s">
+      <c r="C9" s="429" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="326" t="s">
+      <c r="D9" s="437" t="s">
         <v>57</v>
       </c>
-      <c r="E9" s="332" t="s">
+      <c r="E9" s="443" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="340" t="s">
+      <c r="F9" s="451" t="s">
         <v>105</v>
       </c>
-      <c r="G9" s="348" t="s">
+      <c r="G9" s="459" t="s">
         <v>106</v>
       </c>
-      <c r="H9" s="356" t="s">
+      <c r="H9" s="467" t="s">
         <v>107</v>
       </c>
       <c r="I9" s="13"/>
-      <c r="J9" s="364" t="s">
+      <c r="J9" s="475" t="s">
         <v>108</v>
       </c>
-      <c r="K9" s="372" t="s">
+      <c r="K9" s="483" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="380" t="s">
+      <c r="L9" s="491" t="s">
         <v>110</v>
       </c>
       <c r="U9" s="8"/>
@@ -8319,32 +8652,32 @@
     <row r="10">
       <c r="A10" s="22"/>
       <c r="B10"/>
-      <c r="C10" s="319" t="s">
+      <c r="C10" s="430" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="327" t="s">
+      <c r="D10" s="438" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="333" t="s">
+      <c r="E10" s="444" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="341" t="s">
+      <c r="F10" s="452" t="s">
         <v>111</v>
       </c>
-      <c r="G10" s="349" t="s">
+      <c r="G10" s="460" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="357" t="s">
+      <c r="H10" s="468" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="13"/>
-      <c r="J10" s="365" t="s">
+      <c r="J10" s="476" t="s">
         <v>114</v>
       </c>
-      <c r="K10" s="373" t="s">
+      <c r="K10" s="484" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="381" t="s">
+      <c r="L10" s="492" t="s">
         <v>116</v>
       </c>
       <c r="U10" s="8"/>
@@ -27834,34 +28167,34 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="382" t="s">
+      <c r="A3" s="493" t="s">
         <v>150</v>
       </c>
       <c r="B3" s="49"/>
       <c r="C3"/>
-      <c r="D3" s="384" t="s">
+      <c r="D3" s="495" t="s">
         <v>151</v>
       </c>
-      <c r="E3" s="386" t="s">
+      <c r="E3" s="497" t="s">
         <v>152</v>
       </c>
-      <c r="F3" s="388" t="s">
+      <c r="F3" s="499" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="383" t="s">
+      <c r="A4" s="494" t="s">
         <v>154</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4" s="385" t="s">
+      <c r="D4" s="496" t="s">
         <v>155</v>
       </c>
-      <c r="E4" s="387" t="s">
+      <c r="E4" s="498" t="s">
         <v>156</v>
       </c>
-      <c r="F4" s="389" t="s">
+      <c r="F4" s="500" t="s">
         <v>157</v>
       </c>
     </row>

</xml_diff>